<commit_message>
:arrow_up:Atualização das tabelas por gênero, quantidade de gatos e cachorros e faixa etária
</commit_message>
<xml_diff>
--- a/GRÁFICOS.xlsx
+++ b/GRÁFICOS.xlsx
@@ -11,7 +11,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+  <si>
+    <t>Espécie</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
   <si>
     <t>Quantidade animais</t>
   </si>
@@ -19,15 +25,27 @@
     <t>Status do animal</t>
   </si>
   <si>
+    <t>Cachorro</t>
+  </si>
+  <si>
+    <t>Faixa etária</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantidade </t>
+  </si>
+  <si>
     <t>Tipo de doação</t>
   </si>
   <si>
-    <t>Quantidade</t>
-  </si>
-  <si>
     <t>adotado</t>
   </si>
   <si>
+    <t>Gato</t>
+  </si>
+  <si>
+    <t>Filhote</t>
+  </si>
+  <si>
     <t>Veterinários</t>
   </si>
   <si>
@@ -43,6 +61,9 @@
     <t>em quarentena</t>
   </si>
   <si>
+    <t>Adulto</t>
+  </si>
+  <si>
     <t>Dra. Ana Júlia</t>
   </si>
   <si>
@@ -55,6 +76,9 @@
     <t>em tratamento</t>
   </si>
   <si>
+    <t>Idoso</t>
+  </si>
+  <si>
     <t>Dr. Carlos Mendes</t>
   </si>
   <si>
@@ -101,13 +125,22 @@
   </si>
   <si>
     <t>1450.00</t>
+  </si>
+  <si>
+    <t>Gênero</t>
+  </si>
+  <si>
+    <t>Macho</t>
+  </si>
+  <si>
+    <t>Fêmea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -120,17 +153,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -146,14 +193,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3C78D8"/>
-        <bgColor rgb="FF3C78D8"/>
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCFE2F3"/>
-        <bgColor rgb="FFCFE2F3"/>
+        <fgColor rgb="FF3C78D8"/>
+        <bgColor rgb="FF3C78D8"/>
       </patternFill>
     </fill>
   </fills>
@@ -163,30 +210,76 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -206,7 +299,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -214,7 +307,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -261,11 +354,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="931533766"/>
-        <c:axId val="204904480"/>
+        <c:axId val="721686568"/>
+        <c:axId val="490304490"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="931533766"/>
+        <c:axId val="721686568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -278,7 +371,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr lvl="0">
-                  <a:defRPr b="0">
+                  <a:defRPr b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -286,7 +379,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -308,7 +401,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -317,10 +410,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204904480"/>
+        <c:crossAx val="490304490"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204904480"/>
+        <c:axId val="490304490"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -353,7 +446,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr lvl="0">
-                  <a:defRPr b="0">
+                  <a:defRPr b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -361,7 +454,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0">
+                  <a:rPr b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -386,7 +479,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -395,7 +488,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="931533766"/>
+        <c:crossAx val="721686568"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -406,7 +499,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr lvl="0">
-            <a:defRPr b="0">
+            <a:defRPr b="0" i="0">
               <a:solidFill>
                 <a:srgbClr val="1A1A1A"/>
               </a:solidFill>
@@ -431,7 +524,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -439,7 +532,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -544,7 +637,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr lvl="0">
-            <a:defRPr b="0">
+            <a:defRPr b="0" i="0">
               <a:solidFill>
                 <a:srgbClr val="1A1A1A"/>
               </a:solidFill>
@@ -569,7 +662,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -577,7 +670,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -624,11 +717,865 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="226974182"/>
-        <c:axId val="1431436756"/>
+        <c:axId val="657405305"/>
+        <c:axId val="417719007"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="226974182"/>
+        <c:axId val="657405305"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Status do animal</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417719007"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="417719007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Quantidade animais</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="657405305"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="666666"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="666666"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Quantidade de gatos e cachorros</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$T$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3C78D8"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$S$13:$S$14</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$T$13:$T$14</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$U$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$S$13:$S$14</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$U$13:$U$14</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="1300976426"/>
+        <c:axId val="286182791"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1300976426"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="286182791"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="286182791"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1300976426"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="3C78D8"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Faixa etária dos animais</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$X$13</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F1C232"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$W$14:$W$16</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$X$14:$X$16</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$Y$13</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$W$14:$W$16</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$Y$14:$Y$16</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1084108329"/>
+        <c:axId val="2139942766"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1084108329"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2139942766"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2139942766"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1084108329"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="B7B7B7"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="B7B7B7"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Quantidade - Gênero</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$V$21</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F1C232"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F1C232"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="1155CC"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="1155CC"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$U$22:$U$25</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$V$22:$V$25</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$W$21</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$U$22:$U$25</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$W$22:$W$25</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1913273333"/>
+        <c:axId val="867643121"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1913273333"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -655,7 +1602,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>Status do animal</a:t>
+                  <a:t/>
                 </a:r>
               </a:p>
             </c:rich>
@@ -680,10 +1627,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1431436756"/>
+        <c:crossAx val="867643121"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1431436756"/>
+        <c:axId val="867643121"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +1677,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>Quantidade animais</a:t>
+                  <a:t/>
                 </a:r>
               </a:p>
             </c:rich>
@@ -758,7 +1705,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226974182"/>
+        <c:crossAx val="1913273333"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -772,7 +1719,7 @@
           <a:pPr lvl="0">
             <a:defRPr b="0">
               <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
@@ -857,6 +1804,81 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2933700" cy="1876425"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr descr="fdg" id="4" name="Chart 4" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3476625" cy="2171700"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3962400" cy="2447925"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1067,8 +2089,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
+    <col customWidth="1" min="1" max="6" width="12.63"/>
     <col customWidth="1" min="7" max="7" width="14.88"/>
     <col customWidth="1" min="8" max="8" width="21.13"/>
     <col customWidth="1" min="9" max="9" width="18.13"/>
@@ -1076,209 +2099,1427 @@
     <col customWidth="1" min="14" max="14" width="15.88"/>
   </cols>
   <sheetData>
-    <row r="12">
-      <c r="K12" s="1"/>
+    <row r="1" ht="15.75" customHeight="1"/>
+    <row r="2" ht="15.75" customHeight="1"/>
+    <row r="3" ht="15.75" customHeight="1"/>
+    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="3"/>
     </row>
-    <row r="13">
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="3" t="s">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="K12" s="4"/>
+      <c r="S12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="U12" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="V12" s="2"/>
     </row>
-    <row r="14">
-      <c r="K14" s="3" t="s">
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="O13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="4">
+      <c r="S13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="10">
+        <v>17.0</v>
+      </c>
+      <c r="V13" s="2"/>
+      <c r="W13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="K14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="12">
         <v>12.0</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U14" s="10">
+        <v>13.0</v>
+      </c>
+      <c r="W14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y14" s="14">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="G15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="W15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y15" s="14">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="G16" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="16">
+        <v>5.0</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="W16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y16" s="14">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="G17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="16">
+        <v>7.0</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="M17" s="7"/>
+      <c r="N17" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="18"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="G18" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="16">
+        <v>5.0</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="18"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="G19" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="16">
+        <v>7.0</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L19" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="18"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="G20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="16">
+        <v>9.0</v>
+      </c>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="G21" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="V21" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="W21" s="21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="22" t="s">
         <v>4</v>
       </c>
+      <c r="V22" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="W22" s="23">
+        <v>13.0</v>
+      </c>
     </row>
-    <row r="15">
-      <c r="G15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L15" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="4">
-        <v>10.0</v>
-      </c>
-      <c r="O15" s="4" t="s">
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="V23" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="W23" s="23">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="22" t="s">
         <v>9</v>
       </c>
+      <c r="V24" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="W24" s="23">
+        <v>5.0</v>
+      </c>
     </row>
-    <row r="16">
-      <c r="G16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="4">
-        <v>10.0</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>13</v>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="V25" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="W25" s="23">
+        <v>8.0</v>
       </c>
     </row>
-    <row r="17">
-      <c r="G17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L17" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>17</v>
-      </c>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="N26" s="7"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="27"/>
     </row>
-    <row r="18">
-      <c r="G18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="27"/>
     </row>
-    <row r="19">
-      <c r="G19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="25"/>
+      <c r="U28" s="25"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="27"/>
     </row>
-    <row r="20">
-      <c r="G20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="6">
-        <v>9.0</v>
-      </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="25"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="27"/>
     </row>
-    <row r="21">
-      <c r="G21" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
+      <c r="T30" s="25"/>
+      <c r="U30" s="25"/>
+      <c r="V30" s="20"/>
+      <c r="W30" s="27"/>
     </row>
-    <row r="22">
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="25"/>
+      <c r="U31" s="25"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="27"/>
     </row>
-    <row r="23">
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="R32" s="24"/>
+      <c r="S32" s="25"/>
+      <c r="T32" s="25"/>
+      <c r="U32" s="25"/>
+      <c r="V32" s="20"/>
+      <c r="W32" s="27"/>
     </row>
-    <row r="24">
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="R33" s="24"/>
+      <c r="S33" s="25"/>
+      <c r="T33" s="25"/>
+      <c r="U33" s="25"/>
+      <c r="V33" s="20"/>
+      <c r="W33" s="27"/>
     </row>
-    <row r="25">
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="R34" s="24"/>
+      <c r="S34" s="25"/>
+      <c r="T34" s="25"/>
+      <c r="U34" s="25"/>
+      <c r="V34" s="27"/>
     </row>
-    <row r="26">
-      <c r="N26" s="2"/>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="R35" s="24"/>
+      <c r="S35" s="25"/>
+      <c r="T35" s="25"/>
+      <c r="U35" s="25"/>
+      <c r="V35" s="27"/>
     </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="R36" s="24"/>
+      <c r="S36" s="25"/>
+      <c r="T36" s="25"/>
+      <c r="U36" s="25"/>
+      <c r="V36" s="27"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="R37" s="24"/>
+      <c r="S37" s="25"/>
+      <c r="T37" s="25"/>
+      <c r="U37" s="25"/>
+      <c r="V37" s="27"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="S38" s="20"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="27"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="S39" s="20"/>
+      <c r="T39" s="20"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="27"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="S40" s="20"/>
+      <c r="T40" s="20"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="27"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="S41" s="20"/>
+      <c r="T41" s="20"/>
+      <c r="U41" s="20"/>
+      <c r="V41" s="27"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="27"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="S43" s="20"/>
+      <c r="T43" s="20"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="27"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="27"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="8">
     <mergeCell ref="K12:N12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="W16:X16"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
:arrow_up: graficos: veterinario, cirurgia e quarentena
</commit_message>
<xml_diff>
--- a/GRÁFICOS.xlsx
+++ b/GRÁFICOS.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\is064\OneDrive\Área de Trabalho\SQL-M3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
   <si>
     <t>Espécie</t>
   </si>
@@ -134,44 +142,153 @@
   </si>
   <si>
     <t>Fêmea</t>
+  </si>
+  <si>
+    <t>raça</t>
+  </si>
+  <si>
+    <t>espécie</t>
+  </si>
+  <si>
+    <t>veterinario</t>
+  </si>
+  <si>
+    <t>data_entrada</t>
+  </si>
+  <si>
+    <t>data_saida</t>
+  </si>
+  <si>
+    <t>Akita</t>
+  </si>
+  <si>
+    <t>cachorro</t>
+  </si>
+  <si>
+    <t>Border Collie</t>
+  </si>
+  <si>
+    <t>1/15/2025 10:30</t>
+  </si>
+  <si>
+    <t>Chow Chow</t>
+  </si>
+  <si>
+    <t>Golden Retriever</t>
+  </si>
+  <si>
+    <t>Labrador</t>
+  </si>
+  <si>
+    <t>2/28/2025 12:00</t>
+  </si>
+  <si>
+    <t>Persa</t>
+  </si>
+  <si>
+    <t>gato</t>
+  </si>
+  <si>
+    <t>Scottish Fold</t>
+  </si>
+  <si>
+    <t>Shih Tzu</t>
+  </si>
+  <si>
+    <t>Siamês</t>
+  </si>
+  <si>
+    <t>id_animal</t>
+  </si>
+  <si>
+    <t>genero</t>
+  </si>
+  <si>
+    <t>especie</t>
+  </si>
+  <si>
+    <t>idade</t>
+  </si>
+  <si>
+    <t>status_animal</t>
+  </si>
+  <si>
+    <t>macho</t>
+  </si>
+  <si>
+    <t>fêmea</t>
+  </si>
+  <si>
+    <t>Animais por veterinário</t>
+  </si>
+  <si>
+    <t>Animais que fiseram cirurgia</t>
+  </si>
+  <si>
+    <t>Animais em quarentena</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -203,94 +320,141 @@
         <bgColor rgb="FF3C78D8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF145F82"/>
+        <bgColor rgb="FF145F82"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0E4F5"/>
+        <bgColor rgb="FFC0E4F5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="36">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="22" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -307,7 +471,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" i="0">
+              <a:rPr lang="pt-BR" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -318,23 +482,33 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Página1'!$I$15</c:f>
+              <c:f>Página1!$I$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantidade de animais</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="4285F4"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -342,18 +516,89 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Página1'!$G$16:$G$21</c:f>
+              <c:f>Página1!$G$16:$G$21</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Dra. Ana Júlia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dr. Carlos Mendes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dr. Felipe Rocha</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dr. João Silva</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dra. Maria Oliveira</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Dr. Ricardo Alves</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Página1'!$I$16:$I$21</c:f>
-              <c:numCache/>
+              <c:f>Página1!$I$16:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6D55-48B0-B9B8-B45FC4174BA0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="721686568"/>
         <c:axId val="490304490"/>
       </c:barChart>
@@ -379,7 +624,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" i="0">
+                  <a:rPr lang="pt-BR" b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -390,12 +635,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -408,9 +654,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="490304490"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="490304490"/>
@@ -454,7 +706,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" i="0">
+                  <a:rPr lang="pt-BR" b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -465,6 +717,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -486,13 +739,17 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="721686568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -506,16 +763,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -532,7 +801,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" i="0">
+              <a:rPr lang="pt-BR" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -543,8 +812,10 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -554,69 +825,137 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Página1'!$L$14</c:f>
+              <c:f>Página1!$L$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantidade</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:dPt>
             <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="4285F4"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5D63-4211-AA09-C7546CF33AE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="073763"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5D63-4211-AA09-C7546CF33AE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="6D9EEB"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5D63-4211-AA09-C7546CF33AE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFD966"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-5D63-4211-AA09-C7546CF33AE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="F1C232"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-5D63-4211-AA09-C7546CF33AE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Página1'!$K$15:$K$19</c:f>
+              <c:f>Página1!$K$15:$K$19</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>outros</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cobertores</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>medicamentos</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>alimentos</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dinheiro</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Página1'!$L$15:$L$19</c:f>
-              <c:numCache/>
+              <c:f>Página1!$L$15:$L$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-5D63-4211-AA09-C7546CF33AE5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -625,12 +964,14 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -644,16 +985,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -670,7 +1023,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" i="0">
+              <a:rPr lang="pt-BR" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -681,23 +1034,33 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Página1'!$N$13</c:f>
+              <c:f>Página1!$N$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantidade animais</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="4285F4"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -705,18 +1068,77 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Página1'!$O$14:$O$17</c:f>
+              <c:f>Página1!$O$14:$O$17</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>adotado</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>em quarentena</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>em tratamento</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>no abrigo</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Página1'!$N$14:$N$17</c:f>
-              <c:numCache/>
+              <c:f>Página1!$N$14:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C0E-495A-87D5-688FB8C4858E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="657405305"/>
         <c:axId val="417719007"/>
       </c:barChart>
@@ -742,7 +1164,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" i="0">
+                  <a:rPr lang="pt-BR" b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -753,12 +1175,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -771,9 +1194,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="417719007"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="417719007"/>
@@ -817,7 +1246,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" i="0">
+                  <a:rPr lang="pt-BR" b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -828,6 +1257,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -849,14 +1279,17 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="657405305"/>
         <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -870,16 +1303,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -888,7 +1333,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0" sz="1600">
+              <a:defRPr sz="1600" b="0">
                 <a:solidFill>
                   <a:srgbClr val="666666"/>
                 </a:solidFill>
@@ -896,7 +1341,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1600">
+              <a:rPr lang="pt-BR" sz="1600" b="0">
                 <a:solidFill>
                   <a:srgbClr val="666666"/>
                 </a:solidFill>
@@ -907,19 +1352,25 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Página1'!$T$12</c:f>
+              <c:f>Página1!$T$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -932,8 +1383,11 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="1"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
@@ -944,9 +1398,16 @@
                 </a:solidFill>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-CECD-4255-A206-CCC8F01C7F3F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
@@ -957,39 +1418,114 @@
                 </a:solidFill>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-CECD-4255-A206-CCC8F01C7F3F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Página1'!$S$13:$S$14</c:f>
+              <c:f>Página1!$S$13:$S$14</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Cachorro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gato</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Página1'!$T$13:$T$14</c:f>
-              <c:numCache/>
+              <c:f>Página1!$T$13:$T$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-CECD-4255-A206-CCC8F01C7F3F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Página1'!$U$12</c:f>
+              <c:f>Página1!$U$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantidade</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Página1'!$S$13:$S$14</c:f>
+              <c:f>Página1!$S$13:$S$14</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Cachorro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gato</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Página1'!$U$13:$U$14</c:f>
-              <c:numCache/>
+              <c:f>Página1!$U$13:$U$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-CECD-4255-A206-CCC8F01C7F3F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
         <c:axId val="1300976426"/>
         <c:axId val="286182791"/>
@@ -1015,24 +1551,17 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -1045,9 +1574,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="286182791"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="286182791"/>
@@ -1090,18 +1625,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1123,13 +1651,17 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1300976426"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1143,16 +1675,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1169,7 +1713,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="pt-BR" b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -1180,23 +1724,30 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Página1'!$X$13</c:f>
+              <c:f>Página1!$X$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="4285F4"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1204,8 +1755,11 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="1"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000"/>
@@ -1216,9 +1770,16 @@
                 </a:solidFill>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-BBB1-44F0-AF88-75AC847E5617}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="F1C232"/>
@@ -1229,9 +1790,16 @@
                 </a:solidFill>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-BBB1-44F0-AF88-75AC847E5617}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
@@ -1242,39 +1810,123 @@
                 </a:solidFill>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-BBB1-44F0-AF88-75AC847E5617}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Página1'!$W$14:$W$16</c:f>
+              <c:f>Página1!$W$14:$W$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Filhote</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Adulto</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Idoso</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Página1'!$X$14:$X$16</c:f>
-              <c:numCache/>
+              <c:f>Página1!$X$14:$X$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-BBB1-44F0-AF88-75AC847E5617}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Página1'!$Y$13</c:f>
+              <c:f>Página1!$Y$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantidade </c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Página1'!$W$14:$W$16</c:f>
+              <c:f>Página1!$W$14:$W$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Filhote</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Adulto</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Idoso</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Página1'!$Y$14:$Y$16</c:f>
-              <c:numCache/>
+              <c:f>Página1!$Y$14:$Y$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-BBB1-44F0-AF88-75AC847E5617}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="1084108329"/>
         <c:axId val="2139942766"/>
       </c:barChart>
@@ -1299,24 +1951,17 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -1329,9 +1974,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2139942766"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="2139942766"/>
@@ -1374,18 +2025,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1407,13 +2051,17 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1084108329"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1427,16 +2075,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1453,7 +2113,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr lang="pt-BR" b="0">
                 <a:solidFill>
                   <a:srgbClr val="B7B7B7"/>
                 </a:solidFill>
@@ -1464,25 +2124,43 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="15"/>
       <c:rotY val="20"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="1"/>
     </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Página1'!$V$21</c:f>
+              <c:f>Página1!$V$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gênero</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1497,8 +2175,11 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="1"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="F1C232"/>
@@ -1509,9 +2190,16 @@
                 </a:solidFill>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DCB3-4478-9243-DF98E78537EF}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="1155CC"/>
@@ -1522,12 +2210,26 @@
                 </a:solidFill>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-DCB3-4478-9243-DF98E78537EF}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-DCB3-4478-9243-DF98E78537EF}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="1155CC"/>
@@ -1538,41 +2240,150 @@
                 </a:solidFill>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-DCB3-4478-9243-DF98E78537EF}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Página1'!$U$22:$U$25</c:f>
+              <c:f>Página1!$U$22:$U$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Cachorro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cachorro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gato</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Gato</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Página1'!$V$22:$V$25</c:f>
-              <c:numCache/>
+              <c:f>Página1!$V$22:$V$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:srgbClr val="000000">
+                        <a:alpha val="0"/>
+                      </a:srgbClr>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-DCB3-4478-9243-DF98E78537EF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Página1'!$W$21</c:f>
+              <c:f>Página1!$W$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantidade</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Página1'!$U$22:$U$25</c:f>
+              <c:f>Página1!$U$22:$U$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Cachorro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cachorro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gato</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Gato</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Página1'!$W$22:$W$25</c:f>
-              <c:numCache/>
+              <c:f>Página1!$W$22:$W$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-DCB3-4478-9243-DF98E78537EF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
         <c:axId val="1913273333"/>
         <c:axId val="867643121"/>
+        <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
         <c:axId val="1913273333"/>
@@ -1595,24 +2406,17 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -1625,9 +2429,15 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="867643121"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="867643121"/>
@@ -1670,18 +2480,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1703,14 +2506,17 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1913273333"/>
         <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1724,27 +2530,35 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4457700" cy="2571750"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Gráfico"/>
+        <xdr:cNvPr id="2" name="Chart 1" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1753,7 +2567,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1762,14 +2576,14 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3962400" cy="2447925"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2" title="Gráfico"/>
+        <xdr:cNvPr id="3" name="Chart 2" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1778,7 +2592,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1786,15 +2600,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3533775" cy="2171700"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Gráfico"/>
+        <xdr:cNvPr id="4" name="Chart 3" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1803,7 +2617,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1811,15 +2625,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2933700" cy="1876425"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr descr="fdg" id="4" name="Chart 4" title="Chart"/>
+        <xdr:cNvPr id="5" name="Chart 4" descr="fdg" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1828,7 +2642,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1842,9 +2656,9 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3476625" cy="2171700"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
+        <xdr:cNvPr id="6" name="Chart 5" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1853,7 +2667,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1867,9 +2681,9 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3962400" cy="2447925"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
+        <xdr:cNvPr id="7" name="Chart 6" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1878,17 +2692,191 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAeAAAAFoCAYAAACPNyggAAAAAXNSR0IArs4c6QAAIABJREFUeF7tnQW8lcX6tp8ddJeiggiKnWBjH7EVUBRUjoV45NiePwp2Y+uxu7tB9GChYie2iC1KKB0Cu9b3XQMDL4u19pqd7LXee37yE/Z+Y+aemed6npl5Z/ISiUTClKSAFJACUkAKSIFaVSBPAK5VvfUyKSAFpIAUkAJOAQFYDUEKSAEpIAWkwEpQQABeCaLrlVJACkgBKSAFBGC1ASkgBaSAFJACK0EBAXgliK5XSgEpIAWkgBQQgNUGpIAUkAJSQAqsBAUE4JUgul4pBaSAFJACUkAAVhuQAlJACkgBKbASFBCAV4LoeqUUkAJSQApIAQFYbUAKSAEpIAWkwEpQQABeCaLrlVJACkgBKSAFBGC1ASkgBaSAFJACK0EBAXgliK5XSgEpIAWkgBQQgNUGpIAUkAJSQAqsBAUE4JUgul4pBaSAFJACUkAAjkEbKCsrs/z8/KwvqT+6Oi8vL+vLogLUPQVWZvsqLi42+qlPpaWl1qhRI6uutp4rNqDutZqq5UgArpp+dfruefPm2RdffGGTJk2yddZZxzbccEOrX79+nc5zusz9+eef9tlnn9mCBQtso402ss6dO1tBQUFWlkWZrlsKAN4//vjDPv/8c+Pvm222ma2xxhq16rQ+8cQTrn3TpktKSqxDhw523HHHWb169aok1rRp0+zTTz+1v//+2/Wbtddeu1bLVaXMx+BmAbgGK3n+/Pk2fvx4w5sl0bkbNGhgG2ywgft/TacrrrjChg0b5t7bqlUru+WWW6x///41/dpqf/706dPtjDPOsHvuucc9e4sttnB/33zzzav9XXpg/BT47bffbPDgwfbiiy+6wu+66652//33W8eOHWtFjBEjRtgpp5xiv/76q3sf8L3xxhvtgAMOqBIsFy1aZEcddZQ99thj7rnYnYcfftj1H6W6oYAAXIP18OCDD7qODYh9ateunfHzPffcswbfvPjR22+/vb333nvu7wxBH3HEEXbvvffW+Hur+wVffvmlHXLIIc6Z8empp56ygw46qLpfpefVsAKMZDAcykhM69ata/htYY9/5ZVX7JhjjrHff/996Q2ffPKJdevWLewBVbjq66+/tkGDBi3tp9tuu63ddNNN1r179yo8dfGtjICtssoqbtSI1KJFC7vsssvs3//+d5WfrQdUjwICcPXomPIpvXv3tpEjR7oI1CeGmI499li77bbbavDNix9N9HvttddaUVGR64iXXnqpe3e2pcmTJ9v//d//2SOPPOKyzlAajsRWW22VbUWJdX7nzJljp5566tLh0HPPPbdO6PHdd9/ZySefbC+//LLLz3bbbefa2lprrVWj+fvpp58cDF966SVr3Lixi3gZtVpzzTWr5b0LFy60vn372gsvvOCex9A6cN9hhx2q5fl6SNUVEICrrmHKJ+BN9+jRwxjeItHBmIchbbLJJvbWW285j7QmE0O3DzzwgBF1rLfeenbooYfWytB3TZTpm2++saefftp58z179rQdd9zRCgsLa+JVemYNKQDUjj76aOcQMjrzzjvv1NCbKv7Y999/3/73v/+56LxXr14u+q3phYtvvPGG3XnnnW6KCuj/85//rNZRARz/CRMm2OOPP75U83322afi4uiOGlNAAK4haa+//nrDw2cYiI7MUPTNN9/s3sYw9H//+18HxIomvFrgTqclqmVutybS1KlTbebMmQ7Yq666qnMgkhO/B+6AkHmr0HltHBHu4/9ow1Bk27Ztq8XgYXT++usvmz17tjOmzZo1c8+uzsVn5H3GjBlOE8odaqgBD3mbO3euy0/79u1T6hpan7QDpjfQjzaVKlVlZW9597Jql4VLtMemTZtamzZt3Krd8tIee+xhDPeSmGcdM2ZMaFGdbrQ3VgXjuNL2K5PoN7/88otrG6uttprLe1US86z0FRzD5s2bu3oIdQxnzZrlNKRdUCbqkWeEtqdovikXzyIflIvnVCbRntCaeqV900ars+9UJk+5fI8AXEO1yxyvH9LCWDAXy6IhjC8Jb5foNFVizvOOO+5wEMGo3Xrrre4+vOUPPvjAdRAMCJ1s4403tiOPPNItsEhOd999t4u0MaQNGzZ0Q1z77rvv0svI30MPPWQYUyJKFmzgMROpMDfFkCGrMMn/LrvsYocffrgD2vfff2/33XefWzVKHjE4XENUw3xWKlgDLPLy7rvvGkNvGFOMhTeoDLvtvvvuxrB98upmInnex2pOD2yG7ojqfaKMrCR9/fXXnYOC44NRIi8YRa5l6G3rrbe2Jk2alFvr3Pfaa6+5YW7yR70df/zxNmXKFLc4Z9y4ca4+0LRLly522GGH2c4775z2mRhGFtoQZfEMyo1mOAaMhvTp08f9PzlRz7yP+UjKffbZZ7uV7OhAvX311VcGAPbee28bOnRo2vezoAfdcZBYYUs977bbbisYevJ211132bfffuvqgOtPOukk23TTTZc+m7IQUX388ccOPMADHah/pgQOPPDAFYZQWYlLW8ch9aNAGHaiMbTmGUScJ5xwwgoQpx5GjRplP/zwg2tr1AdtEN0pN3+SE6uJ/cgP+broooscaKmDZ5991n7++Wf3b95HHhilon0xFI3OAOz000938CHR15gCoRzcR3+jTfA8Fm5NnDjRlYG21qlTJzv44INdf0m1gpm2TORLW8ARoEy+H9CfGfbea6+93BqR5PuZirnmmmvcVw30F9/v33zzTddn0Qh9zzrrLNtvv/1cXTPnS3+jDGjBPdH69NrxtQTTZdge2h02gfpHi2222cb1S5xNpepVQACuXj3d0wAThoiGT2IBER28X79+9vzzz7ufsRLxmWeeSTnPxJwNRpIOjyHkOgwKP8czjSYMBlAhuk5eNDJgwAC36pEEyJkTjs67XXnllXbmmWe63wNwjAzvGTt27HLz1vweI8s8GcNzgACY+tXdPj8YICDNPFPUa8YQkA9WegL16Jx4tCx8+kGehw8fvtz3jxhMwI4xJhFtAVsg4g3kaaed5sAAFFIlDDdRF3PizIWVlzCmlOE///mPuwwnh6FTykz9JZcbuDN3hzbJCVifd955zjGILsaLXrfllls60LFILpp+/PFHB/5XX33V/fjRRx91oxHojyPmv+0cOHCgc9jSJer9qquuWppv2iYGO3nEgvLhBFF+30ajq82B+IUXXugA4q+JvpM2hsaUF6NNAmrnn3++a8MY9XSJ9z755JPWsmVLdwkak2fKBaiS2wz1CRBoF7ThaHsDsuiJs0ACkPyM5/F3Es4PbQFHGAeHT35wbEisfsY5XX/99ZfmBd2BJ5rhcNF/ATt9NDlx/3XXXbeCM4mzhJ7UB+BNl7if/FCuKISZhqHN08ZxBHDIiZzpVzjFPrHIk36IraBtcR8JvfgSYv/991/u1fQb8osO9NXkRJmpH75E2GmnndLmW7+ouAICcMU1y3gHRgqD7FcfYuyAMHBjtSUJQwNoMLDJiUUZGAY8UQwNXjVGqLyEIbr88suXm0NiwRUdHuNF1Ad8PXB5FsPkgItER2cIDCOTqhNyDZ2daBJPO10ivzgKyZEJ82ssCPERkB+uw5gQrfpEZ0cvIOETn2eg0+jRo92P8MqBkY86+TsGyz+HPABpyoSGvjx8goWjkmn1LaDAULFgiITzgXPB81OBh2vWXXdd57hgqH3CKJ544olLR0LKqz+cD6BPpOETjgdTF7QHEqMXtAMMqgcSkTQRD20uXcIJwCAT2ZJoC9Shj/D4GWW+4YYbnBPm0znnnOMgg56ACwfSr6rnGqY/unbt6iKy6Api8smziFKZtyfSTOcY+XclA5j7AXkUVDhClJcI1ydAdMEFFyx1lvg5ThLv9LClzz333HNu2sCn1Vdf3RghItrkebSfjz76yP2ab+Zpw9QpCWeA7855no/AAX4q+Prncz0OS1RjfkfEHB2FStcPcGaI/L2Tyb04M0TG/nMlfodDy2hENDHMj57YH0a2ACuJqJnFn9G+SZ/CWSmvT/tnM4LEaIo+/yuvJ1fsdwJwxfTKeDVRCZ3ERy0YbwwpHZH/06k9EPCkfYQafXAUwP7ndEg6CgYDzxbjgXHzCa8ZIxONgisC4KjhwEPH+6fjMrSJ5x5NOASAhUVmXAP4fbTBdf/6178cwKJzWYAdL5tRAUCIcfZDohha8u51wUBhfHzKBGCiZiCM9hho8ga4+DcGCmjgADDnzhBcppQMYH89w4oMfeMAEAUSUfF8ErAHBMDQG23KO2TIkKWvwwByP0O1GG8cIIYiPUz59ITn+nnJZADzDmBAuXCEWA3OtThrOHjlJYZF+XTLJ4a2oxE39UeU7+docSRw3vyiHUY/MN4+iiXav+SSS9xwMHOZRKrUuU8YauqB+XI+HwM8QNU7pQyDMpzK8ygT7yOqpP4YBmUEyEekOD88n090aFNMj1C/HvpEeZSH4XlSMoCBJY4T8GQjCoZ5qUPqhqH/igDYl4980s9xDHGmiSIZ5Yo6k/RPpheiu1mhB8PCtBucTEBNP6CP0XbIu28P1AdTAr4fJQPYT9WgH30SZ4hyEhljZzIBmLzSduh7PmE/iKiJlqk3RgkYifEJx4a6ra4dujL1xVz/vQBczTWMAWVI0A8/00lp4IAYbx5D6I0cniRGLvnD+GQA09mJxjB4ftiQIUhAx3C3T0D/H//4x9J/VwbAvJtVxnQwOjDDTkRmPhEFE23RSX0ibxhfb5yJTFlgEwUwRsXPy/KMaAcmckQXjBMJUHkvn39nAjCGDI15R6rPvMgXBg8nJtX8dHITSAVg6grD4z/h8POCRNQ+KgYqvj6IKICIX+kLPIEIPyP53ZeiK+Ux5EAKo0hKBrDPJ/rjdABfNKZMmcoFHIhucYRIOHJEeb6OPvzwQ7cS12+HiKaUDceRCJcFVICPRATN3zH6PjEfTZ58+XF2cDD8YimmDOgXHlDlLcJi9Ihhdj/Uz3wsbd8v8sJRAzL+e1aiSJwhothUAOZnDDmzloIyAmTKzX3US2UATBtnWN2PpuAU04ajjiMOGeWILspCX6YiqH+cl2g/oA3jWDAXTwKGROXpAMw1jELwHuoLG8PzyRPvzARg5nxxkqLD8kzz+DlinsX8Mm0l2sZpx36KoZrNZ+weJwBXc5UTPTK36g0Z8MJLBgwYdoyAhxcdhmFoP9Tps5IMYIwr0UB00RGGFMMUXciFQY1+ZlBRAAMXoiQ/jIqRwChEh4OZb2aOyQ/PkWeGjCkDw72pDEcqiTEOLMTC82dolGFCP0wJoImqfMoE4Oj3ztyDrkST5ImFZxVdxZkKwAzxA+DovCnGEQeLcpCISikLw99vv/22c2T8nD1zZ7fffvvSeUVfNqYAWBGP1hha4Ass0wGYMjGn6udKQ5svzh/DkUSXXiMiG4ZiqQNgGV3IdfXVVy8d1mWxkV+Exr20Ab/AkH9j7HGeGLL232pjoIneGDYmsRsTGoYAGCeFiNYnIkmGVH1kCDQBfhQCTK0wEpMOwLRrotFUK4wrCmAcEMqavPAN2OI8eMeBusIWlLedJP2AoXGcCpw1nCQWW5EYCicK9ZFucgTMNdiPdAvwMgEYpya6JgR7QTuILlJkpIZI3DsW9C36QTbuJxDaV2rzOgG4GtUGGgwF+giXR2OQgZWPzujs0YiX4VgMbtSwJwMYw+6jQ59dDBlGJzrsV1UAE0EQSUQ/YSCSjUbVAB7PP5pfOif3esNBtOhX7vr84vVTLgw04MKBQBP/Bwh4A1tRABMpEpF4T96/E8PHcKNf4BT63XUqADM8yEYm0UQdMKTp64ZohBEQIojkuT6GexnOA87RRN0TGXqHDSeIxVDpAMzvKruRQnQYmcgL55AoEseH6M2/l2FZnAWiRRJROYbaD7cDBAxxciJK8qMgTGHgHPrNUkIBjMHHGfOLFb2zkLwynrbi1xNwDeXwn/klD0Ezvw7I0n1yVFEAMyqAPjh30QR8GZ3ww+zojSMTBTBthvwxZI1T7UckeI5fEe77AW0L6KYDMEPOODnpFkZlAjD9Ijq6BXzRMZpf+i3rAHAkfLr44oudA6JUdQUE4KpruPQJdCyGdPzmG/wi2fulc0UXOTFvxdwa0YlPyQAm8o1uw8h1dAwA7I0OP6sqgBluZj426gGzeje6EIRFQqwojSbeS3STDsDoQQTFPKxPRCIYFh+RYLwrC2CeCdQx3HxGlWqhFNESxob5wkwpFYAZ5iPyjCbyy1yij9yJStGCz7EYcmXRkk+UHyPGsGM0oSWL0zyAyZ9fDJQ8BA30mHpI9RlJpjLxe6Jy3uXzi+FmiJFFWtG1A0Sg0S1LcTyYt4wCL9X7/HAqutBmATDRMikUwDhR1KNfQ8G9PDfVyvno+9CX0SVSMoDJA45Ruu+UKwpg1lvwGVgy+KhfAOx1SgYwC+hYg8CUiy9TtB9QRtpeKIApF8PB6Vb1ZwIwUSxrSXxiOgxHMersMIKDExGNlIn0iZ6Vqq6AAFx1DZc+AYARQVY0sRiF4WSfkgFMRMJ3etFUEwAmyqNzRecTkwHMMB4RcDSVB2DyCbzoxD4xH0f0QNQKwBi6jg5hVzQC9s/1i9MwSgyvJn/2w3AxRpqFL+WlVABOZXQwcETY0QiYoVkgytA9WvkEVKjn5KFjFo8xd+oBHN0hKhnAOEasrK0sgMkLc848g8TzgC9DvAzjk4jiqSu/Wp+fMbSLwfV6Mkdf3l7FOJhcw1QLURopFMAsrGJEIDrEzVA+jku6z9eoBxxD1kSkAjCRPHOb1QVg5r4ZyaGuoqk8AKMdQPYHinAfkTSfBAFypgKIdok2/RxwpgiYRWlE4unaQyYA47Rwv0+MpuFIR+escSYY5o4ClzzWlW1EK2pr69r1AnA11Ugqzz3deZ4Y2+j3vERKRLJ+eDKXAIwurB72i9IYBmRIk3klnzA8DHP7ldSVBbB/HgDFSWBulU80/LAoc8HMLWY6ESoVgDHuzH1FRzSYXmA42H/egmMB0FhBSsTFQiOfWMiCgUuGP8YMB8XDhQMm/GrlmgAw2jNniHEmoiayxYHy31gDaOAS3Y+YaJi5SV9OHBmG2CuyY1MygBlV8e+MdkEMPhE43wT7RNTvI+mQ7pocAdcFADPqgDPiN+KJfofsy4RjxJcRfgFiTQOYYeTotEryYjfyxbQao3r+aw0id9oQP1OqugICcNU1dE/AYLBE3y9EwtACVoAT9dwxWsz7EPn4IVs8aoaC/FxrLgEY8PK5jHc4GOokQo1GUBhn5p78YqaKApgFRkRIyUCgLog6/HFs1BMQZKVpeSkVgFMN9zHnBzx92TCwDIGT+FaXb2/9N6sYXOZ7o9+AAhtABGBIRKQ8z3+LWxMAJrpCe1Y240yQH4ZEPVzRC8clmpI3lqFNs2o61e5r3AfcqYvoOoHkVdDl7QXN1Ep0zpG5SrROFcESbfvduHz910UA44hGnZpUixnpFzhHvh/UNIDpF4w8+SkJpsP4Ljh6DCOr3VkBT3shYdeYMuNnSlVXQACuuobuCcnDz3iTRDeptj3E2PENYnQ4CoPjvxnNJQDjzTMk6zctYEEMiziI9DCcGCbgy/ewPlUUwAz7A2DmwliwxiIyol0cHRY+RReqEc35T4HSVX2674CJ2llsxrtwLACDj1aYN8MB8/ACQpST4TufiBwxeBhiFp3htDHc6yN0hrNZwMfqV1JNAJjnEmWxCIhEffjFa7wfCDDkm5wY4mU1tE84DpSNoVO0pgxEdwwhM+rAqAdDpD4R7VLnfmMNPk8iquL9DM8yKsS8MXWPBjhJ/vtTHAUWCLESmt/j0KIv0RkODo4MdeOnTuoigHF8mG7xCa3Rj0WNtAXaE1FldFONmgYwecJJjO7Jje6sxKcPYacYoo7uVcAXESz8qqk96KvJHGfNYwTgaqgqFkgxREkk4RNGgP1Y0yWioegwLHOiLBLC+8wlAANByhld1comHCw6w5Cy2AbvGuOJUeVnFQUwURxDotzHfDnGjeex6CW6bSK/4/vRTN8wJgOYYTf+AAkiWYwPC8uiG5QAFAwZ0b5PwAHYR7/VxrABHUCEAfRzv0SLzDNH59ZqCsDkE82StzUlqkHH5BXHlIfhURYQRXdMwtkhksUhYXUvevvdtliAFd0chNEI9I/uiMUQOKulmXpg2B7nyC8oIgoGutEFdQCdCAzNaFeMNlAPDO8zbO+d3boIYJwFdqCKOpqUBUeF9kY/oD3gbBDV0w9qGsDUK58UsuWqH7njZ7RxPkUkP9FV2tQR0zDR3dqqwXzG+hECcDVUP8aGhSN+dTMGlg7l95JN9QqGHfF+/dAfxoNhOn7GamFWI/qokc+YmCeNJgweUbdf+cnvkldBYzD9d8IAyS+y8s8h+oru1ITRYxV0dBFW8mdIqVZB80E/DohfPAKEgA6GHEPC7wFR9NveaFnYtAF4Mj8LhDHo/pMXrsOwE3n6z7sw/ERwfo4Vw+a3qUxXncyvs0LVf5NdXrWn2oqST6uAB1BMTkCV0Y7o5iT+GvKMxlEIJ99P3bP4hWHW6DfLREXk15cb48wK6Ux7WWdq0gCMOoqurE/3bWv0WWhOHnEs0i2I4nrqEphGF6Hxc3Rgd7DkvbT5HZ/m4ZT6BUUsbGPxFxF5uj20fd6SP40jUmc0wq8pYMidT6zSLcLicyDal9+ykSkhnGD/3T35pU9754ERDKLC5M/BmE9lsZJ3bMgDIzDUKc9gxIPFbf4zpeR68t9Js4CPa3DGaW/eIcK5YRTADweHrILGafELOHkeo0HJgQGjNtSrnxJL1X4oP7bBb3aSqY3p92EKCMBhOqW9CkPEMA3RK3NjREU0cIagyxumAVY0eiI0oh+MDBEQC4SYX6OxA2fmtfCEk7espIPyTjxYgOlPS4quzMQg+K3tMD44CX6XJQrEHBAGguiOfANRotXoN54YJz5XwIhgWBhGJd/RxAYCDKdhoMgvhgtj6ufkGCLEuSCvOBKUlfxgEIAom1HwbAwQkAbA0QU6aIUx5pMZVmjinTO867+nphx8zsPey3jyvA/IoAuRKXNbOA5EfZl2jKJcqYagKTObSrBYzp8URX3zM76hxcFItz0fwKL+2BKTIWucJ3/KFCAkgmNYOPlwBAwtUxO0EfQHkkTwfoi6Kk2XcvApjf8sDuigsV+1nO7ZOI4Agv/703yAC22GHZiI6ljIxdBmdKcsnsfcJk4fK5wZ9qbNcR8OFU4UkVj0mEHaNDDFIWVO3R/7R7tCe4Z0cXLZFpP69frzuRW6oR/X+oPo0x2XSSRN2aknrmcEhX7h52xpSzgTvN/DmPaXfIIV7Zu1HLQ/dMWxZE7dryrm5ziZODK0Vf5NP0AnRh+4ljzjCNOO+Tn9xvcj2g5OHo4F+WA9BXPG6dqD79NoRxmIYHm2/747Wsc47/Qh+jsgpj+SN6YY6GdMH9BOlapXAQG4inoS9dJpPCz9OaMYlfJWidKBAAsdjev8+b4YFTomQ2s+osZIRXeeIsu8h44SvR9QRzfRwMj5BR28A+MWNXBE2N6b5nl8FsHvo/kGFszF+SFYnIpkw0q06s815bpU+aV85AdjR/m4Bq8ag++Bj6EAfnj8fgclysowJM/3x9EBL4xjdGMFdMBAUQ8YD8qDAWE4DShkOoAh2gxSAdh/esEcJ2UADsCceiEvmfbG9fN8aED5/XGEGE/ymCpFy02d8IfrU22CUdFmTJ35Az6ABWXJBN/oO9AgeuwjcOMTK9oGbThd2+ddgI62S/m4j77CtES6OqJOGQ2gjtHRb79JWwWWyWffJrdH2gF9I12ecGYpi/9+lzz5PZopM3lmtMB/o8vvqfNkZ46oHUj7zWUoF1pE2wZ9Gt0ZyqcsPAtHlPxRr9yLk+p/Fx1F823ID8vjkAHVdO2BPkDf9VM7OHFcn/wtuq9X2jSOAWXw78cm0ObS3VPRdqfrl1dAAFaLkAJJCoRuxCHhpIAUkAJVUUAArop6ujcnFUgFYOaPmRZQkgJSQApUlwICcHUpqefkjAICcM5UpQoiBeq0AgJwna4eZW5lKCAArwzV9U4pED8FBOD41blKnEEBAMwqYVZn+8RBDOxSpSQFpIAUqC4FBODqUlLPyRkFWD3Kimw2VmHFNatO+XQjemJQzhRWBZECUmClKSAArzTp9eK6rkDyZhOZPjWq6+VR/qSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADXZkWXlppNmmRWVpb+rYmEWfPmZi1bmuXn12bulnvXxIUzbEFZUdr3JyxhjQrqW/v6Lax+XuFKy2eVX5wosdJFv5slSsp5VMLyClpafv22ZpZX5VfqAYsVSJjZ/LIym1NaVr6qeWZZGbNyAAAgAElEQVSrFBZaQUyFKytL2O/TF9iCovQ6YTaaNCyw1Vo3tIL87GijZWVllpeX5/7ENQnAtVnzM2aY7bGH2Zw5Zuka3aJFZgMGmA0data0aW3mbrl3df/kIvt01oT07y8rtu6t1rd7NhhkmzbpUOl8Tps2zRYuXGjt27e3wsLaB3nZwp9s1sc7WqLoL7O81A5PonSRNer4b2vS9Vqz/AaurBiP3377zeU9Pz/fOnbsaI0aNaqwDolEwj2H8jdosPjZ8+fPt5kzZ9pqq61mBQXpscO9v/76q6211lrlvpc8/vHHH7ZgwQJr0aKFrbHGGs7offbZZ7bZZpvZn3/+aa1bt7b69euX+5ySkhJ3LXmlzFVNRYmEjZg9zx6cOccalGOES83s1g6r2qqFy7SYM2eOTcKZNXNlIk+ZDDl6kf9VV101ZdanTJlif//9t9Mc7cvTo7i42Lh+9uzZ1qpVK/cHfalD8tWpU6el9VlVnWbOK7JdzhhrX3w93awgDaxKymy77u3tmfO2s/atFrcjyuvziDZt27a1Nm3aVDo7c+fOde29Xbt2FX4G9y1atMiaN2/u6on2PXHiRFt77bWtSZMmNm7cONtkk03s999/z9ieK/zyOnyDAFyblQOA99nHDMimMzhFRWZ9+pidcYZZs2bL5Q6jTydv2LCh+zmGoqioyDXoevXq2YQJE9zvMEbeeGDMaeAVTVt9col9PPeXcgBcYlu06GL3rne0bda04wrX8d7GjRu7vJFv8unzzcV0SP49atQoA8L77befMxA+YTzosJQjauyj5QUIXAe4/TsqCsHSBRNszrh9LVEy3czSAXieNVzjOGuyzuVm+Y1dFjEgZ5xxhjPmGF2gdsghh1jTJU5TaWmpkT9+F81zslBc179/fxswYID16tXL/RpNnn32WbviiiucJuhAXUcdFJ7NvXfffbf9+9//dvcBBXTwIOdn/HvkyJH20UcfubrgOX379rUNNtjA+vTpY08//bT973//s+233345w+qjE/LOe7kP6L344ot20EEHufaG9tQjmkfLG9rWAPDI2fPsidlzywUw1/13jVWt/RIAU/bRo0fbk08+aeuss45rIzvvvLNtu+22S1/t8x1tO/Sdc889166++mp3Hc/hD+2Q8o4YMcI+/fRTW2WVVeywww5bCqtUfejLL7+0hx9+2Gm6+eab2zbbbGO//PKL63v33XefnXDCCc4p8wl90DBVHWXSa+a8Ytt16Fv2+Y8zzdJFtyVltu1Gbe3Zc7e19q0W2wfaDeWlfLybtvqPf/zDunbt6n4fbZdc6+s5XX7Q+9tvv7Xzzjuv3H6aqoyff/65odmBBx7o7MLrr79uf/31l+21114Oyr1797YHH3zQHnroIRs8eHDa9pxJq2z7vQBcmzUGgPfdF/qUD+ADDzQbMmQ5AONpv/32287QzZs3z3r27OmM3xdffOEAhQG46aabXGc74IADnCF48803nWFp1qyZ7b777hUq6dafXGIfZQBwtxZd7J4kAGOkX3vtNZenTTfd1Bmxd9991+Wjc+fOzvB//PHH9v3339v666/vvGDKsOGGGzqDvtNOO7lo7K233rIZM2Y447711ls7w8V9GInVV1/dRYmTJ092zwM4X3/9tdOGckcNcaZCVwzAV5jlL45yefeNN95oZ555ptP3sssuc+8GpC+88IJzeigv/8f4YKi7d+++QvSFLtQXxhGYYpQuvfRSB4azzz7b6fjVV1/ZrFmzHCQBH9ECkRoRAzruueeeLrL75JNPXN7WXXddF1mQ3nnnHQero446yv2MvNBOrrvuOjvmmGPs0UcfdfrjOBBN004ACdEObennn3927Y284wxw/1ZbbeWgTV6IhoDge++95+qYd3sDn0n7ygIYcOCk8H+cF9o5+cFw00++++47VxfkGWPvE23myCOPtKeeespdQ7kpA22PfNOG0JO02267ud/Rlml7PGePPfZY6lA+8cQTDkYXXnihu5730pbR8f7773f9kWcyOkGd8j7egyOUXEeZdAoF8HYbt7VnzlkGYNrIKaecYnfeeafrG9T1N9984342fvx416ZoQ/Qx8kd/o6/5EZJovigbjgWgBpZbbrml0x1H1EfXlJl/M7JC3ay33nqubZCwAR9++KFz3tCKUQscHdos7Yl6ueOOO9x16JyuPWfSKtt+LwDXZo1VEsAYNjxGGjyNlQ6OsaaR0qExRhh+/g4MiGwwSBgcIPj888/bv/71L9fZQlNlAXzbbbe5jkxnJAIALOSPDk9HpaORf4wTw58YeKKqffbZxxl3DNYuu+xiZ511lv3zn/90BgNDSDluuOEGO+KII1zHfeCBB9y1RCrABOPGzzGuXIdXHZIqC2CG9v773/86ALds2dJBirwBZSLh//znP84RwAhieKiDww8/3EX60UTdUk6MFWXBCbngggtcRLfvvvs6QwYonnnmGdt///3d0OY111zjfoezQvQL8Bn2HDNmjBsFQS8iH9L1119va665pos8fNp7773tscces+OOO861o2uvvda22GILZ/zOP/98V18YXIw2xpKE40PkjDG/5JJLnAN4/PHHu3oGwkCe6BGHi7oLSVUFMNrS7nFWgANtDeeE4fZjjz3WtZnoaAD9YdCgQXbrrbfaxRdf7GADHKm7//u//3PtD/2IwoiScfgYEgXkzz33nA0cONC6devmikadEBHS7nCMqDfqaIcddrCXX37ZNt54Y5eXoUOH2l133WUdOnRw173yyisr1FEmraoC4FNPPdW1ARwIHAb6GsPrOEw4r7QLRgZw8mg/OE+0i+TpIBy5sWPHunumT5/utEBLHJ1dd93VtSPaPu0VW0Ud0Ef8aAPvo33QXvg7TiOgp63Th8jnLbfc4voA7S9de86kVbb9XgCuzRqrJIDp3O+//75rmAAY8GLMMZh0FDzbfv362Q8//OCghuHHS2WIDO/2pZdesh9//NFOPPHE4NJWFsD+vUR+RA7Ah6iYyALvmPxh3E866SSXF/JGZwNaGDuMWo8ePeyDDz5wxgsjdu+99zrPmfIOGzbMfvrpJwda3gXIMSKAHwAzPMbPvaHMVOCqABjQMwwNgDHkJ598sl111VUu3xhxyuujduoIgPInmoAcxuz00093EGFIDkMJRBkuxJnhOegAfHE6MIToh8ZEgI888ogznkTLAAQdichJGEWM5MEHH5wSwPfcc49zJIjCiXyZjwaowI164h1oTP0BXRwf4E59YcyJiKgrjDgGFoeCyD0kVRXAvJN+wP/JF44GUSwQ8cP50XwAYOBy+eWXu3qjTugXAJPRAYZp0Z16HT58uIMDzh3tikgYQFNPPqEJjhUjBYAJ7YE1/ZT6AepXXnmlgwvRHRBLVUeZtKoKgE877TRXv+QRpwFnDX2Y9qFPUdevvvqqq0faGWXCgYo6LrQFnGYgzSgIbZZr0JFoFacDxxrHkPZOGXGK0JdhZZIH8HbbbeeuoW3jCKAz+hCVA2Cgjt1K154zaZVtvxeAa7PGKglgskiHwdjg2dPJ8S7xuI8++mjXiIlOADOeNtEkEKBzADM6Cp4nxj00VRbAdCQgw1AmBpwhOvJI58eAESVizIjciJaYn8SjxqBjDJn75O+ADDgQMWAgiRw9gHE0MHK8B8NJFER5u3Tp4vTB62aYOiRVFsAMQTNHi5HFsGNgiVqZD6TMRASAkvL5OiK/1AnX+wVWGDOGh2+++WZXjo022sgZMxwThuhxYHCoeBYRA7/nZ4xoENVQ70RYlJuoDmMKCHgeieHAxx9/3DkpOG9AE+NGHom8AReGk3cy7DxkyBDnwAB2ysc7aU9+/hgg8R7upa6IdHgW7yfyQRcirpBUFQATkQIMNGMeG3Aw6oDuwJA840zgoPpFYz4Cpgw4arQxoAIYARTlB0oMZXMNdcdQK44HfYy6pQ6pM5xKP2yPAwT8mRLC8eM+nDHaLiM4XEd9paujTFpVBcD0M5wA8sawOXAEgvTFQw891Dkc9Fn+Tl5xhmkD9F1GEEgMT+OUoDUOFm2TUSqgSpsHwNgmnD0cPbTjWdgn3ukBzHAzWjLXji3yYGfKhdEU2jF9obz2nEmrbPu9AFybNVZJANPomRPF4Pn5UDxXgEt0TGfBaBKt0LgBNCBmGJrf481iMCuyQKmyAMYQkgfggPHi3xg+PGyAC1wxnkCC35M3DBqOAsYbuPgomqFBFtjsuOOObmgLQGMguY7hdoACyIjAiL6IuJk/xlCEpsoCmKFZDDjREcabKBjI4UwQxTPaQL0wNAsE+DtTA34lKeWl7NQtEQoRE4abaA7jBBQAMIaS8gJAphB4H9pxDfcDSSIIwIPm6MyKXEZEfALKRIb+kw+GoJmfJv/cS30wjEg+iVhwZIiIqQt0pg2hNffg+Phhf0YjqCMASP1QNiL06HB3efVQWQDTXpiOAXDkiciVtsToCkafkQL6AL9HI4ADaKJzwDiBOIVoQp8issMxQUP0BZjcQ58jmuMdOI/AlPcTxdEn+Tn1xFwnbZ3oEt1wALgfp4BokXrDoUxXR+XpVFkAUyc4Q/R78kK7AJi0XUaRmMIgP4wwoQ39k7qmv1HPfnEfMAWe2BASutLmadNMXeDwAF0cDEZxeB+2iPbAiIMHMLpwDe2RKSmmDGg/OKhEvyxcA+I4BOW159C+nQ3XCcC1WUuVBDBGmQiPBorBwMAT+TEPyMIZ/3kBBpSOhdEhAsRwM4SJQWJuuCKpsgDmHXRMFngQFQBQwAmgyCcdl+iBa5inxSjgldNpMXSUlZ8DEgwh9zGXzM8BLL/z13GPn6tiLhmPmrnUinzOVFkAA06iP95JPigribxRPhwBEkPTOEqUHacJ48e9vtxcA7QxfhhMv3Ka52Ls0ZGohPvRgoQ21CdtgZERfoex822B66Irzv2nTrybdsG7/L38nXsxxMAEg8jv/GpuhrPJH5Gwn+tmAQ0/86vWuYfha8rEz6LDlzUBYJ7JO9HFLwDi3SS0BzbUCXnk9/yOFbg4GpSRIXI0pM3QPnEaaIPUJ/dTT9QfP2OkiTqkfik3CT2pF9owZcXZRW/qjH/TVtGPd6EfvyeVV0c1AWDySftAB/LFSAC6UHa/sIwyUhbKTtsgz2hCmel3fqU7bdZ/TUH5/FcKtBuezTvQGQ38anA0QQf+zSgcToofMWJ0guu5hj7NaAb/xl5las8VsWN1/VoBuDZraPr0xd8Bl/cZEr/r29ds2LClq6B9BEw0hPdNhMIQkDcINVGEzT++wD6fU/5nSJu1WNvu3WCgbdF0MXyyMZX+/Z3NGbeHJYozfYZ0vDXperVZwbJVtdlY3rqUZyLgZ2fPs8dnlf8d8KJEwm7p0H7pZ0iVKQNAAbg4rlX5FrYy767qPTPmFtmOQ8baNz+U/xnSVpu0tZEXbL/0M6Sqvre67geqDGNjt9J9g11d78q25wjAtVljCxaY3XOP2axZ6T9DKi4223HHxX/q1VuaOyCMEcHzxGOMfl5RE0W4edLr9tW839M+ujhRahs3WcMOW2VbW6V+xaLrmshvpZ9ZOt/+/u1qS5TMSbvLVSJRZPVb7W712x1Q6dfoxhUVYD+48YuK7N15C6ywnI048i1hfVs2t8ZZssNTddf1wqJSu+OlX+yrX2an3eWqpDRhW67T0gbstqY1aVj7G9pkKjN2K9NGKZmekYu/F4Brs1bZL46NNvh/eQnwlrMDUm1keVFZiZUmytkyk41A8vKtfn5h1m/OmChbuGRjxHTKJszy6lle3jKHqDbqIA7voIWVZOoPZlaPLQvjIEiKMmItiorLrLSsfLtRWJBn9QrzY6tTNjYPATgba015lgJSQApIgaxXQADO+ipUAaSAFJACUiAbFRCAs7HWlGcpIAWkgBTIegUE4KyvQhVACkgBKSAFslEBATgba015lgJSQApIgaxXQADO+ipUAaSAFJACUiAbFRCAs7HWlGcpIAWkgBTIegUE4KyvQhVACkgBKSAFslEBATgba62681xaYvbzB2bzppnl5ad+OptyNG1r1nkbs4K6t9NOdUtS3c9jr1v2xGYf3XQ7AvFz9utlu0Sl6lNg9shxVjx58bnGqVKitMzqrd7Smu60nhW2blJ9L9aTpEAGBQRgNRGzhXPNRl5o9sfXZgVpdnsqLTZbY2OzA843a9jUqcb2mJxswvGAbOLO/tScHZtpyzk2seckGbbW5OByTl8BTjyPk1XYIL4yiaP1OInHHySQ7hlsPk+eObiBQw04TYn8c4JOprxXJl/cw2lEnKzDpvW8K1Xi3ZzqEz3JiIMc0IqDNdj7m2MZ/cEDmfLCO99++20Hfc5fRet05eOgAE744WACThgKSexLzolCHPJA3ZPQlrOLK/Ic/y4OBOBEIY5c5ECE6krf/+NK+/vj9PuaJxYVW5Pt1rEONxxujTZZfHACiROX2MOYdkmeaKeZEoc3cNISOpA46Se6bSzP4ghE9OaEJA5/oN1VJHGwxBtvvOEOneBEow033DDj7bQ7TiPiWFJ/UEjGm3RBjSsgANe4xFnwggWzzEZeZPbHNxkAvJHZAeeZNVp8KgxHmHH2LqemYHA5J5TjBjkTlb1f+cNG7MnGlCPjOOmIY+I4MpEzVjltBzhw6gz3+ROAOC0FgHDKCpvoY8AANO8GAAAUAAA1Dh/n1BVOU+G0F06C4bjC5MRxiZwoxTm2RJscwccJShyD6I9s5D384XQiTt4Bfhg8EkaW9/rTYUJqGKMJgNGjPACjHcf9+YShff/9991RhOSFYwo54s5vao+h5/Sa5L3BgTYAwbijJ44NYCUSR2fKw/8pI//nyDnO88UB4PxhNEVfYO+h7Z0A/y5O1eG4Ow4Jeeihh1y9AHyOOeRMXY5M5IQn8ojRR2PK4E8Z8mc2kz/qGJjzZ7fddnMn50ydOtWdwORPV6IeAFboWc9ewwk7DrcF436zdHs0JhaVWONtuljHGw+3RpsvO1iEIwk5VhCHDn3Yg51zk9GFctEG/YlQ/l3AF4eOoxFpS5yVS7uhLL4fvPDCC6594yyiDU4rKbm8/AynhL7hE/o99dRT9u2339r222/vjgmk/9A+qDN+Hz1pi35DPvnz2GOPueM8GWWJno6Gk0d7CD3FKqS965owBQTgMJ1y+6oFsxcDeFIGAK/uAdzc6UGHv+2225yRwgBwQPejjz7qIAjcMJ4Yc86ajab777/fGTWMwWWXXebggHEDTJwvetFFFzmjxOkpAIHzZjFUGF7OssWQYJgwPBgPf+g5EHj++eeX5ssfA8e5ph6e5OPaa691ETcGkLxxaDiQIXIj70TmvJOoDihh+DGeRJFAzR/GDrDJd0gi6gkFMIej+/Tiiy+6/HDQOeC7+OKL3cHwlA0nAmNKVIxWPnH4uj97lgPOfSIPn332mTsiD9ATPXE0H04KwCNKQm/AijOFJpxvy7GXOCmAHgN/zDHHOD2B5q233uoOvt9zzz1d3aA/Z7uiOdEW2gJ5rica5Pxi6p6yUKecKcw5yICEZwO2M844w8aOHeuifv5wDi2OC2c+Aw7yBHxC04SdL88M4K27WMcbDlsOwBwyj4NB3XPMJ3nlYPrbb7/dOV9Advfdd18uG5yjiy5oRhkpO2fl+qMlca4YmcCJo93Ttig3jgugZQSA8gND7sMhpY3zbhL64EDyXEZKzj//fAd5nBv0wZkBptQ7/ZH2w8gHzheOr3ck+Xf//v1dPeMMAHQc2FQOa6jOuq7iCgjAFdcs9+6oJIABEQbYAxhhMDyPPPKI+xkHfROpJR+biAePocYoESWcfPLJLmogasWwYJiBMwYfwGGUXn75ZQe+Xr16uQgACHHNwIEDnbHBKPP3O++80wA8IGeIefTo0Q7c3EfC0BNFAiCM5emnn+6G80gYWYYZMUJE9hgongcQMVTcQyTLc3ke0U/ocHllAUz+gVDfvn0dfBgx4NxfgIsOHPaOxj5ypxwYVBwINMA4+4TxJlolL/wfR4f6evjhh532OBuAHeeGOsMBQYc+ffrYzTff7CALcBg6Bc5EVzhcRITcAygZ5uTYP+DE/xlqJR84NuSXuiJC5n7aDjDn/QAbCJA34Eq5GVlhFAPHjNEPnIdTTz3V1U+maYZoJ60sgCkPzhoABqpDhgyxI444wrUJnAmczuRztjmsnkPpyS/3UW/nnXeeG9WgbDgiOCY4QZQBfWjvlBHgA3hGhoA0cF5//fWdbhdccIH7O1pzWD0wpR3iqHIf+vbs2dPliTZNvhkpwcGineLA4KBSf7RZYE29Anr6F7A/88wzbauttso9+1aHSyQA1+HKqbWsVRLAyREwnjqdGCPCUB1GIlXC4DIk1qlTJ+elY3zfffdd590z50ZUCjiAAgaNuUnAgDEmaiNS5fcYG95DFACQjj32WPd3oiwicIY9Ge4DrECeBEh4HsaL6IB/E0FjALfeemu75JJL3NApkQRQw5kAGhgwAExUw8HuzGNzuHjo2bJVATDREs4Gxp78AkCMKkaUqCXZCcCgE7Gi7wEHLDtCkbIRMQMwok7gCgCJpImyiaxweKhXDDFODtBhpAEHh3uA5PDhw502HsDkBQCTGP6kHtGFuiXP6EaUDISor8cff9w5U9dcc42ra0YGbrzxRgeojz76yN1DHTM9wPP4Q174GU4TECHaDk3VAWDaK0Amz9TBpZdemnLIFgcJoO2xxx5uBIi/EzHjzBHpAmWexXAzTg4AZuSB9stIBtrQFllbQZmpK0Y0cIZwtOgTANkPx/MO2uc555zjtAXSxx9/vIMvbZ78kNCfkSOuYYSDoXL6ByNBTB/RF3BgGbGqqXUQofUVp+sE4DjVdrqyVhLAGFE85x49ejjDwnAy82ZAkqgRw05nx5v3Q4dkATgADTx3IjiMFfAm+sVwEx1j4DDqRJ4YJ343ZswYd48HMAtjMDbMO7MQBXASOREtY+SIwhmK5edEFUAGoDIvShTCMCdGH6hi5IkGBw0a5CIThtb5PQu7iD4AMnlmTpqo4cQTT3Q/x3iFpMoCmPLjlBDdsHAM5wUHgyiXuWEiQqIzHBUMuJ9fxtgyDwyggSX64+gwlEkkSdRPlER5uRb9cZg23XRTGz9+vCsvoCNKZageGDIigd7cBwzQmKgKWBPtAiaiP/QHyoAczakfrsXpYdjUA5hIGMeC9xIp8gyGYnGkqDfaFc8GCMAL2ACMu+66y70rNFUWwLQ1HEo0ZVSFIWLyT76JOIlm0ZKo1C+kwkHAWfOLAfn7gAEDnFNKO+Na2gK6AGBAik7UJ9AcOnSoc4qIkBlNoP6Yt/f649zgAFI/TIlQP0SytAucGUYeqCNGn8g7Tg/TCuhGW8KJAOi0baBMv6Xd0zZ4V/J0UajGuq5yCgjAldMtt+6qJIAxihhTvHw6Mp0XIwuo+DleP3DAqAJWIiESRouEh4+hATB+XhAPHiNGlMpwMM/DmBAJ4J1j2IkIie6IBImKgSSGDRgCIYwTc48YHeDuV6/yb6JDwA1ISRh/nk3kx5wcQ9QYQ4aYiTaAGFDndwzB8m8cAJ4JoEIXrlQWwAw3E51QTubteCdRLMYT7RiuJYoChBhunx/0YKgdMPN3ohscGiIrRg+oOww4Ua8HJI4Sw75ogy68GzAyh4jTRD1RBzg2zDmiD3XJPCWOFsPzGHPAwTOAObDAUaAeARrRLu/jeubTcdYYTcAxog3RRngf0GEYHVABMN7FvbQT2pWf3w/piJUFsG9DODCUmxESgImutAXaOcP2aImDREIjRgZoYzgsvr2jJ04QAKfsPIfn0laBIeVEU0BLG0Y/tENL6h2nhPdRl4zY4JACW95Pn6DecKRou7wDh5Q2gyND4pm0fe4hvzhz9B/6JiNE1A/tgralCDikVVXPNQJw9eiY3U/xAM74GRKLsM43a7Rs4ZFf7UynjXZcfu7/zd9J0X+nu5brkp/pV+qmu5/fk6JDsanyFc2Tr7BMP/PP8c/3/w6d+/XvAcAY4YquguZ+X77yNParw5MbYlSbqCa+PlKVP10dJGuc/C7/rOS69/8m/8m/8z+LXhOtGz/ykFwPFelwE3YKWAXNIqykVdDp3lle206Xr+Q6jD6DYW2AmTysXl6ZU2mdqh9E3xvtg6k0roimurZ6FBCAq0fH7H7KgjlmLww3m/xt+Z8hrbaB2b5nmTVqlt3lXQm5J2phaJ3ILh28gRGjAqx4Vqo+BX7Y6xpb8NnE8j9D2qqzrXFVP2u06bLvgKsvB+U/iVEVolGiUKV4KSAAx6u+U5eWXa5+/jjzTljN2pqttWX63bKkZVoFmOdjqC/TTlgMhzO8rlR9Csx55Wsrnjgj7QPdTlhrtLKmPbpaQYtG1fdiPUkKZFBAAFYTkQJSQApIASmwEhQQgFeC6HqlFJACUkAKSAEBWG1ACkgBKSAFpMBKUEAAXgmi65VSQApIASkgBQRgtQEpIAWkgBSQAitBAQF4JYiuV0oBKSAFpIAUyHkAl/z8sxW89ZblLVzIThCxr/EEm1YkbZoRZ1HKSkstP835vLHSJZGw0hYtrKRHD2vQofa/ha2LWrNjFBtZ+B2t6mIeazNP6MFOXKG7v9Vm3lbGu9gWtKptI+cBXMTB1ZddZnkzZ7JV0sqopzr1TvakkhuyrErS7QRVpyqtNjLDGbft2lnRySdb0wocdFAbWVtZ7+CbbYDD0YPantHcN+xAJ/l0s5VVPyv7vWw5ynaiVWkbOQ/g4jFjrPDCCwXgld1a9f66rQAAbt3aik491Zr26VO381pLuROAlxca4LAntwC8WBcBOKAjFr/+uhVedJEAHKCVLomxAh7Ap5xiTXv3dkJwZB2HOXB6DocBcEhCnJIALACX194F4ABrIAAHiKRLpEAKAHPiEvtWc4oOJwOdcMIJ7hjCuCQBWAAWgKvY2wXgKgqo2+OhQAoA+/lxznXmyECONIzT8KMALAALwFU0fwJwFSpTBMcAACAASURBVAXU7fFQIAWAOUCCs5g5rYczZnv37l3lVZ/ZJKYALAALwFXssQJwFQXU7fFQIAnARL98glOw5BOto446ys4//3x3OHxckgAsAAvAVeztAnAVBdTt8VAgCcAsvBo/frzVq1fP/vrrLxs9erSdfvrp7tzauCQBWAAWgKvY2wXgKgqo2+OhQIoI+O2337Z33nnHzfsecsgh1qZNm3hosaSUArAALABXscs7AJ9/vuXNmKGNONDS7waWYEsOJaeHtDDzAD7tNGt64IFqGLZ44wltxLGsKeg74BUdEm3EkcFUFI99ywpvvMnyZs8WgNGqLLF4Kyxty7m45ZSWmRVohzQrK7OSVq2t+NiB1qjnPwRgmsbCIjcPXq9RQ20fZ2aLFiy0kqJia9KimdrHEj0aNGxQJVua8zth/fbdVzb9u08sUVJUJaFyocWVlSXcTjb16hW67zvjnthC7u/5f1vDRg2rtJ1cLuiYlzBbVL+BLVpnbWu+5pqWKC3NhWJVqQwLFy2ysrLSxdsNxnwDV/oKIwLFJSXWvFkzY5FenFPC8qxNaQPr1GKVKtmOnAfwy1O/ssunv26zEgstP+adiE5TWlZq+fkFlq8I2NmP4pJiKyworFInyhVDVFZaYmWLiqwwX7uFLx4cKXPTE34leK7Uc2XLwWgANkR6mJUmyuyAZpvYOV17Wb38gspKajkP4GenfmKDvrvHphfPMctT1Ld4zpP2Em8PdmmP0Rzw8sZDekT0yFs89BzzaG+5BqL2sViORJnt16qbPbn5idYwv54AnE6BEVM+sYE/PGDTi+cKwJVuJrpRCkgBKSAFliqQKLPeLTe3xzYbbA0iAJ43b55NmjTJOnbs6KYuMqWcj4AF4ExNQL+XAlJACkiBCimQBGBWy/PZ3uuvv27bbLONdevWLWjfdAG4QqrrYikgBaSAFIi9AkkAnjFjhtsp7txzz7XmzZtbYWGh+5MpCcCZFNLvpYAUkAJSQApEFUgC8I8//mjHHXec7bbbbg68hx9+uHXo0CGjZgJwRol0gRSQAlJACkiBiAJLAfxva5BfaJ999pldccUV9uCDD7pztD/99FMbNmxYRskE4IwS6QIpIAWkgBSQAqkAvHgR1uTJk+2CCy6w22+/3Z0e9tJLL9kll1ySUTIBOKNEukAKSAEpIAWkQHoAs0nJnXfeaZ9//rmbAz700ENt6623ziiZAJxRIl0gBaSAFJACUmB5APdqubk9HvkMiU1K2GmQXQZDFmDxtJwH8OKNOO7VRhy+7fhNjrQPx2JF3EYLMi1LFZAeyxqD+sqKHUPtY7EmiTI7sPVW9shmxy/3HXBFLUnOA/jVKV/YFVNesVllC7QV5ZJD1vHQ2NtVyaykpMRtrSc9zB08wJ9Q7z3X208ZB3WYWb4O63A6uK0oyxJWUFj5rRdzpc2wFWX/lt3t1C57WmFe5fXIeQBP/WOytW7X1urVr/x2YbnSaKw0Ybaw1KxBoVnmT9RyptjlFWTRjLlWv2UTy9PhFFa6qNhKFhZZgxZNYlH3GQu5qGzx6WGNKm9gM74jiy4oWVBkZcUlVr954yzKdc1lldOyChrUr9JJWTkP4D/++MPatWtn9evXr7mayJIns1vL/PnzrWHDhtJjSZ1NmzbNWrVqpQ3mzWzhwoXuxBv0UNJ5wMltQOcBL68Ieug84AyWQgBeJpAAvGJjEYCXaSIAL98+cEboM02aNNEUhZkJwAJwhR1zAVgALq/RCMACcLr2IQCvCBxW+bZo0aLCdjgXb1AEHFCrArAALAAHdBQNQa8gkgAsAJfXcwTgALsiAAvAAnBARxGABeAMzURD0BqCDrMkkasEYAFYAA7rNpoD1hxwpohPQ9DLFFIEHGBXBGABWAAO6CiKgBUBKwIO6yhLrhKAA+QSgAVgATigowjAArAAHNZRBOBwnQRgAVgADusvGoLWELSGoMP6ClcpAg7QSgAWgAXggI6iCFgRsCLgsI6iCDhcJwFYABaAw/qLImBFwIqAw/qKIuBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1ldyGsBAc/Lkybbuuuta8+bNl1Nk5syZVlhYaM2aNQtSSgAWgAXgoK5iArAALACH9ZWcBvCbb75piUTCdtlllxXU+Prrr61hw4a29tprByklAAvAAnBQVxGAk2RasGCBlZaWWpMmTSwvLy9MxBy+SucBL1+5dXov6LKyMhsxYoS9++671q9fP9tyyy3txRdftHHjxlnjxo3txBNPdP/+888/berUqdanTx/baKONbMKECXb77bdbhw4d7Mgjj7TWrVvbE088YZ988ontuuuuLvKlQ2y88cY2evRo++CDD2zHHXe0PfbYI2XTF4AFYAE4jAqKgBUBKwIO6yt1PgJ+8sknbd68ebbXXnvZjTfe6AD77LPP2sCBA61BgwbWqlUrGzBggJ111lmGpwlMjz76aCP63Xzzze3TTz91EOYZDDsD33bt2rnrmjZtap07dzbeccQRR9ioUaNshx12sO7du6+gngAsAAvAYUZFABaABeCwvlLnAXzllVfaq6++6sBIlHr99dfbK6+8Yp9//rn985//tC222MLB8+mnn7ZJkybZM888Y/Xq1XMR8yqrrOLmgPfcc08bO3asHX/88Uvh+sADD1ijRo1s9uzZDuibbrqp+zuA79mzpwBcTvthOG3+/PluCL9+/frhLS2Hr5w2bZpzBgsKCnK4lGFFE4AFYAE4rK/UeQDfcMMNLtIdNGiQOzeRYeeSkhIX0Q4ePNiuvfZa93/AO3HiRHvsscesa9eu9ssvv1ivXr2sY8eODhTnnnuui36ZD87Pz7cHH3zQPYuFWD/++KOddNJJVlxc7IDCz5KTImBFwIqAw4yKACwAC8BhfaXOA/j777+3O+64w+bOneuGi/v27WuPPvqog+WUKVPs6quvtv79+9t6661nRUVF1qlTJxsyZIg9/PDDbpiZ1c+HHXaYdenSxS666CIH15133tktFCFi2X777d31wHiNNdZww9n8XwBO34AUAa+ojSLgZZoIwAKwAJwjAPbFIPr10Skrm5nvBZoMhR5zzDH2+OOPL42Q/T0YAhIRsE9EzsmrEVnoxbXpol/uVQSsCFgRcJhREYAFYAE4rK/U+Qg4UzEA8bBhw9zccE0mAVgAFoDDepgALAALwGF9JesBTAEYEq3pxS8CsAAsAIcZFQFYABaAw/pKTgA4vKiVv1IAFoAF4LD+IwALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQpz/+mGTt2rW1+vXrB96Ru5eVlpba/L8XWsOGDax+vcLcLWgFSjZt2jRr1aqVFRQUVOCu3LxUABaABeDwvv33339bo0aNLC8vL/ympCvzEolEotJ3Z8GNk/6YaG1bN3HAyemCBtQFAKbROADXb2A5XvUZFckrqGd/TZtnrVu3sYKC/IzX5/oFArAALACH93IBOECrWZPft4J5IyzfFphZ5T2VgFfV+UsAbklxsRUUFlp+ftyBk7C8vAKb3+hQa7NaN+lhZgKwACwAh5txAThAqwVTR9mCCf+yRPE0s7y4Q8fMjZYk3H9KZQst0flha71WfwFYAF6hPyxYsMAYNWrSpEmVhhlzpaMBnOLiYmvRokWuFKlK5RCAA+T7e+qLtvDHU8yKpwvAAXrF6pKyBVbW6W5r3elgy89fPAc8d+5cmzlzpq255pqxkoLCKgJWBKwIOLzbC8ABWgnAASLF9ZIkAH/55Zf2+uuvu4UVRUVFdsIJJ8RKGQFYABaAw7u8AByglQAcIFJcL0kCMCui+cPQ48MPP2xDhgyxVVddNTbqCMACsAAc3t0F4ACtBOAAkeJ6SYohaKT49ddfbfjw4XbLLbfEam5YABaABeBwYygAB2glAAeIFNdLUgB49uzZdtlll9nBBx9sW265ZayUEYAFYAE4vMsLwAFaCcABIsX1kiQA06EuuugiB9/u3bvHThUBWAAWgMO7vQAcoJUAHCBSXC+JADgvL99Fvs8//7xtuOGG1rJlSzvssMNiFQULwAKwABxuDAXgAK0E4ACR4npJUgRcVla23O5gbFZSlW3msk1WAVgAFoDDe60AHKDV31NfsIU/nGSmjTiWqOV3A9NWHAaA17p/ue+AA5pUzl4iAAvAAnB49xaAA7SaN/VVS/x+qeWVzTIz7YRFlEdUF6fILm0zSSyyhateY6079ozVaud0egjAArAAHACVJZcIwAFa/TJ1ki1oXM/ydNqNAd9FCxe6k6HYDzreKWEFBQ2t8ZwFtlqb1gKwdsJaoTtoK8rlJdFWlCvqodOQMlDkg7l/262z5tjssoTiX3ccxeIh6IR2g7ZiMzujQYH1WKWt5cX+cAptRZlsSgRgATjTiIAAnAHAH82ZZ/fMnmdzEgJwvCPeFUtfZGb/alBou7RrowhYEbAi4AwGQhGwIuAKM0QArrBksbkBAB/foNB2XgLgWbNm2XvvvefKv/7661vnzp1jowUF1Ryw5oAzRXw6DWmZQpoDDjCPAnCASDG9JBnAP/zwg7377rvuIIbp06fbqaeeag0aNIiNOgKwACwAh3d3AThAKwE4QKSYXpIM4Pnz57uzX3///Xe78sor7YILLrDWrVvHRh0BWAAWgMO7uwAcoJUAHCBSTC9JBjAysFKcKPjll19221LGKQnAArAAHN7jBeAArQTgAJFiekkygBOJhH322Wc2atQoO+6442J1FKHmgFfsBFoFvbwmWoS1oh5ZuQqauTYWuBSk+TZ3ypQpNn78eLcn7yqrrLJcqSdMmGBdu3YN3khCAI4pXQOKnQzgjz/+2O6++2476qijXBujc/EnLkkRsCJgRcDhvb1ORcAsWvn2229thx12yFiC//3vf7bzzjtb48aNU177xhtvuJ/vsssuK/z+mWeesT59+gjAGVXWBZkUWA7AeXk2YuRIe+utt1zk27BhQ+vZs6dbDR2XJAALwAJweG+vNQCPGDHCNt54Y1t77bXtqaeecpDl0PInnnjC1lhjDRs0aJDddNNNBljPOussd4LMfffdZ3/++af7HSfLfP311/bSSy85o/bzzz/bgQceaO+8847NmDHDxo0bZ9tss43179/fvvnmG3vggQestLTUBg8e7NSYOHGiGxbkdJq3337bTjzxRJs0aZJdd911bpXqIYccYptttllK5RQBhzeouF2ZHAEvWrTISkpKXNtjq04gXK9evdjIIgALwAJweHevNQBfccUV7nzU3Xff3Y4++mg755xz3AKVa6+91saMGWPTpk2zbt262ejRo+3cc8+1e++911q0aGHt27e3L7/80jbYYAO75ZZbHJw333xzB9ChQ4faHXfcYV26dHHPfeyxx2yvvfaydddd1/jWDOizZSJDgEB/2LBh7neHHnqo3XnnnXbmmWfa6aefbojw4IMPumcD+uTkADxnns3VRhyLpdEZDEubCAAe3KDAdmzXVhtx6DvgFWyH5oCXl0RzwCvqUStzwCxMef/99x3g5s2b5+bHLrzwQttqq63cN5NExttvv7298sorbvHKJZdcYlOnTrV27dq5P8D7q6++siOPPNLatm3rIluAef/997tImCj62WefdfPCRB1Eyt9995316NHDzQHPmTPHHZLerFkzF+3edddd7lncQ5RNJI4DQB6S0/g/p9k3eYVWwtFy4c5NTl6ZSJRZaUmxNWxQP+38e04WPEWh8EPq5eXZhgvm25ptBWAkUgSsCFgRcLgFrLUImCxdfPHFDsI33HCDi0yHDx/uQFtYWOjmcj/99FMbOXKki0qffPJJW3311V1kyxAew8p81kH03KZNGwdpHykD1NVWW81FvBgAhgEZ4gbAeKB4GEAeUDdt2tQOOuggN7x90kknuQh88uTJ9txzz7nhaxyB5DT289/tvtcm27yFnAIULm6uXZlImNUvNNt7i9Z2eM8u/79GC3KtiJUqD6M3rVq1ir1DIgCv2HwUASsCzuSQ1EoETCaefvppt00fQ8dEsddff72bB27evLn17t3bGbGzzz7brSBl8wIgCZxZSLXWWmu5zzt69erlomg2ODj++OONBVV77723i5JfffVV97vffvvNPvroIwfubbfd1g1lA2VgDuhPOeUUu+aaa+zDDz907+BdROQDBw5MqdVz7060Y68fZ9NnF5nlx5jAqFOasL47r2ZPns1IQcy1WNJaBOBl3UYRsCLgTMDRVpTLFKrVCDhdxfDtpD9blr+zkQGfF9XGubPR96XL34h3J9rAGz4TgJcA+JCdVrPHz9puKYBnzpxp6Ijzkx/DE4EEYAE4ne1QBKwIOJNDUmsRcKXG9+rATQJwpBJKExYFMJ+OMQ/PKEO/fv3cEH/ckgAsAAvAYb1ei7BWdEgE4AxtRwBOD2A+/2KFeadOnaxv376x2vfYqyIAC8ACsAAcpoAAXGGdBOD0AOY3fFfNd9n77LOPWyAXtyQAC8ACcFivVwQsAIe1lMhVAnD5AB47dqz98ssvtu+++wrAFW5duXWDFmEtX5+aA14ROFqEtUyTOrEIq66bIAG4fACz7ScR8AEHHCAA1/XGXMP5E4AF4PKamCJgRcAVNkECcPkAZoMUNk3Zeuut3UYncUsagtYQtIagw3q9ACwAh7UUDUGn1ilpFTQX+f2PWc2nz5Aq3Lxy6gZFwIqAFQGHd2kNQQdo9ey7E23QdeNs+qxF2oijNGEH7rKaPX1OD23EsaTtKAJWBKwIOMCQmrl99zUHrDngsNay5KrXP/vdbn95is1dWBbrjbDYirJegdl+3VrawL3ZslNbUdJEBGABWAAOM6kCsIagw1pK5KppP4+3wsnfWn6iJOZRX8LK8gqtbJW1rVnnja1eQX6FtczFGwRgAVgADuvZArAAHNZSIlcV//C+Fb5xi+UtnGOWF2foJNxRhMVdd7LEnqdZ/QormZs3CMACsAAc1rcFYAE4rKVEAfz9e1b4+k2Wt2B2zAFsZmVlVrzOjpbY70wBWHPAK/QlLcJaXhJ9B7wicDQHrDngCkG4WABeplcSgDmE4Y8//rDS0lJ3fCQnUMUtKQJWBKwIOKzXKwJWBBzWUhQBp9YpCcAcJ3neeee54yI5x5lDGeKWBGABWAAO6/UCsAAc1lIE4CAAE/2yFzSRcM+ePbUTVoVbV27doCFoDUGX16IFYAG4whZPQ9ARyVLMAWsv6GnWqlUrd4Z13JMALAALwOFWQBtxBGglAAvA5TUTDUFrCFpD0AGGVBtxrCCSABzQbgTg8gE8ZswYdxhDr169rG3btgGK5tYlArAALACH9WkNQWsIOqylaA44aA6Yi1iINWvWLFt33XWN/aDjlgRgAVgADuv1ArAAHNZSBOA0AC614rV3sMT+w/Qd8BKFBGABWAAOM6sCsAAc1lIiV5VOeMfyX77a8hbMivlGHAlL5BVY8Ub7Wt5ep1r8vvhN3XQEYAFYAA4zqwKwABzWUiJX/fnrD9asaIYVxnkXyiV6lJYlbEG95tagfWerX1joPj+KcyosLLTp06db69atY3kUY3LdaxX08opoJ6wVgaOdsJZpokVYAfT4+ptv7Y2xb9nCRYssLy8v4I7cvQTglpUUW76VWV6s98VeXMfsALbHHnvYJptsIgCbmQAsAJdn/RQBKwKuMB2/+OILe/zxx23+/PmxB3CFxcvxG/DmDz30UNtuu+0EYAF4hdauCFgRcCaHhIWrVQns8hI5Pg4JgJ966ikBOMdhWpniAeB+/frZtttuKwALwAJwhk6kCFgRcIXtrABcYclic0MygH/66Se76aabrKyszHbaaSc78MADY6MFBdUQtIagM0V8mgPWHHCFjKIAXCG5YnVxMoDZG7tJkyY2b948u/76623o0KGx2pxEABaABeBwE6hFWAFaCcABIsX0knRD0L/88ouLhC+++OJYbU4iAAvAAnC4MRSAA7QSgANEiuklqQA8d+5ce+aZZ9zhDAMGDIiVMgKwACwAh3d5AThAKwE4QKSYXpIM4NmzZ9vTTz/thqBPPvlkNxecnx+fD8gFYAFYAA43hgJwgFYCcIBIMb0kGcCjRo2yhx56yAYPHmwlJSW20UYbWfv27WOjjgAsAAvA4d1dAA7QSgAOECmmlyQD+NNPP7XffvvN+P6zYcOG1r17d1tzzTVjo44ALAALwOHdXQAO0AoAP/roo25YsSofTAe8SpdkmQJFRUV2xBFH6DvgJfUmAAvAAnC4EROAA7Qa/8ME+/L7b624tMTyLN5bUTKnWTx/geUXJSy/ID5zm+maCQutunXrZl27do3VXG86PQRgAVgADoDKkksE4ACtpr7/rc156hOzv4vM4rwXdMIsUZhnhdt1tra9u1s9K4j9YQz169d3ZyHrMIbFHUkAFoAF4ACoCMDhIs0YOc4mDbrPSv+caxbnqI+Tj/LzrPnRPazTHUeb4t/FbUjHES7rSwKwACwAh7NFEXCAVtNHfWaTT3rYSqfNcwCKbSICLi2zZgd1s7UeOM4KYivE8gUXgAXgdF1BhzEsr4z2gl5RDx3GkAEkAvASgQBwWZk169vN1rpvGYDHjh1rLEbaYYcd3MrfuCUBWAAWgMN6vQAsAIe1lMhVAnB6AAPfBx54wH1uw7F8LVu2rLC+2X6DACwAC8BhvVgAFoDDWooAvKJOKSJgVkWPHj3a/vrrL9t///3dYqS4JQFYABaAw3q9ACwAh7UUATgIwFxEFMzhA/vuu6+1adOmwvpm+w0CsAAsAIf1YgFYAA5rKQJwMIDffPNN+/XXXwXgAi1L0yro5buNFmGtCBydB7xME62CDsCx5oCXiJRmEdbbb7/ttl/ca6+9NAQd0J5y+RIBWAAur30rAlYEot3blgAABrNJREFUXGH7JwCXD+DJkycbR/Cx57FWQVe4eeXUDQKwACwAh3dpRcABWs14fpz98e8H9R2w/w744O7W+aHj9R3wkrajOWDNAWsOOMCQmpkiYEXAYS0lctXMV7+2qec+a2Uz5sd+Iw6zhDXpvbl1uLyfALykjcyYMcN9fhWnc3/TdaJFixa57ShbtGhR4X6WizegRWlpqTVu3FgHuZi5U8KYA27evHkuVneFy+RPTavKIT95iQR7FOZuKpoy2xZ+MdESRaUW67MYqOV6+VZ/3VWtYedVYi1FtLWzCUm9evVkYM2Mz9IADnoomdOCxKEdSov1oI2ofSxuDZwZXlhYWKWmkfMArpI6ulkKSAEpIAWkQA0pIADXkLB6rBSQAlJACkiB8hQQgNU+pIAUkAJSQAqsBAVyHsA//vijrbrqqta0adOVIG/deyXzOPzhLNy4pzlz5rhtODt16lTluZxs15KlIKwIZ+FRx44ds7041ZZ/5vlYeMSpN3FOtIvp06e7OeBWrVrJni45P5tdBOkvTZo0qVTzyGkA33zzze7QeTaaOOGEE5yhjXOaPXu2XX/99W5RyTnnnBNnKeybb75x23DiiOCknXfeedagQYNYagJkPvzwQ/vggw+cgWUV9BFHHCEnzcxOP/1022mnnaxXr16xXajHQkX2jH/rrbesc+fO1qNHD9tss81i2Vd8oekrb7zxhts/Yccdd7QOHTpUSo+cBfAPP/xgTz31lDtkAAD/9NNPdtxxx8V6BR/R3i233OJW71188cWVajC5chPRLw4JIyMnnXSSXX311da+fftcKV6FyoGTOmvWLDcyQj8ZM2aMHXTQQda1a9cKPSfXLr7vvvuco7b++uvb0UcfHVsA0zZGjhzp9ooHNqz85dOsOKfTTjvNBg4caF26dHGOamVXQ+csgF966SU3vOg916FDh9pVV10V+6Ektp7Ekx02bFic+8/SsgOfAQMG2G233WbNmjWLrSZssvDqq6+6P1tssYUDTpzTl19+6UZImL5i+PXwww+PNYDvvfde+/zzz2299daz3r172wYbbBDb5vH7778bPFlnnXVs/vz5NnjwYAfiyqScBTBDJsxpAWA2WTjjjDNclBP3uRyGGl955RU7++yzK9Necu6eIUOGWJ8+fWy77baLrYGlUol+p06dahzOMWHCBDcEzXBjHBNDrueff76D7s8//2xTpkxxDkllo5xs1xAnFQeN/7/22mtulOSoo45yc8FxTF999ZUbSTzzzDNd8a+44gr378qknAUwQ9CjRo2yfv36GR4LhuXkk0+O/bwWAH755ZdjPweMMTnrrLNs9913d3N8GNeq7GhTmc5Xl+5BD8qP0/rkk086j37PPfesS1mstbxMmjTJ7rzzTmOagukrdjxi9CzOUZ9vH++99559/PHH1rdvX1tttdVqrU7q0osYkr/00kud/WD4edCgQfbII49UKos5C2DUuPHGG91ZtxMnTrThw4fb2muvXSmRcummTz75xM3xEfnFOeGxjhgxws37Al8ivp133jmWkhDdAN1x48YZ21EC3xNPPDG2o0XAhj+MnDFaxFRW//79Y7td6cyZMx1gGBmhrbCu5oADDohlX/GFvv322238+PFuZfgxxxxju+yyS6X0yGkAowirOrXPb6Xahm6KmQJ+V9o4jwTErMorXFwfCVf4xhy8oTq0yHkA52C9q0hSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KfD/ACv5gltg2onZAAAAAElFTkSuQmCC"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9477375" y="5200650"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142873</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>158628</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>69333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9596436" y="4921128"/>
+          <a:ext cx="3690939" cy="2768205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>29283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1322916</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>170536</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4180417" y="8876950"/>
+          <a:ext cx="3492500" cy="2755336"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>47623</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>5132</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>122910</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7834312" y="8429623"/>
+          <a:ext cx="3402383" cy="2551787"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -2078,518 +3066,896 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="F1:Y1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="12.63"/>
-    <col customWidth="1" min="7" max="7" width="14.88"/>
-    <col customWidth="1" min="8" max="8" width="21.13"/>
-    <col customWidth="1" min="9" max="9" width="18.13"/>
-    <col customWidth="1" min="11" max="11" width="26.75"/>
-    <col customWidth="1" min="14" max="14" width="15.88"/>
+    <col min="1" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="26.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1"/>
-    <row r="2" ht="15.75" customHeight="1"/>
-    <row r="3" ht="15.75" customHeight="1"/>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="1" spans="7:25" ht="15.75" customHeight="1"/>
+    <row r="2" spans="7:25" ht="15.75" customHeight="1"/>
+    <row r="3" spans="7:25" ht="15.75" customHeight="1"/>
+    <row r="4" spans="7:25" ht="15.75" customHeight="1"/>
+    <row r="5" spans="7:25" ht="15.75" customHeight="1"/>
+    <row r="6" spans="7:25" ht="15.75" customHeight="1"/>
+    <row r="7" spans="7:25" ht="15.75" customHeight="1"/>
+    <row r="8" spans="7:25" ht="15.75" customHeight="1"/>
+    <row r="9" spans="7:25" ht="15.75" customHeight="1"/>
+    <row r="10" spans="7:25" ht="15.75" customHeight="1"/>
+    <row r="11" spans="7:25" ht="15.75" customHeight="1">
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="2"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="K12" s="4"/>
-      <c r="S12" s="5" t="s">
+    <row r="12" spans="7:25" ht="15.75" customHeight="1">
+      <c r="K12" s="22"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="S12" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="U12" s="6" t="s">
+      <c r="T12" s="23"/>
+      <c r="U12" s="4" t="s">
         <v>1</v>
       </c>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="8" t="s">
+    <row r="13" spans="7:25" ht="15.75" customHeight="1">
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="O13" s="8" t="s">
+      <c r="O13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="S13" s="9" t="s">
+      <c r="S13" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="U13" s="10">
-        <v>17.0</v>
+      <c r="T13" s="23"/>
+      <c r="U13" s="7">
+        <v>17</v>
       </c>
       <c r="V13" s="2"/>
-      <c r="W13" s="11" t="s">
+      <c r="W13" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="Y13" s="6" t="s">
+      <c r="X13" s="23"/>
+      <c r="Y13" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="K14" s="8" t="s">
+    <row r="14" spans="7:25" ht="15.75" customHeight="1">
+      <c r="K14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="12">
-        <v>12.0</v>
-      </c>
-      <c r="O14" s="12" t="s">
+      <c r="M14" s="5"/>
+      <c r="N14" s="8">
+        <v>12</v>
+      </c>
+      <c r="O14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="S14" s="9" t="s">
+      <c r="S14" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="U14" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="W14" s="13" t="s">
+      <c r="T14" s="23"/>
+      <c r="U14" s="7">
+        <v>13</v>
+      </c>
+      <c r="W14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="Y14" s="14">
-        <v>3.0</v>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="9">
+        <v>3</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="G15" s="15" t="s">
+    <row r="15" spans="7:25" ht="15.75" customHeight="1">
+      <c r="G15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L15" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="M15" s="7"/>
-      <c r="N15" s="12">
-        <v>10.0</v>
-      </c>
-      <c r="O15" s="12" t="s">
+      <c r="L15" s="8">
+        <v>2</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="8">
+        <v>10</v>
+      </c>
+      <c r="O15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="W15" s="13" t="s">
+      <c r="W15" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="Y15" s="14">
-        <v>25.0</v>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="9">
+        <v>25</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="G16" s="16" t="s">
+    <row r="16" spans="7:25" ht="15.75" customHeight="1">
+      <c r="G16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="K16" s="12" t="s">
+      <c r="I16" s="11">
+        <v>5</v>
+      </c>
+      <c r="K16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="M16" s="7"/>
-      <c r="N16" s="12">
-        <v>10.0</v>
-      </c>
-      <c r="O16" s="12" t="s">
+      <c r="L16" s="8">
+        <v>2</v>
+      </c>
+      <c r="M16" s="5"/>
+      <c r="N16" s="8">
+        <v>10</v>
+      </c>
+      <c r="O16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="W16" s="17" t="s">
+      <c r="W16" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="Y16" s="14">
-        <v>2.0</v>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="9">
+        <v>2</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="G17" s="16" t="s">
+    <row r="17" spans="6:23" ht="15.75" customHeight="1">
+      <c r="G17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="16">
-        <v>7.0</v>
-      </c>
-      <c r="K17" s="12" t="s">
+      <c r="I17" s="11">
+        <v>7</v>
+      </c>
+      <c r="K17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L17" s="12">
-        <v>4.0</v>
-      </c>
-      <c r="M17" s="7"/>
-      <c r="N17" s="12">
-        <v>4.0</v>
-      </c>
-      <c r="O17" s="12" t="s">
+      <c r="L17" s="8">
+        <v>4</v>
+      </c>
+      <c r="M17" s="5"/>
+      <c r="N17" s="8">
+        <v>4</v>
+      </c>
+      <c r="O17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="18"/>
+      <c r="W17" s="12"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="G18" s="16" t="s">
+    <row r="18" spans="6:23" ht="15.75" customHeight="1">
+      <c r="G18" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="K18" s="12" t="s">
+      <c r="I18" s="11">
+        <v>5</v>
+      </c>
+      <c r="K18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L18" s="12">
-        <v>4.0</v>
-      </c>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
+      <c r="L18" s="8">
+        <v>4</v>
+      </c>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="2"/>
-      <c r="W18" s="18"/>
+      <c r="W18" s="12"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="G19" s="16" t="s">
+    <row r="19" spans="6:23" ht="15.75" customHeight="1">
+      <c r="G19" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="16">
-        <v>7.0</v>
-      </c>
-      <c r="K19" s="12" t="s">
+      <c r="I19" s="11">
+        <v>7</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="12">
-        <v>6.0</v>
-      </c>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
+      <c r="L19" s="8">
+        <v>6</v>
+      </c>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="2"/>
-      <c r="W19" s="18"/>
+      <c r="W19" s="12"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="G20" s="16" t="s">
+    <row r="20" spans="6:23" ht="15.75" customHeight="1">
+      <c r="G20" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="16">
-        <v>9.0</v>
-      </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
+      <c r="I20" s="11">
+        <v>9</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="G21" s="16" t="s">
+    <row r="21" spans="6:23" ht="15.75" customHeight="1">
+      <c r="G21" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I21" s="16">
-        <v>4.0</v>
-      </c>
-      <c r="K21" s="19" t="s">
+      <c r="I21" s="11">
+        <v>4</v>
+      </c>
+      <c r="K21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L21" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="T21" s="20"/>
-      <c r="U21" s="21" t="s">
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="V21" s="21" t="s">
+      <c r="V21" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="W21" s="21" t="s">
+      <c r="W21" s="15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="22" t="s">
+    <row r="22" spans="6:23" ht="15.75" customHeight="1">
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="V22" s="22" t="s">
+      <c r="V22" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="W22" s="23">
-        <v>13.0</v>
+      <c r="W22" s="17">
+        <v>13</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="T23" s="20"/>
-      <c r="U23" s="22" t="s">
+    <row r="23" spans="6:23" ht="15.75" customHeight="1">
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="V23" s="22" t="s">
+      <c r="V23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="W23" s="23">
-        <v>4.0</v>
+      <c r="W23" s="17">
+        <v>4</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="22" t="s">
+    <row r="24" spans="6:23" ht="15.75" customHeight="1">
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="V24" s="22" t="s">
+      <c r="V24" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="W24" s="23">
-        <v>5.0</v>
+      <c r="W24" s="17">
+        <v>5</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="25"/>
-      <c r="U25" s="26" t="s">
+    <row r="25" spans="6:23" ht="15.75" customHeight="1">
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="V25" s="22" t="s">
+      <c r="V25" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="W25" s="23">
-        <v>8.0</v>
+      <c r="W25" s="17">
+        <v>8</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="N26" s="7"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="25"/>
-      <c r="U26" s="25"/>
-      <c r="V26" s="20"/>
-      <c r="W26" s="27"/>
+    <row r="26" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F26" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="N26" s="5"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="14"/>
+      <c r="W26" s="21"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="T27" s="25"/>
-      <c r="U27" s="25"/>
-      <c r="V27" s="20"/>
-      <c r="W27" s="27"/>
+    <row r="27" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F27" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="14"/>
+      <c r="W27" s="21"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="25"/>
-      <c r="U28" s="25"/>
-      <c r="V28" s="20"/>
-      <c r="W28" s="27"/>
+    <row r="28" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F28" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="34">
+        <v>45933.426388888889</v>
+      </c>
+      <c r="J28" s="32"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="14"/>
+      <c r="W28" s="21"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="25"/>
-      <c r="U29" s="25"/>
-      <c r="V29" s="20"/>
-      <c r="W29" s="27"/>
+    <row r="29" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F29" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="J29" s="33"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="14"/>
+      <c r="W29" s="21"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="25"/>
-      <c r="U30" s="25"/>
-      <c r="V30" s="20"/>
-      <c r="W30" s="27"/>
+    <row r="30" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F30" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="34">
+        <v>45933.390972222223</v>
+      </c>
+      <c r="J30" s="32"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="14"/>
+      <c r="W30" s="21"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="25"/>
-      <c r="U31" s="25"/>
-      <c r="V31" s="20"/>
-      <c r="W31" s="27"/>
+    <row r="31" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F31" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="35">
+        <v>45872.520833333336</v>
+      </c>
+      <c r="J31" s="33"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="14"/>
+      <c r="W31" s="21"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="R32" s="24"/>
-      <c r="S32" s="25"/>
-      <c r="T32" s="25"/>
-      <c r="U32" s="25"/>
-      <c r="V32" s="20"/>
-      <c r="W32" s="27"/>
+    <row r="32" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F32" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="J32" s="32"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="14"/>
+      <c r="W32" s="21"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="R33" s="24"/>
-      <c r="S33" s="25"/>
-      <c r="T33" s="25"/>
-      <c r="U33" s="25"/>
-      <c r="V33" s="20"/>
-      <c r="W33" s="27"/>
+    <row r="33" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F33" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="35">
+        <v>45660.458333333336</v>
+      </c>
+      <c r="J33" s="33"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="14"/>
+      <c r="W33" s="21"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="R34" s="24"/>
-      <c r="S34" s="25"/>
-      <c r="T34" s="25"/>
-      <c r="U34" s="25"/>
-      <c r="V34" s="27"/>
+    <row r="34" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F34" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H34" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="34">
+        <v>45933.611111111109</v>
+      </c>
+      <c r="J34" s="32"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="21"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="R35" s="24"/>
-      <c r="S35" s="25"/>
-      <c r="T35" s="25"/>
-      <c r="U35" s="25"/>
-      <c r="V35" s="27"/>
+    <row r="35" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F35" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="35">
+        <v>45903.368055555555</v>
+      </c>
+      <c r="J35" s="33"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="21"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="R36" s="24"/>
-      <c r="S36" s="25"/>
-      <c r="T36" s="25"/>
-      <c r="U36" s="25"/>
-      <c r="V36" s="27"/>
+    <row r="36" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F36" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="34">
+        <v>45932.65625</v>
+      </c>
+      <c r="J36" s="32"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="21"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="R37" s="24"/>
-      <c r="S37" s="25"/>
-      <c r="T37" s="25"/>
-      <c r="U37" s="25"/>
-      <c r="V37" s="27"/>
+    <row r="37" spans="6:23" ht="15.75" customHeight="1">
+      <c r="R37" s="18"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="21"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="S38" s="20"/>
-      <c r="T38" s="20"/>
-      <c r="U38" s="20"/>
-      <c r="V38" s="27"/>
+    <row r="38" spans="6:23" ht="15.75" customHeight="1">
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="21"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="S39" s="20"/>
-      <c r="T39" s="20"/>
-      <c r="U39" s="20"/>
-      <c r="V39" s="27"/>
+    <row r="39" spans="6:23" ht="15.75" customHeight="1">
+      <c r="S39" s="14"/>
+      <c r="T39" s="14"/>
+      <c r="U39" s="14"/>
+      <c r="V39" s="21"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="S40" s="20"/>
-      <c r="T40" s="20"/>
-      <c r="U40" s="20"/>
-      <c r="V40" s="27"/>
+    <row r="40" spans="6:23" ht="15.75" customHeight="1">
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="21"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="S41" s="20"/>
-      <c r="T41" s="20"/>
-      <c r="U41" s="20"/>
-      <c r="V41" s="27"/>
+    <row r="41" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F41" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="14"/>
+      <c r="U41" s="14"/>
+      <c r="V41" s="21"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="S42" s="20"/>
-      <c r="T42" s="20"/>
-      <c r="U42" s="20"/>
-      <c r="V42" s="27"/>
+    <row r="42" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F42" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G42" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="H42" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I42" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="J42" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="K42" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="21"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="S43" s="20"/>
-      <c r="T43" s="20"/>
-      <c r="U43" s="20"/>
-      <c r="V43" s="27"/>
+    <row r="43" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F43" s="32">
+        <v>10</v>
+      </c>
+      <c r="G43" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="H43" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="I43" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="J43" s="32">
+        <v>7</v>
+      </c>
+      <c r="K43" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="21"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="S44" s="20"/>
-      <c r="T44" s="20"/>
-      <c r="U44" s="20"/>
-      <c r="V44" s="27"/>
+    <row r="44" spans="6:23" ht="15.75" customHeight="1">
+      <c r="F44" s="33">
+        <v>23</v>
+      </c>
+      <c r="G44" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H44" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="J44" s="33">
+        <v>3</v>
+      </c>
+      <c r="K44" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="21"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="45" spans="6:23" ht="15.75" customHeight="1"/>
+    <row r="46" spans="6:23" ht="15.75" customHeight="1"/>
+    <row r="47" spans="6:23" ht="15.75" customHeight="1"/>
+    <row r="48" spans="6:23" ht="15.75" customHeight="1"/>
+    <row r="49" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="50" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="51" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="52" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="53" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="54" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="55" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="56" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="57" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="58" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="59" spans="6:11" ht="15.75" customHeight="1">
+      <c r="F59" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G59" s="30"/>
+      <c r="H59" s="30"/>
+      <c r="I59" s="30"/>
+      <c r="J59" s="30"/>
+      <c r="K59" s="30"/>
+    </row>
+    <row r="60" spans="6:11" ht="15.75" customHeight="1">
+      <c r="F60" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G60" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="H60" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I60" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="J60" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="K60" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11" ht="15.75" customHeight="1">
+      <c r="F61" s="32">
+        <v>23</v>
+      </c>
+      <c r="G61" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H61" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="I61" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="J61" s="32">
+        <v>3</v>
+      </c>
+      <c r="K61" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11" ht="15.75" customHeight="1">
+      <c r="F62" s="33">
+        <v>1</v>
+      </c>
+      <c r="G62" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H62" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="I62" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="J62" s="33">
+        <v>3</v>
+      </c>
+      <c r="K62" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="6:11" ht="15.75" customHeight="1">
+      <c r="F63" s="32">
+        <v>22</v>
+      </c>
+      <c r="G63" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="H63" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="I63" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="J63" s="32">
+        <v>7</v>
+      </c>
+      <c r="K63" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="6:11" ht="15.75" customHeight="1">
+      <c r="F64" s="33">
+        <v>10</v>
+      </c>
+      <c r="G64" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="H64" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="I64" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="J64" s="33">
+        <v>7</v>
+      </c>
+      <c r="K64" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="6:11" ht="15.75" customHeight="1">
+      <c r="F65" s="32">
+        <v>6</v>
+      </c>
+      <c r="G65" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="H65" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="I65" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="J65" s="32">
+        <v>3</v>
+      </c>
+      <c r="K65" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="6:11" ht="15.75" customHeight="1">
+      <c r="F66" s="33">
+        <v>9</v>
+      </c>
+      <c r="G66" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="H66" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="I66" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="J66" s="33">
+        <v>5</v>
+      </c>
+      <c r="K66" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="6:11" ht="15.75" customHeight="1">
+      <c r="F67" s="32">
+        <v>13</v>
+      </c>
+      <c r="G67" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="H67" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="I67" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="J67" s="32">
+        <v>3</v>
+      </c>
+      <c r="K67" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="69" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="70" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="71" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="72" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="73" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="74" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="75" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="76" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="77" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="78" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="79" spans="6:11" ht="15.75" customHeight="1"/>
+    <row r="80" spans="6:11" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -3510,17 +4876,23 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="F41:J41"/>
+    <mergeCell ref="F59:K59"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="W16:X16"/>
+    <mergeCell ref="F26:J26"/>
     <mergeCell ref="K12:N12"/>
     <mergeCell ref="S12:T12"/>
     <mergeCell ref="S13:T13"/>
     <mergeCell ref="W13:X13"/>
     <mergeCell ref="S14:T14"/>
     <mergeCell ref="W14:X14"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="W16:X16"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:bug:fix:Corrigindo tabelas de faixa etária , gênero e animais
</commit_message>
<xml_diff>
--- a/GRÁFICOS.xlsx
+++ b/GRÁFICOS.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="93">
   <si>
     <t>Espécie</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>maria.oliveira@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Dr. Ricardo Alves</t>
@@ -312,6 +315,10 @@
     </font>
     <font/>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -327,10 +334,6 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="12">
@@ -401,8 +404,21 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border/>
+    <border>
+      <left/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <bottom/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -410,8 +426,15 @@
       <bottom/>
     </border>
     <border>
+      <top/>
+    </border>
+    <border>
+      <right/>
+      <bottom/>
+    </border>
+    <border>
       <left/>
-      <top/>
+      <right/>
       <bottom/>
     </border>
     <border>
@@ -420,36 +443,48 @@
       <bottom/>
     </border>
     <border>
+      <right/>
       <top/>
-      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+    </border>
+    <border>
+      <right/>
+    </border>
+    <border>
+      <left/>
+      <right/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -458,49 +493,65 @@
     <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="6" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="5" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="4" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="6" numFmtId="22" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="9" fontId="7" numFmtId="22" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="22" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="22" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="10" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="10" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="10" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -574,11 +625,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2033683896"/>
-        <c:axId val="1690654519"/>
+        <c:axId val="1348629204"/>
+        <c:axId val="442649725"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2033683896"/>
+        <c:axId val="1348629204"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,10 +681,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1690654519"/>
+        <c:crossAx val="442649725"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1690654519"/>
+        <c:axId val="442649725"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -708,7 +759,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2033683896"/>
+        <c:crossAx val="1348629204"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -935,11 +986,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1282295360"/>
-        <c:axId val="1135564427"/>
+        <c:axId val="1167882422"/>
+        <c:axId val="144969631"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1282295360"/>
+        <c:axId val="1167882422"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -991,10 +1042,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1135564427"/>
+        <c:crossAx val="144969631"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1135564427"/>
+        <c:axId val="144969631"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1120,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1282295360"/>
+        <c:crossAx val="1167882422"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -1209,11 +1260,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1401009771"/>
-        <c:axId val="1903193136"/>
+        <c:axId val="1583976512"/>
+        <c:axId val="569022532"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1401009771"/>
+        <c:axId val="1583976512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,10 +1316,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1903193136"/>
+        <c:crossAx val="569022532"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1903193136"/>
+        <c:axId val="569022532"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1343,27 +1394,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1401009771"/>
+        <c:crossAx val="1583976512"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0" i="0">
-              <a:solidFill>
-                <a:srgbClr val="3C78D8"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
 </c:chartSpace>
@@ -1388,573 +1421,6 @@
             </a:pPr>
             <a:r>
               <a:rPr b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t>Faixa etária dos animais</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Página1'!$X$13</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4285F4"/>
-            </a:solidFill>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="F1C232"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Página1'!$W$14:$W$16</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Página1'!$X$14:$X$16</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Página1'!$Y$13</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Página1'!$W$14:$W$16</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Página1'!$Y$14:$Y$16</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="862999861"/>
-        <c:axId val="1461298903"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="862999861"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:spPr/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1461298903"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1461298903"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="862999861"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0" i="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="B7B7B7"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="B7B7B7"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t>Quantidade - Gênero</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Gênero</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="F1C232"/>
-            </a:solidFill>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="F1C232"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="1155CC"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="1155CC"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Página1'!$U$22:$U$25</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Página1'!$V$22:$V$25</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Página1'!$W$21</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Página1'!$U$22:$U$25</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Página1'!$W$22:$W$25</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="408525779"/>
-        <c:axId val="1931540588"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="408525779"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:spPr/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1931540588"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1931540588"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="408525779"/>
-        <c:crosses val="max"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -2067,7 +1533,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr lvl="0">
-            <a:defRPr b="0">
+            <a:defRPr b="0" i="0">
               <a:solidFill>
                 <a:srgbClr val="1A1A1A"/>
               </a:solidFill>
@@ -2082,7 +1548,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -2092,7 +1558,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -2100,7 +1566,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -2147,11 +1613,580 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1295572514"/>
-        <c:axId val="879517025"/>
+        <c:axId val="535300859"/>
+        <c:axId val="2055535"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1295572514"/>
+        <c:axId val="535300859"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Raça</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2055535"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2055535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Total de raças</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="535300859"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="434343"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="434343"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Quantidade de animais - Gênero</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$V$21</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="1C8AEE"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="3C78D8"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF00FF"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF00FF"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$U$22:$U$25</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$V$22:$V$25</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$W$21</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$U$22:$U$25</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$W$22:$W$25</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="374061098"/>
+        <c:axId val="201532628"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="374061098"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="201532628"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="201532628"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="374061098"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="434343"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="434343"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Faixa Etária</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$X$13</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F1C232"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$W$14:$W$16</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$X$14:$X$16</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página1'!$Y$13</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página1'!$W$14:$W$16</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página1'!$Y$14:$Y$16</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="625840032"/>
+        <c:axId val="1347045405"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="625840032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2178,7 +2213,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>Raça</a:t>
+                  <a:t/>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2194,7 +2229,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2203,10 +2238,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="879517025"/>
+        <c:crossAx val="1347045405"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="879517025"/>
+        <c:axId val="1347045405"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2253,7 +2288,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>Total de raças</a:t>
+                  <a:t/>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2272,7 +2307,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2281,27 +2316,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1295572514"/>
+        <c:crossAx val="625840032"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
 </c:chartSpace>
@@ -2361,10 +2378,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3533775" cy="2171700"/>
     <xdr:graphicFrame>
@@ -2387,9 +2404,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
+      <xdr:colOff>866775</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2933700" cy="1876425"/>
     <xdr:graphicFrame>
@@ -2411,15 +2428,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3476625" cy="2171700"/>
+    <xdr:ext cx="8458200" cy="2276475"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
+        <xdr:cNvPr id="5" name="Chart 5" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2436,15 +2453,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3962400" cy="2447925"/>
+    <xdr:ext cx="8458200" cy="2495550"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
+        <xdr:cNvPr id="6" name="Chart 6" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2461,15 +2478,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8458200" cy="2276475"/>
+    <xdr:ext cx="4914900" cy="3028950"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 7" title="Gráfico"/>
+        <xdr:cNvPr id="7" name="Chart 7" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2486,15 +2503,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8458200" cy="2495550"/>
+    <xdr:ext cx="3400425" cy="2105025"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 8" title="Gráfico"/>
+        <xdr:cNvPr id="8" name="Chart 8" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2516,7 +2533,7 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:ext cx="333375" cy="333375"/>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAeAAAAFoCAYAAACPNyggAAAAAXNSR0IArs4c6QAAIABJREFUeF7tnQW8lcX6tp8ddJeiggiKnWBjH7EVUBRUjoV45NiePwp2Y+uxu7tB9GChYie2iC1KKB0Cu9b3XQMDL4u19pqd7LXee37yE/Z+Y+aemed6npl5Z/ISiUTClKSAFJACUkAKSIFaVSBPAK5VvfUyKSAFpIAUkAJOAQFYDUEKSAEpIAWkwEpQQABeCaLrlVJACkgBKSAFBGC1ASkgBaSAFJACK0EBAXgliK5XSgEpIAWkgBQQgNUGpIAUkAJSQAqsBAUE4JUgul4pBaSAFJACUkAAVhuQAlJACkgBKbASFBCAV4LoeqUUkAJSQApIAQFYbUAKSAEpIAWkwEpQQABeCaLrlVJACkgBKSAFBGC1ASkgBaSAFJACK0EBAXgliK5XSgEpIAWkgBQQgNUGpIAUkAJSQAqsBAUE4JUgul4pBaSAFJACUkAAjkEbKCsrs/z8/KwvqT+6Oi8vL+vLogLUPQVWZvsqLi42+qlPpaWl1qhRI6uutp4rNqDutZqq5UgArpp+dfruefPm2RdffGGTJk2yddZZxzbccEOrX79+nc5zusz9+eef9tlnn9mCBQtso402ss6dO1tBQUFWlkWZrlsKAN4//vjDPv/8c+Pvm222ma2xxhq16rQ+8cQTrn3TpktKSqxDhw523HHHWb169aok1rRp0+zTTz+1v//+2/Wbtddeu1bLVaXMx+BmAbgGK3n+/Pk2fvx4w5sl0bkbNGhgG2ywgft/TacrrrjChg0b5t7bqlUru+WWW6x///41/dpqf/706dPtjDPOsHvuucc9e4sttnB/33zzzav9XXpg/BT47bffbPDgwfbiiy+6wu+66652//33W8eOHWtFjBEjRtgpp5xiv/76q3sf8L3xxhvtgAMOqBIsFy1aZEcddZQ99thj7rnYnYcfftj1H6W6oYAAXIP18OCDD7qODYh9ateunfHzPffcswbfvPjR22+/vb333nvu7wxBH3HEEXbvvffW+Hur+wVffvmlHXLIIc6Z8empp56ygw46qLpfpefVsAKMZDAcykhM69ata/htYY9/5ZVX7JhjjrHff/996Q2ffPKJdevWLewBVbjq66+/tkGDBi3tp9tuu63ddNNN1r179yo8dfGtjICtssoqbtSI1KJFC7vsssvs3//+d5WfrQdUjwICcPXomPIpvXv3tpEjR7oI1CeGmI499li77bbbavDNix9N9HvttddaUVGR64iXXnqpe3e2pcmTJ9v//d//2SOPPOKyzlAajsRWW22VbUWJdX7nzJljp5566tLh0HPPPbdO6PHdd9/ZySefbC+//LLLz3bbbefa2lprrVWj+fvpp58cDF966SVr3Lixi3gZtVpzzTWr5b0LFy60vn372gsvvOCex9A6cN9hhx2q5fl6SNUVEICrrmHKJ+BN9+jRwxjeItHBmIchbbLJJvbWW285j7QmE0O3DzzwgBF1rLfeenbooYfWytB3TZTpm2++saefftp58z179rQdd9zRCgsLa+JVemYNKQDUjj76aOcQMjrzzjvv1NCbKv7Y999/3/73v/+56LxXr14u+q3phYtvvPGG3XnnnW6KCuj/85//rNZRARz/CRMm2OOPP75U83322afi4uiOGlNAAK4haa+//nrDw2cYiI7MUPTNN9/s3sYw9H//+18HxIomvFrgTqclqmVutybS1KlTbebMmQ7Yq666qnMgkhO/B+6AkHmr0HltHBHu4/9ow1Bk27Ztq8XgYXT++usvmz17tjOmzZo1c8+uzsVn5H3GjBlOE8odaqgBD3mbO3euy0/79u1T6hpan7QDpjfQjzaVKlVlZW9597Jql4VLtMemTZtamzZt3Krd8tIee+xhDPeSmGcdM2ZMaFGdbrQ3VgXjuNL2K5PoN7/88otrG6uttprLe1US86z0FRzD5s2bu3oIdQxnzZrlNKRdUCbqkWeEtqdovikXzyIflIvnVCbRntCaeqV900ars+9UJk+5fI8AXEO1yxyvH9LCWDAXy6IhjC8Jb5foNFVizvOOO+5wEMGo3Xrrre4+vOUPPvjAdRAMCJ1s4403tiOPPNItsEhOd999t4u0MaQNGzZ0Q1z77rvv0svI30MPPWQYUyJKFmzgMROpMDfFkCGrMMn/LrvsYocffrgD2vfff2/33XefWzVKHjE4XENUw3xWKlgDLPLy7rvvGkNvGFOMhTeoDLvtvvvuxrB98upmInnex2pOD2yG7ojqfaKMrCR9/fXXnYOC44NRIi8YRa5l6G3rrbe2Jk2alFvr3Pfaa6+5YW7yR70df/zxNmXKFLc4Z9y4ca4+0LRLly522GGH2c4775z2mRhGFtoQZfEMyo1mOAaMhvTp08f9PzlRz7yP+UjKffbZZ7uV7OhAvX311VcGAPbee28bOnRo2vezoAfdcZBYYUs977bbbisYevJ211132bfffuvqgOtPOukk23TTTZc+m7IQUX388ccOPMADHah/pgQOPPDAFYZQWYlLW8ch9aNAGHaiMbTmGUScJ5xwwgoQpx5GjRplP/zwg2tr1AdtEN0pN3+SE6uJ/cgP+broooscaKmDZ5991n7++Wf3b95HHhilon0xFI3OAOz000938CHR15gCoRzcR3+jTfA8Fm5NnDjRlYG21qlTJzv44INdf0m1gpm2TORLW8ARoEy+H9CfGfbea6+93BqR5PuZirnmmmvcVw30F9/v33zzTddn0Qh9zzrrLNtvv/1cXTPnS3+jDGjBPdH69NrxtQTTZdge2h02gfpHi2222cb1S5xNpepVQACuXj3d0wAThoiGT2IBER28X79+9vzzz7ufsRLxmWeeSTnPxJwNRpIOjyHkOgwKP8czjSYMBlAhuk5eNDJgwAC36pEEyJkTjs67XXnllXbmmWe63wNwjAzvGTt27HLz1vweI8s8GcNzgACY+tXdPj8YICDNPFPUa8YQkA9WegL16Jx4tCx8+kGehw8fvtz3jxhMwI4xJhFtAVsg4g3kaaed5sAAFFIlDDdRF3PizIWVlzCmlOE///mPuwwnh6FTykz9JZcbuDN3hzbJCVifd955zjGILsaLXrfllls60LFILpp+/PFHB/5XX33V/fjRRx91oxHojyPmv+0cOHCgc9jSJer9qquuWppv2iYGO3nEgvLhBFF+30ajq82B+IUXXugA4q+JvpM2hsaUF6NNAmrnn3++a8MY9XSJ9z755JPWsmVLdwkak2fKBaiS2wz1CRBoF7ThaHsDsuiJs0ACkPyM5/F3Es4PbQFHGAeHT35wbEisfsY5XX/99ZfmBd2BJ5rhcNF/ATt9NDlx/3XXXbeCM4mzhJ7UB+BNl7if/FCuKISZhqHN08ZxBHDIiZzpVzjFPrHIk36IraBtcR8JvfgSYv/991/u1fQb8osO9NXkRJmpH75E2GmnndLmW7+ouAICcMU1y3gHRgqD7FcfYuyAMHBjtSUJQwNoMLDJiUUZGAY8UQwNXjVGqLyEIbr88suXm0NiwRUdHuNF1Ad8PXB5FsPkgItER2cIDCOTqhNyDZ2daBJPO10ivzgKyZEJ82ssCPERkB+uw5gQrfpEZ0cvIOETn2eg0+jRo92P8MqBkY86+TsGyz+HPABpyoSGvjx8goWjkmn1LaDAULFgiITzgXPB81OBh2vWXXdd57hgqH3CKJ544olLR0LKqz+cD6BPpOETjgdTF7QHEqMXtAMMqgcSkTQRD20uXcIJwCAT2ZJoC9Shj/D4GWW+4YYbnBPm0znnnOMgg56ACwfSr6rnGqY/unbt6iKy6Api8smziFKZtyfSTOcY+XclA5j7AXkUVDhClJcI1ydAdMEFFyx1lvg5ThLv9LClzz333HNu2sCn1Vdf3RghItrkebSfjz76yP2ab+Zpw9QpCWeA7855no/AAX4q+Prncz0OS1RjfkfEHB2FStcPcGaI/L2Tyb04M0TG/nMlfodDy2hENDHMj57YH0a2ACuJqJnFn9G+SZ/CWSmvT/tnM4LEaIo+/yuvJ1fsdwJwxfTKeDVRCZ3ERy0YbwwpHZH/06k9EPCkfYQafXAUwP7ndEg6CgYDzxbjgXHzCa8ZIxONgisC4KjhwEPH+6fjMrSJ5x5NOASAhUVmXAP4fbTBdf/6178cwKJzWYAdL5tRAUCIcfZDohha8u51wUBhfHzKBGCiZiCM9hho8ga4+DcGCmjgADDnzhBcppQMYH89w4oMfeMAEAUSUfF8ErAHBMDQG23KO2TIkKWvwwByP0O1GG8cIIYiPUz59ITn+nnJZADzDmBAuXCEWA3OtThrOHjlJYZF+XTLJ4a2oxE39UeU7+docSRw3vyiHUY/MN4+iiXav+SSS9xwMHOZRKrUuU8YauqB+XI+HwM8QNU7pQyDMpzK8ygT7yOqpP4YBmUEyEekOD88n090aFNMj1C/HvpEeZSH4XlSMoCBJY4T8GQjCoZ5qUPqhqH/igDYl4980s9xDHGmiSIZ5Yo6k/RPpheiu1mhB8PCtBucTEBNP6CP0XbIu28P1AdTAr4fJQPYT9WgH30SZ4hyEhljZzIBmLzSduh7PmE/iKiJlqk3RgkYifEJx4a6ra4dujL1xVz/vQBczTWMAWVI0A8/00lp4IAYbx5D6I0cniRGLvnD+GQA09mJxjB4ftiQIUhAx3C3T0D/H//4x9J/VwbAvJtVxnQwOjDDTkRmPhEFE23RSX0ibxhfb5yJTFlgEwUwRsXPy/KMaAcmckQXjBMJUHkvn39nAjCGDI15R6rPvMgXBg8nJtX8dHITSAVg6grD4z/h8POCRNQ+KgYqvj6IKICIX+kLPIEIPyP53ZeiK+Ux5EAKo0hKBrDPJ/rjdABfNKZMmcoFHIhucYRIOHJEeb6OPvzwQ7cS12+HiKaUDceRCJcFVICPRATN3zH6PjEfTZ58+XF2cDD8YimmDOgXHlDlLcJi9Ihhdj/Uz3wsbd8v8sJRAzL+e1aiSJwhothUAOZnDDmzloIyAmTKzX3US2UATBtnWN2PpuAU04ajjiMOGeWILspCX6YiqH+cl2g/oA3jWDAXTwKGROXpAMw1jELwHuoLG8PzyRPvzARg5nxxkqLD8kzz+DlinsX8Mm0l2sZpx36KoZrNZ+weJwBXc5UTPTK36g0Z8MJLBgwYdoyAhxcdhmFoP9Tps5IMYIwr0UB00RGGFMMUXciFQY1+ZlBRAAMXoiQ/jIqRwChEh4OZb2aOyQ/PkWeGjCkDw72pDEcqiTEOLMTC82dolGFCP0wJoImqfMoE4Oj3ztyDrkST5ImFZxVdxZkKwAzxA+DovCnGEQeLcpCISikLw99vv/22c2T8nD1zZ7fffvvSeUVfNqYAWBGP1hha4Ass0wGYMjGn6udKQ5svzh/DkUSXXiMiG4ZiqQNgGV3IdfXVVy8d1mWxkV+Exr20Ab/AkH9j7HGeGLL232pjoIneGDYmsRsTGoYAGCeFiNYnIkmGVH1kCDQBfhQCTK0wEpMOwLRrotFUK4wrCmAcEMqavPAN2OI8eMeBusIWlLedJP2AoXGcCpw1nCQWW5EYCicK9ZFucgTMNdiPdAvwMgEYpya6JgR7QTuILlJkpIZI3DsW9C36QTbuJxDaV2rzOgG4GtUGGgwF+giXR2OQgZWPzujs0YiX4VgMbtSwJwMYw+6jQ59dDBlGJzrsV1UAE0EQSUQ/YSCSjUbVAB7PP5pfOif3esNBtOhX7vr84vVTLgw04MKBQBP/Bwh4A1tRABMpEpF4T96/E8PHcKNf4BT63XUqADM8yEYm0UQdMKTp64ZohBEQIojkuT6GexnOA87RRN0TGXqHDSeIxVDpAMzvKruRQnQYmcgL55AoEseH6M2/l2FZnAWiRRJROYbaD7cDBAxxciJK8qMgTGHgHPrNUkIBjMHHGfOLFb2zkLwynrbi1xNwDeXwn/klD0Ezvw7I0n1yVFEAMyqAPjh30QR8GZ3ww+zojSMTBTBthvwxZI1T7UckeI5fEe77AW0L6KYDMEPOODnpFkZlAjD9Ijq6BXzRMZpf+i3rAHAkfLr44oudA6JUdQUE4KpruPQJdCyGdPzmG/wi2fulc0UXOTFvxdwa0YlPyQAm8o1uw8h1dAwA7I0OP6sqgBluZj426gGzeje6EIRFQqwojSbeS3STDsDoQQTFPKxPRCIYFh+RYLwrC2CeCdQx3HxGlWqhFNESxob5wkwpFYAZ5iPyjCbyy1yij9yJStGCz7EYcmXRkk+UHyPGsGM0oSWL0zyAyZ9fDJQ8BA30mHpI9RlJpjLxe6Jy3uXzi+FmiJFFWtG1A0Sg0S1LcTyYt4wCL9X7/HAqutBmATDRMikUwDhR1KNfQ8G9PDfVyvno+9CX0SVSMoDJA45Ruu+UKwpg1lvwGVgy+KhfAOx1SgYwC+hYg8CUiy9TtB9QRtpeKIApF8PB6Vb1ZwIwUSxrSXxiOgxHMersMIKDExGNlIn0iZ6Vqq6AAFx1DZc+AYARQVY0sRiF4WSfkgFMRMJ3etFUEwAmyqNzRecTkwHMMB4RcDSVB2DyCbzoxD4xH0f0QNQKwBi6jg5hVzQC9s/1i9MwSgyvJn/2w3AxRpqFL+WlVABOZXQwcETY0QiYoVkgytA9WvkEVKjn5KFjFo8xd+oBHN0hKhnAOEasrK0sgMkLc848g8TzgC9DvAzjk4jiqSu/Wp+fMbSLwfV6Mkdf3l7FOJhcw1QLURopFMAsrGJEIDrEzVA+jku6z9eoBxxD1kSkAjCRPHOb1QVg5r4ZyaGuoqk8AKMdQPYHinAfkTSfBAFypgKIdok2/RxwpgiYRWlE4unaQyYA47Rwv0+MpuFIR+escSYY5o4ClzzWlW1EK2pr69r1AnA11Ugqzz3deZ4Y2+j3vERKRLJ+eDKXAIwurB72i9IYBmRIk3klnzA8DHP7ldSVBbB/HgDFSWBulU80/LAoc8HMLWY6ESoVgDHuzH1FRzSYXmA42H/egmMB0FhBSsTFQiOfWMiCgUuGP8YMB8XDhQMm/GrlmgAw2jNniHEmoiayxYHy31gDaOAS3Y+YaJi5SV9OHBmG2CuyY1MygBlV8e+MdkEMPhE43wT7RNTvI+mQ7pocAdcFADPqgDPiN+KJfofsy4RjxJcRfgFiTQOYYeTotEryYjfyxbQao3r+aw0id9oQP1OqugICcNU1dE/AYLBE3y9EwtACVoAT9dwxWsz7EPn4IVs8aoaC/FxrLgEY8PK5jHc4GOokQo1GUBhn5p78YqaKApgFRkRIyUCgLog6/HFs1BMQZKVpeSkVgFMN9zHnBzx92TCwDIGT+FaXb2/9N6sYXOZ7o9+AAhtABGBIRKQ8z3+LWxMAJrpCe1Y240yQH4ZEPVzRC8clmpI3lqFNs2o61e5r3AfcqYvoOoHkVdDl7QXN1Ep0zpG5SrROFcESbfvduHz910UA44hGnZpUixnpFzhHvh/UNIDpF4w8+SkJpsP4Ljh6DCOr3VkBT3shYdeYMuNnSlVXQACuuobuCcnDz3iTRDeptj3E2PENYnQ4CoPjvxnNJQDjzTMk6zctYEEMiziI9DCcGCbgy/ewPlUUwAz7A2DmwliwxiIyol0cHRY+RReqEc35T4HSVX2674CJ2llsxrtwLACDj1aYN8MB8/ACQpST4TufiBwxeBhiFp3htDHc6yN0hrNZwMfqV1JNAJjnEmWxCIhEffjFa7wfCDDkm5wY4mU1tE84DpSNoVO0pgxEdwwhM+rAqAdDpD4R7VLnfmMNPk8iquL9DM8yKsS8MXWPBjhJ/vtTHAUWCLESmt/j0KIv0RkODo4MdeOnTuoigHF8mG7xCa3Rj0WNtAXaE1FldFONmgYwecJJjO7Jje6sxKcPYacYoo7uVcAXESz8qqk96KvJHGfNYwTgaqgqFkgxREkk4RNGgP1Y0yWioegwLHOiLBLC+8wlAANByhld1comHCw6w5Cy2AbvGuOJUeVnFQUwURxDotzHfDnGjeex6CW6bSK/4/vRTN8wJgOYYTf+AAkiWYwPC8uiG5QAFAwZ0b5PwAHYR7/VxrABHUCEAfRzv0SLzDNH59ZqCsDkE82StzUlqkHH5BXHlIfhURYQRXdMwtkhksUhYXUvevvdtliAFd0chNEI9I/uiMUQOKulmXpg2B7nyC8oIgoGutEFdQCdCAzNaFeMNlAPDO8zbO+d3boIYJwFdqCKOpqUBUeF9kY/oD3gbBDV0w9qGsDUK58UsuWqH7njZ7RxPkUkP9FV2tQR0zDR3dqqwXzG+hECcDVUP8aGhSN+dTMGlg7l95JN9QqGHfF+/dAfxoNhOn7GamFWI/qokc+YmCeNJgweUbdf+cnvkldBYzD9d8IAyS+y8s8h+oru1ITRYxV0dBFW8mdIqVZB80E/DohfPAKEgA6GHEPC7wFR9NveaFnYtAF4Mj8LhDHo/pMXrsOwE3n6z7sw/ERwfo4Vw+a3qUxXncyvs0LVf5NdXrWn2oqST6uAB1BMTkCV0Y7o5iT+GvKMxlEIJ99P3bP4hWHW6DfLREXk15cb48wK6Ux7WWdq0gCMOoqurE/3bWv0WWhOHnEs0i2I4nrqEphGF6Hxc3Rgd7DkvbT5HZ/m4ZT6BUUsbGPxFxF5uj20fd6SP40jUmc0wq8pYMidT6zSLcLicyDal9+ykSkhnGD/3T35pU9754ERDKLC5M/BmE9lsZJ3bMgDIzDUKc9gxIPFbf4zpeR68t9Js4CPa3DGaW/eIcK5YRTADweHrILGafELOHkeo0HJgQGjNtSrnxJL1X4oP7bBb3aSqY3p92EKCMBhOqW9CkPEMA3RK3NjREU0cIagyxumAVY0eiI0oh+MDBEQC4SYX6OxA2fmtfCEk7espIPyTjxYgOlPS4quzMQg+K3tMD44CX6XJQrEHBAGguiOfANRotXoN54YJz5XwIhgWBhGJd/RxAYCDKdhoMgvhgtj6ufkGCLEuSCvOBKUlfxgEIAom1HwbAwQkAbA0QU6aIUx5pMZVmjinTO867+nphx8zsPey3jyvA/IoAuRKXNbOA5EfZl2jKJcqYagKTObSrBYzp8URX3zM76hxcFItz0fwKL+2BKTIWucJ3/KFCAkgmNYOPlwBAwtUxO0EfQHkkTwfoi6Kk2XcvApjf8sDuigsV+1nO7ZOI4Agv/703yAC22GHZiI6ljIxdBmdKcsnsfcJk4fK5wZ9qbNcR8OFU4UkVj0mEHaNDDFIWVO3R/7R7tCe4Z0cXLZFpP69frzuRW6oR/X+oPo0x2XSSRN2aknrmcEhX7h52xpSzgTvN/DmPaXfIIV7Zu1HLQ/dMWxZE7dryrm5ziZODK0Vf5NP0AnRh+4ljzjCNOO+Tn9xvcj2g5OHo4F+WA9BXPG6dqD79NoRxmIYHm2/747Wsc47/Qh+jsgpj+SN6YY6GdMH9BOlapXAQG4inoS9dJpPCz9OaMYlfJWidKBAAsdjev8+b4YFTomQ2s+osZIRXeeIsu8h44SvR9QRzfRwMj5BR28A+MWNXBE2N6b5nl8FsHvo/kGFszF+SFYnIpkw0q06s815bpU+aV85AdjR/m4Bq8ag++Bj6EAfnj8fgclysowJM/3x9EBL4xjdGMFdMBAUQ8YD8qDAWE4DShkOoAh2gxSAdh/esEcJ2UADsCceiEvmfbG9fN8aED5/XGEGE/ymCpFy02d8IfrU22CUdFmTJ35Az6ABWXJBN/oO9AgeuwjcOMTK9oGbThd2+ddgI62S/m4j77CtES6OqJOGQ2gjtHRb79JWwWWyWffJrdH2gF9I12ecGYpi/9+lzz5PZopM3lmtMB/o8vvqfNkZ46oHUj7zWUoF1pE2wZ9Gt0ZyqcsPAtHlPxRr9yLk+p/Fx1F823ID8vjkAHVdO2BPkDf9VM7OHFcn/wtuq9X2jSOAWXw78cm0ObS3VPRdqfrl1dAAFaLkAJJCoRuxCHhpIAUkAJVUUAArop6ujcnFUgFYOaPmRZQkgJSQApUlwICcHUpqefkjAICcM5UpQoiBeq0AgJwna4eZW5lKCAArwzV9U4pED8FBOD41blKnEEBAMwqYVZn+8RBDOxSpSQFpIAUqC4FBODqUlLPyRkFWD3Kimw2VmHFNatO+XQjemJQzhRWBZECUmClKSAArzTp9eK6rkDyZhOZPjWq6+VR/qSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADHpKJVTCkgBaSAFKhbCgjAdas+lBspIAWkgBSIiQICcEwqWsWUAlJACkiBuqWAAFy36kO5kQJSQApIgZgoIADXZkWXlppNmmRWVpb+rYmEWfPmZi1bmuXn12bulnvXxIUzbEFZUdr3JyxhjQrqW/v6Lax+XuFKy2eVX5wosdJFv5slSsp5VMLyClpafv22ZpZX5VfqAYsVSJjZ/LIym1NaVr6qeWZZGbNyAAAgAElEQVSrFBZaQUyFKytL2O/TF9iCovQ6YTaaNCyw1Vo3tIL87GijZWVllpeX5/7ENQnAtVnzM2aY7bGH2Zw5Zuka3aJFZgMGmA0data0aW3mbrl3df/kIvt01oT07y8rtu6t1rd7NhhkmzbpUOl8Tps2zRYuXGjt27e3wsLaB3nZwp9s1sc7WqLoL7O81A5PonSRNer4b2vS9Vqz/AaurBiP3377zeU9Pz/fOnbsaI0aNaqwDolEwj2H8jdosPjZ8+fPt5kzZ9pqq61mBQXpscO9v/76q6211lrlvpc8/vHHH7ZgwQJr0aKFrbHGGs7offbZZ7bZZpvZn3/+aa1bt7b69euX+5ySkhJ3LXmlzFVNRYmEjZg9zx6cOccalGOES83s1g6r2qqFy7SYM2eOTcKZNXNlIk+ZDDl6kf9VV101ZdanTJlif//9t9Mc7cvTo7i42Lh+9uzZ1qpVK/cHfalD8tWpU6el9VlVnWbOK7JdzhhrX3w93awgDaxKymy77u3tmfO2s/atFrcjyuvziDZt27a1Nm3aVDo7c+fOde29Xbt2FX4G9y1atMiaN2/u6on2PXHiRFt77bWtSZMmNm7cONtkk03s999/z9ieK/zyOnyDAFyblQOA99nHDMimMzhFRWZ9+pidcYZZs2bL5Q6jTydv2LCh+zmGoqioyDXoevXq2YQJE9zvMEbeeGDMaeAVTVt9col9PPeXcgBcYlu06GL3rne0bda04wrX8d7GjRu7vJFv8unzzcV0SP49atQoA8L77befMxA+YTzosJQjauyj5QUIXAe4/TsqCsHSBRNszrh9LVEy3czSAXieNVzjOGuyzuVm+Y1dFjEgZ5xxhjPmGF2gdsghh1jTJU5TaWmpkT9+F81zslBc179/fxswYID16tXL/RpNnn32WbviiiucJuhAXUcdFJ7NvXfffbf9+9//dvcBBXTwIOdn/HvkyJH20UcfubrgOX379rUNNtjA+vTpY08//bT973//s+233345w+qjE/LOe7kP6L344ot20EEHufaG9tQjmkfLG9rWAPDI2fPsidlzywUw1/13jVWt/RIAU/bRo0fbk08+aeuss45rIzvvvLNtu+22S1/t8x1tO/Sdc889166++mp3Hc/hD+2Q8o4YMcI+/fRTW2WVVeywww5bCqtUfejLL7+0hx9+2Gm6+eab2zbbbGO//PKL63v33XefnXDCCc4p8wl90DBVHWXSa+a8Ytt16Fv2+Y8zzdJFtyVltu1Gbe3Zc7e19q0W2wfaDeWlfLybtvqPf/zDunbt6n4fbZdc6+s5XX7Q+9tvv7Xzzjuv3H6aqoyff/65odmBBx7o7MLrr79uf/31l+21114Oyr1797YHH3zQHnroIRs8eHDa9pxJq2z7vQBcmzUGgPfdF/qUD+ADDzQbMmQ5AONpv/32287QzZs3z3r27OmM3xdffOEAhQG46aabXGc74IADnCF48803nWFp1qyZ7b777hUq6dafXGIfZQBwtxZd7J4kAGOkX3vtNZenTTfd1Bmxd9991+Wjc+fOzvB//PHH9v3339v666/vvGDKsOGGGzqDvtNOO7lo7K233rIZM2Y447711ls7w8V9GInVV1/dRYmTJ092zwM4X3/9tdOGckcNcaZCVwzAV5jlL45yefeNN95oZ555ptP3sssuc+8GpC+88IJzeigv/8f4YKi7d+++QvSFLtQXxhGYYpQuvfRSB4azzz7b6fjVV1/ZrFmzHCQBH9ECkRoRAzruueeeLrL75JNPXN7WXXddF1mQ3nnnHQero446yv2MvNBOrrvuOjvmmGPs0UcfdfrjOBBN004ACdEObennn3927Y284wxw/1ZbbeWgTV6IhoDge++95+qYd3sDn0n7ygIYcOCk8H+cF9o5+cFw00++++47VxfkGWPvE23myCOPtKeeespdQ7kpA22PfNOG0JO02267ud/Rlml7PGePPfZY6lA+8cQTDkYXXnihu5730pbR8f7773f9kWcyOkGd8j7egyOUXEeZdAoF8HYbt7VnzlkGYNrIKaecYnfeeafrG9T1N9984342fvx416ZoQ/Qx8kd/o6/5EZJovigbjgWgBpZbbrml0x1H1EfXlJl/M7JC3ay33nqubZCwAR9++KFz3tCKUQscHdos7Yl6ueOOO9x16JyuPWfSKtt+LwDXZo1VEsAYNjxGGjyNlQ6OsaaR0qExRhh+/g4MiGwwSBgcIPj888/bv/71L9fZQlNlAXzbbbe5jkxnJAIALOSPDk9HpaORf4wTw58YeKKqffbZxxl3DNYuu+xiZ511lv3zn/90BgNDSDluuOEGO+KII1zHfeCBB9y1RCrABOPGzzGuXIdXHZIqC2CG9v773/86ALds2dJBirwBZSLh//znP84RwAhieKiDww8/3EX60UTdUk6MFWXBCbngggtcRLfvvvs6QwYonnnmGdt///3d0OY111zjfoezQvQL8Bn2HDNmjBsFQS8iH9L1119va665pos8fNp7773tscces+OOO861o2uvvda22GILZ/zOP/98V18YXIw2xpKE40PkjDG/5JJLnAN4/PHHu3oGwkCe6BGHi7oLSVUFMNrS7nFWgANtDeeE4fZjjz3WtZnoaAD9YdCgQXbrrbfaxRdf7GADHKm7//u//3PtD/2IwoiScfgYEgXkzz33nA0cONC6devmikadEBHS7nCMqDfqaIcddrCXX37ZNt54Y5eXoUOH2l133WUdOnRw173yyisr1FEmraoC4FNPPdW1ARwIHAb6GsPrOEw4r7QLRgZw8mg/OE+0i+TpIBy5sWPHunumT5/utEBLHJ1dd93VtSPaPu0VW0Ud0Ef8aAPvo33QXvg7TiOgp63Th8jnLbfc4voA7S9de86kVbb9XgCuzRqrJIDp3O+//75rmAAY8GLMMZh0FDzbfv362Q8//OCghuHHS2WIDO/2pZdesh9//NFOPPHE4NJWFsD+vUR+RA7Ah6iYyALvmPxh3E866SSXF/JGZwNaGDuMWo8ePeyDDz5wxgsjdu+99zrPmfIOGzbMfvrpJwda3gXIMSKAHwAzPMbPvaHMVOCqABjQMwwNgDHkJ598sl111VUu3xhxyuujduoIgPInmoAcxuz00093EGFIDkMJRBkuxJnhOegAfHE6MIToh8ZEgI888ogznkTLAAQdichJGEWM5MEHH5wSwPfcc49zJIjCiXyZjwaowI164h1oTP0BXRwf4E59YcyJiKgrjDgGFoeCyD0kVRXAvJN+wP/JF44GUSwQ8cP50XwAYOBy+eWXu3qjTugXAJPRAYZp0Z16HT58uIMDzh3tikgYQFNPPqEJjhUjBYAJ7YE1/ZT6AepXXnmlgwvRHRBLVUeZtKoKgE877TRXv+QRpwFnDX2Y9qFPUdevvvqqq0faGWXCgYo6LrQFnGYgzSgIbZZr0JFoFacDxxrHkPZOGXGK0JdhZZIH8HbbbeeuoW3jCKAz+hCVA2Cgjt1K154zaZVtvxeAa7PGKglgskiHwdjg2dPJ8S7xuI8++mjXiIlOADOeNtEkEKBzADM6Cp4nxj00VRbAdCQgw1AmBpwhOvJI58eAESVizIjciJaYn8SjxqBjDJn75O+ADDgQMWAgiRw9gHE0MHK8B8NJFER5u3Tp4vTB62aYOiRVFsAMQTNHi5HFsGNgiVqZD6TMRASAkvL5OiK/1AnX+wVWGDOGh2+++WZXjo022sgZMxwThuhxYHCoeBYRA7/nZ4xoENVQ70RYlJuoDmMKCHgeieHAxx9/3DkpOG9AE+NGHom8AReGk3cy7DxkyBDnwAB2ysc7aU9+/hgg8R7upa6IdHgW7yfyQRcirpBUFQATkQIMNGMeG3Aw6oDuwJA840zgoPpFYz4Cpgw4arQxoAIYARTlB0oMZXMNdcdQK44HfYy6pQ6pM5xKP2yPAwT8mRLC8eM+nDHaLiM4XEd9paujTFpVBcD0M5wA8sawOXAEgvTFQw891Dkc9Fn+Tl5xhmkD9F1GEEgMT+OUoDUOFm2TUSqgSpsHwNgmnD0cPbTjWdgn3ukBzHAzWjLXji3yYGfKhdEU2jF9obz2nEmrbPu9AFybNVZJANPomRPF4Pn5UDxXgEt0TGfBaBKt0LgBNCBmGJrf481iMCuyQKmyAMYQkgfggPHi3xg+PGyAC1wxnkCC35M3DBqOAsYbuPgomqFBFtjsuOOObmgLQGMguY7hdoACyIjAiL6IuJk/xlCEpsoCmKFZDDjREcabKBjI4UwQxTPaQL0wNAsE+DtTA34lKeWl7NQtEQoRE4abaA7jBBQAMIaS8gJAphB4H9pxDfcDSSIIwIPm6MyKXEZEfALKRIb+kw+GoJmfJv/cS30wjEg+iVhwZIiIqQt0pg2hNffg+Phhf0YjqCMASP1QNiL06HB3efVQWQDTXpiOAXDkiciVtsToCkafkQL6AL9HI4ADaKJzwDiBOIVoQp8issMxQUP0BZjcQ58jmuMdOI/AlPcTxdEn+Tn1xFwnbZ3oEt1wALgfp4BokXrDoUxXR+XpVFkAUyc4Q/R78kK7AJi0XUaRmMIgP4wwoQ39k7qmv1HPfnEfMAWe2BASutLmadNMXeDwAF0cDEZxeB+2iPbAiIMHMLpwDe2RKSmmDGg/OKhEvyxcA+I4BOW159C+nQ3XCcC1WUuVBDBGmQiPBorBwMAT+TEPyMIZ/3kBBpSOhdEhAsRwM4SJQWJuuCKpsgDmHXRMFngQFQBQwAmgyCcdl+iBa5inxSjgldNpMXSUlZ8DEgwh9zGXzM8BLL/z13GPn6tiLhmPmrnUinzOVFkAA06iP95JPigribxRPhwBEkPTOEqUHacJ48e9vtxcA7QxfhhMv3Ka52Ls0ZGohPvRgoQ21CdtgZERfoex822B66Irzv2nTrybdsG7/L38nXsxxMAEg8jv/GpuhrPJH5Gwn+tmAQ0/86vWuYfha8rEz6LDlzUBYJ7JO9HFLwDi3SS0BzbUCXnk9/yOFbg4GpSRIXI0pM3QPnEaaIPUJ/dTT9QfP2OkiTqkfik3CT2pF9owZcXZRW/qjH/TVtGPd6EfvyeVV0c1AWDySftAB/LFSAC6UHa/sIwyUhbKTtsgz2hCmel3fqU7bdZ/TUH5/FcKtBuezTvQGQ38anA0QQf+zSgcToofMWJ0guu5hj7NaAb/xl5las8VsWN1/VoBuDZraPr0xd8Bl/cZEr/r29ds2LClq6B9BEw0hPdNhMIQkDcINVGEzT++wD6fU/5nSJu1WNvu3WCgbdF0MXyyMZX+/Z3NGbeHJYozfYZ0vDXperVZwbJVtdlY3rqUZyLgZ2fPs8dnlf8d8KJEwm7p0H7pZ0iVKQNAAbg4rlX5FrYy767qPTPmFtmOQ8baNz+U/xnSVpu0tZEXbL/0M6Sqvre67geqDGNjt9J9g11d78q25wjAtVljCxaY3XOP2axZ6T9DKi4223HHxX/q1VuaOyCMEcHzxGOMfl5RE0W4edLr9tW839M+ujhRahs3WcMOW2VbW6V+xaLrmshvpZ9ZOt/+/u1qS5TMSbvLVSJRZPVb7W712x1Q6dfoxhUVYD+48YuK7N15C6ywnI048i1hfVs2t8ZZssNTddf1wqJSu+OlX+yrX2an3eWqpDRhW67T0gbstqY1aVj7G9pkKjN2K9NGKZmekYu/F4Brs1bZL46NNvh/eQnwlrMDUm1keVFZiZUmytkyk41A8vKtfn5h1m/OmChbuGRjxHTKJszy6lle3jKHqDbqIA7voIWVZOoPZlaPLQvjIEiKMmItiorLrLSsfLtRWJBn9QrzY6tTNjYPATgba015lgJSQApIgaxXQADO+ipUAaSAFJACUiAbFRCAs7HWlGcpIAWkgBTIegUE4KyvQhVACkgBKSAFslEBATgba015lgJSQApIgaxXQADO+ipUAaSAFJACUiAbFRCAs7HWlGcpIAWkgBTIegUE4KyvQhVACkgBKSAFslEBATgba62681xaYvbzB2bzppnl5ad+OptyNG1r1nkbs4K6t9NOdUtS3c9jr1v2xGYf3XQ7AvFz9utlu0Sl6lNg9shxVjx58bnGqVKitMzqrd7Smu60nhW2blJ9L9aTpEAGBQRgNRGzhXPNRl5o9sfXZgVpdnsqLTZbY2OzA843a9jUqcb2mJxswvGAbOLO/tScHZtpyzk2seckGbbW5OByTl8BTjyPk1XYIL4yiaP1OInHHySQ7hlsPk+eObiBQw04TYn8c4JOprxXJl/cw2lEnKzDpvW8K1Xi3ZzqEz3JiIMc0IqDNdj7m2MZ/cEDmfLCO99++20Hfc5fRet05eOgAE744WACThgKSexLzolCHPJA3ZPQlrOLK/Ic/y4OBOBEIY5c5ECE6krf/+NK+/vj9PuaJxYVW5Pt1rEONxxujTZZfHACiROX2MOYdkmeaKeZEoc3cNISOpA46Se6bSzP4ghE9OaEJA5/oN1VJHGwxBtvvOEOneBEow033DDj7bQ7TiPiWFJ/UEjGm3RBjSsgANe4xFnwggWzzEZeZPbHNxkAvJHZAeeZNVp8KgxHmHH2LqemYHA5J5TjBjkTlb1f+cNG7MnGlCPjOOmIY+I4MpEzVjltBzhw6gz3+ROAOC0FgHDKCpvoY8AANO8GAAAUAAA1Dh/n1BVOU+G0F06C4bjC5MRxiZwoxTm2RJscwccJShyD6I9s5D384XQiTt4Bfhg8EkaW9/rTYUJqGKMJgNGjPACjHcf9+YShff/9991RhOSFYwo54s5vao+h5/Sa5L3BgTYAwbijJ44NYCUSR2fKw/8pI//nyDnO88UB4PxhNEVfYO+h7Z0A/y5O1eG4Ow4Jeeihh1y9AHyOOeRMXY5M5IQn8ojRR2PK4E8Z8mc2kz/qGJjzZ7fddnMn50ydOtWdwORPV6IeAFboWc9ewwk7DrcF436zdHs0JhaVWONtuljHGw+3RpsvO1iEIwk5VhCHDn3Yg51zk9GFctEG/YlQ/l3AF4eOoxFpS5yVS7uhLL4fvPDCC6594yyiDU4rKbm8/AynhL7hE/o99dRT9u2339r222/vjgmk/9A+qDN+Hz1pi35DPvnz2GOPueM8GWWJno6Gk0d7CD3FKqS965owBQTgMJ1y+6oFsxcDeFIGAK/uAdzc6UGHv+2225yRwgBwQPejjz7qIAjcMJ4Yc86ajab777/fGTWMwWWXXebggHEDTJwvetFFFzmjxOkpAIHzZjFUGF7OssWQYJgwPBgPf+g5EHj++eeX5ssfA8e5ph6e5OPaa691ETcGkLxxaDiQIXIj70TmvJOoDihh+DGeRJFAzR/GDrDJd0gi6gkFMIej+/Tiiy+6/HDQOeC7+OKL3cHwlA0nAmNKVIxWPnH4uj97lgPOfSIPn332mTsiD9ATPXE0H04KwCNKQm/AijOFJpxvy7GXOCmAHgN/zDHHOD2B5q233uoOvt9zzz1d3aA/Z7uiOdEW2gJ5rica5Pxi6p6yUKecKcw5yICEZwO2M844w8aOHeuifv5wDi2OC2c+Aw7yBHxC04SdL88M4K27WMcbDlsOwBwyj4NB3XPMJ3nlYPrbb7/dOV9Advfdd18uG5yjiy5oRhkpO2fl+qMlca4YmcCJo93Ttig3jgugZQSA8gND7sMhpY3zbhL64EDyXEZKzj//fAd5nBv0wZkBptQ7/ZH2w8gHzheOr3ck+Xf//v1dPeMMAHQc2FQOa6jOuq7iCgjAFdcs9+6oJIABEQbYAxhhMDyPPPKI+xkHfROpJR+biAePocYoESWcfPLJLmogasWwYJiBMwYfwGGUXn75ZQe+Xr16uQgACHHNwIEDnbHBKPP3O++80wA8IGeIefTo0Q7c3EfC0BNFAiCM5emnn+6G80gYWYYZMUJE9hgongcQMVTcQyTLc3ke0U/ocHllAUz+gVDfvn0dfBgx4NxfgIsOHPaOxj5ypxwYVBwINMA4+4TxJlolL/wfR4f6evjhh532OBuAHeeGOsMBQYc+ffrYzTff7CALcBg6Bc5EVzhcRITcAygZ5uTYP+DE/xlqJR84NuSXuiJC5n7aDjDn/QAbCJA34Eq5GVlhFAPHjNEPnIdTTz3V1U+maYZoJ60sgCkPzhoABqpDhgyxI444wrUJnAmczuRztjmsnkPpyS/3UW/nnXeeG9WgbDgiOCY4QZQBfWjvlBHgA3hGhoA0cF5//fWdbhdccIH7O1pzWD0wpR3iqHIf+vbs2dPliTZNvhkpwcGineLA4KBSf7RZYE29Anr6F7A/88wzbauttso9+1aHSyQA1+HKqbWsVRLAyREwnjqdGCPCUB1GIlXC4DIk1qlTJ+elY3zfffdd590z50ZUCjiAAgaNuUnAgDEmaiNS5fcYG95DFACQjj32WPd3oiwicIY9Ge4DrECeBEh4HsaL6IB/E0FjALfeemu75JJL3NApkQRQw5kAGhgwAExUw8HuzGNzuHjo2bJVATDREs4Gxp78AkCMKkaUqCXZCcCgE7Gi7wEHLDtCkbIRMQMwok7gCgCJpImyiaxweKhXDDFODtBhpAEHh3uA5PDhw502HsDkBQCTGP6kHtGFuiXP6EaUDISor8cff9w5U9dcc42ra0YGbrzxRgeojz76yN1DHTM9wPP4Q174GU4TECHaDk3VAWDaK0Amz9TBpZdemnLIFgcJoO2xxx5uBIi/EzHjzBHpAmWexXAzTg4AZuSB9stIBtrQFllbQZmpK0Y0cIZwtOgTANkPx/MO2uc555zjtAXSxx9/vIMvbZ78kNCfkSOuYYSDoXL6ByNBTB/RF3BgGbGqqXUQofUVp+sE4DjVdrqyVhLAGFE85x49ejjDwnAy82ZAkqgRw05nx5v3Q4dkATgADTx3IjiMFfAm+sVwEx1j4DDqRJ4YJ343ZswYd48HMAtjMDbMO7MQBXASOREtY+SIwhmK5edEFUAGoDIvShTCMCdGH6hi5IkGBw0a5CIThtb5PQu7iD4AMnlmTpqo4cQTT3Q/x3iFpMoCmPLjlBDdsHAM5wUHgyiXuWEiQqIzHBUMuJ9fxtgyDwyggSX64+gwlEkkSdRPlER5uRb9cZg23XRTGz9+vCsvoCNKZageGDIigd7cBwzQmKgKWBPtAiaiP/QHyoAczakfrsXpYdjUA5hIGMeC9xIp8gyGYnGkqDfaFc8GCMAL2ACMu+66y70rNFUWwLQ1HEo0ZVSFIWLyT76JOIlm0ZKo1C+kwkHAWfOLAfn7gAEDnFNKO+Na2gK6AGBAik7UJ9AcOnSoc4qIkBlNoP6Yt/f649zgAFI/TIlQP0SytAucGUYeqCNGn8g7Tg/TCuhGW8KJAOi0baBMv6Xd0zZ4V/J0UajGuq5yCgjAldMtt+6qJIAxihhTvHw6Mp0XIwuo+DleP3DAqAJWIiESRouEh4+hATB+XhAPHiNGlMpwMM/DmBAJ4J1j2IkIie6IBImKgSSGDRgCIYwTc48YHeDuV6/yb6JDwA1ISRh/nk3kx5wcQ9QYQ4aYiTaAGFDndwzB8m8cAJ4JoEIXrlQWwAw3E51QTubteCdRLMYT7RiuJYoChBhunx/0YKgdMPN3ohscGiIrRg+oOww4Ua8HJI4Sw75ogy68GzAyh4jTRD1RBzg2zDmiD3XJPCWOFsPzGHPAwTOAObDAUaAeARrRLu/jeubTcdYYTcAxog3RRngf0GEYHVABMN7FvbQT2pWf3w/piJUFsG9DODCUmxESgImutAXaOcP2aImDREIjRgZoYzgsvr2jJ04QAKfsPIfn0laBIeVEU0BLG0Y/tENL6h2nhPdRl4zY4JACW95Pn6DecKRou7wDh5Q2gyND4pm0fe4hvzhz9B/6JiNE1A/tgralCDikVVXPNQJw9eiY3U/xAM74GRKLsM43a7Rs4ZFf7UynjXZcfu7/zd9J0X+nu5brkp/pV+qmu5/fk6JDsanyFc2Tr7BMP/PP8c/3/w6d+/XvAcAY4YquguZ+X77yNParw5MbYlSbqCa+PlKVP10dJGuc/C7/rOS69/8m/8m/8z+LXhOtGz/ykFwPFelwE3YKWAXNIqykVdDp3lle206Xr+Q6jD6DYW2AmTysXl6ZU2mdqh9E3xvtg6k0roimurZ6FBCAq0fH7H7KgjlmLww3m/xt+Z8hrbaB2b5nmTVqlt3lXQm5J2phaJ3ILh28gRGjAqx4Vqo+BX7Y6xpb8NnE8j9D2qqzrXFVP2u06bLvgKsvB+U/iVEVolGiUKV4KSAAx6u+U5eWXa5+/jjzTljN2pqttWX63bKkZVoFmOdjqC/TTlgMhzO8rlR9Csx55Wsrnjgj7QPdTlhrtLKmPbpaQYtG1fdiPUkKZFBAAFYTkQJSQApIASmwEhQQgFeC6HqlFJACUkAKSAEBWG1ACkgBKSAFpMBKUEAAXgmi65VSQApIASkgBQRgtQEpIAWkgBSQAitBAQF4JYiuV0oBKSAFpIAUyHkAl/z8sxW89ZblLVzIThCxr/EEm1YkbZoRZ1HKSkstP835vLHSJZGw0hYtrKRHD2vQofa/ha2LWrNjFBtZ+B2t6mIeazNP6MFOXKG7v9Vm3lbGu9gWtKptI+cBXMTB1ZddZnkzZ7JV0sqopzr1TvakkhuyrErS7QRVpyqtNjLDGbft2lnRySdb0wocdFAbWVtZ7+CbbYDD0YPantHcN+xAJ/l0s5VVPyv7vWw5ynaiVWkbOQ/g4jFjrPDCCwXgld1a9f66rQAAbt3aik491Zr26VO381pLuROAlxca4LAntwC8WBcBOKAjFr/+uhVedJEAHKCVLomxAh7Ap5xiTXv3dkJwZB2HOXB6DocBcEhCnJIALACX194F4ABrIAAHiKRLpEAKAHPiEvtWc4oOJwOdcMIJ7hjCuCQBWAAWgKvY2wXgKgqo2+OhQAoA+/lxznXmyECONIzT8KMALAALwFU0fwJwFSpTBMcAACAASURBVAXU7fFQIAWAOUCCs5g5rYczZnv37l3lVZ/ZJKYALAALwFXssQJwFQXU7fFQIAnARL98glOw5BOto446ys4//3x3OHxckgAsAAvAVeztAnAVBdTt8VAgCcAsvBo/frzVq1fP/vrrLxs9erSdfvrp7tzauCQBWAAWgKvY2wXgKgqo2+OhQIoI+O2337Z33nnHzfsecsgh1qZNm3hosaSUArAALABXscs7AJ9/vuXNmKGNONDS7waWYEsOJaeHtDDzAD7tNGt64IFqGLZ44wltxLGsKeg74BUdEm3EkcFUFI99ywpvvMnyZs8WgNGqLLF4Kyxty7m45ZSWmRVohzQrK7OSVq2t+NiB1qjnPwRgmsbCIjcPXq9RQ20fZ2aLFiy0kqJia9KimdrHEj0aNGxQJVua8zth/fbdVzb9u08sUVJUJaFyocWVlSXcTjb16hW67zvjnthC7u/5f1vDRg2rtJ1cLuiYlzBbVL+BLVpnbWu+5pqWKC3NhWJVqQwLFy2ysrLSxdsNxnwDV/oKIwLFJSXWvFkzY5FenFPC8qxNaQPr1GKVKtmOnAfwy1O/ssunv26zEgstP+adiE5TWlZq+fkFlq8I2NmP4pJiKyworFInyhVDVFZaYmWLiqwwX7uFLx4cKXPTE34leK7Uc2XLwWgANkR6mJUmyuyAZpvYOV17Wb38gspKajkP4GenfmKDvrvHphfPMctT1Ld4zpP2Em8PdmmP0Rzw8sZDekT0yFs89BzzaG+5BqL2sViORJnt16qbPbn5idYwv54AnE6BEVM+sYE/PGDTi+cKwJVuJrpRCkgBKSAFliqQKLPeLTe3xzYbbA0iAJ43b55NmjTJOnbs6KYuMqWcj4AF4ExNQL+XAlJACkiBCimQBGBWy/PZ3uuvv27bbLONdevWLWjfdAG4QqrrYikgBaSAFIi9AkkAnjFjhtsp7txzz7XmzZtbYWGh+5MpCcCZFNLvpYAUkAJSQApEFUgC8I8//mjHHXec7bbbbg68hx9+uHXo0CGjZgJwRol0gRSQAlJACkiBiAJLAfxva5BfaJ999pldccUV9uCDD7pztD/99FMbNmxYRskE4IwS6QIpIAWkgBSQAqkAvHgR1uTJk+2CCy6w22+/3Z0e9tJLL9kll1ySUTIBOKNEukAKSAEpIAWkQHoAs0nJnXfeaZ9//rmbAz700ENt6623ziiZAJxRIl0gBaSAFJACUmB5APdqubk9HvkMiU1K2GmQXQZDFmDxtJwH8OKNOO7VRhy+7fhNjrQPx2JF3EYLMi1LFZAeyxqD+sqKHUPtY7EmiTI7sPVW9shmxy/3HXBFLUnOA/jVKV/YFVNesVllC7QV5ZJD1vHQ2NtVyaykpMRtrSc9zB08wJ9Q7z3X208ZB3WYWb4O63A6uK0oyxJWUFj5rRdzpc2wFWX/lt3t1C57WmFe5fXIeQBP/WOytW7X1urVr/x2YbnSaKw0Ybaw1KxBoVnmT9RyptjlFWTRjLlWv2UTy9PhFFa6qNhKFhZZgxZNYlH3GQu5qGzx6WGNKm9gM74jiy4oWVBkZcUlVr954yzKdc1lldOyChrUr9JJWTkP4D/++MPatWtn9evXr7mayJIns1vL/PnzrWHDhtJjSZ1NmzbNWrVqpQ3mzWzhwoXuxBv0UNJ5wMltQOcBL68Ieug84AyWQgBeJpAAvGJjEYCXaSIAL98+cEboM02aNNEUhZkJwAJwhR1zAVgALq/RCMACcLr2IQCvCBxW+bZo0aLCdjgXb1AEHFCrArAALAAHdBQNQa8gkgAsAJfXcwTgALsiAAvAAnBARxGABeAMzURD0BqCDrMkkasEYAFYAA7rNpoD1hxwpohPQ9DLFFIEHGBXBGABWAAO6CiKgBUBKwIO6yhLrhKAA+QSgAVgATigowjAArAAHNZRBOBwnQRgAVgADusvGoLWELSGoMP6ClcpAg7QSgAWgAXggI6iCFgRsCLgsI6iCDhcJwFYABaAw/qLImBFwIqAw/qKIuBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1ldyGsBAc/Lkybbuuuta8+bNl1Nk5syZVlhYaM2aNQtSSgAWgAXgoK5iArAALACH9ZWcBvCbb75piUTCdtlllxXU+Prrr61hw4a29tprByklAAvAAnBQVxGAk2RasGCBlZaWWpMmTSwvLy9MxBy+SucBL1+5dXov6LKyMhsxYoS9++671q9fP9tyyy3txRdftHHjxlnjxo3txBNPdP/+888/berUqdanTx/baKONbMKECXb77bdbhw4d7Mgjj7TWrVvbE088YZ988ontuuuuLvKlQ2y88cY2evRo++CDD2zHHXe0PfbYI2XTF4AFYAE4jAqKgBUBKwIO6yt1PgJ+8sknbd68ebbXXnvZjTfe6AD77LPP2sCBA61BgwbWqlUrGzBggJ111lmGpwlMjz76aCP63Xzzze3TTz91EOYZDDsD33bt2rnrmjZtap07dzbeccQRR9ioUaNshx12sO7du6+gngAsAAvAYUZFABaABeCwvlLnAXzllVfaq6++6sBIlHr99dfbK6+8Yp9//rn985//tC222MLB8+mnn7ZJkybZM888Y/Xq1XMR8yqrrOLmgPfcc08bO3asHX/88Uvh+sADD1ijRo1s9uzZDuibbrqp+zuA79mzpwBcTvthOG3+/PluCL9+/frhLS2Hr5w2bZpzBgsKCnK4lGFFE4AFYAE4rK/UeQDfcMMNLtIdNGiQOzeRYeeSkhIX0Q4ePNiuvfZa93/AO3HiRHvsscesa9eu9ssvv1ivXr2sY8eODhTnnnuui36ZD87Pz7cHH3zQPYuFWD/++KOddNJJVlxc7IDCz5KTImBFwIqAw4yKACwAC8BhfaXOA/j777+3O+64w+bOneuGi/v27WuPPvqog+WUKVPs6quvtv79+9t6661nRUVF1qlTJxsyZIg9/PDDbpiZ1c+HHXaYdenSxS666CIH15133tktFCFi2X777d31wHiNNdZww9n8XwBO34AUAa+ojSLgZZoIwAKwAJwjAPbFIPr10Skrm5nvBZoMhR5zzDH2+OOPL42Q/T0YAhIRsE9EzsmrEVnoxbXpol/uVQSsCFgRcJhREYAFYAE4rK/U+Qg4UzEA8bBhw9zccE0mAVgAFoDDepgALAALwGF9JesBTAEYEq3pxS8CsAAsAIcZFQFYABaAw/pKTgA4vKiVv1IAFoAF4LD+IwALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQJwFYABaAwzqLACwAC8BhfUUADtRJABaABeCwziIAC8ACcFhfEYADdRKABWABOKyzCMACsAAc1lcE4ECdBGABWAAO6ywCsAAsAIf1FQE4UCcBWAAWgMM6iwAsAAvAYX1FAA7USQAWgAXgsM4iAAvAAnBYXxGAA3USgAVgATisswjAArAAHNZXBOBAnQRgAVgADussArAALACH9RUBOFAnAVgAFoDDOosALAALwGF9RQAO1EkAFoAF4LDOIgALwAJwWF8RgAN1EoAFYAE4rLMIwAKwABzWVwTgQJ0EYAFYAA7rLAKwACwAh/UVAThQpz/+mGTt2rW1+vXrB96Ru5eVlpba/L8XWsOGDax+vcLcLWgFSjZt2jRr1aqVFRQUVOCu3LxUABaABeDwvv33339bo0aNLC8vL/ympCvzEolEotJ3Z8GNk/6YaG1bN3HAyemCBtQFAKbROADXb2A5XvUZFckrqGd/TZtnrVu3sYKC/IzX5/oFArAALACH93IBOECrWZPft4J5IyzfFphZ5T2VgFfV+UsAbklxsRUUFlp+ftyBk7C8vAKb3+hQa7NaN+lhZgKwACwAh5txAThAqwVTR9mCCf+yRPE0s7y4Q8fMjZYk3H9KZQst0flha71WfwFYAF6hPyxYsMAYNWrSpEmVhhlzpaMBnOLiYmvRokWuFKlK5RCAA+T7e+qLtvDHU8yKpwvAAXrF6pKyBVbW6W5r3elgy89fPAc8d+5cmzlzpq255pqxkoLCKgJWBKwIOLzbC8ABWgnAASLF9ZIkAH/55Zf2+uuvu4UVRUVFdsIJJ8RKGQFYABaAw7u8AByglQAcIFJcL0kCMCui+cPQ48MPP2xDhgyxVVddNTbqCMACsAAc3t0F4ACtBOAAkeJ6SYohaKT49ddfbfjw4XbLLbfEam5YABaABeBwYygAB2glAAeIFNdLUgB49uzZdtlll9nBBx9sW265ZayUEYAFYAE4vMsLwAFaCcABIsX1kiQA06EuuugiB9/u3bvHThUBWAAWgMO7vQAcoJUAHCBSXC+JADgvL99Fvs8//7xtuOGG1rJlSzvssMNiFQULwAKwABxuDAXgAK0E4ACR4npJUgRcVla23O5gbFZSlW3msk1WAVgAFoDDe60AHKDV31NfsIU/nGSmjTiWqOV3A9NWHAaA17p/ue+AA5pUzl4iAAvAAnB49xaAA7SaN/VVS/x+qeWVzTIz7YRFlEdUF6fILm0zSSyyhateY6079ozVaud0egjAArAAHACVJZcIwAFa/TJ1ki1oXM/ydNqNAd9FCxe6k6HYDzreKWEFBQ2t8ZwFtlqb1gKwdsJaoTtoK8rlJdFWlCvqodOQMlDkg7l/262z5tjssoTiX3ccxeIh6IR2g7ZiMzujQYH1WKWt5cX+cAptRZlsSgRgATjTiIAAnAHAH82ZZ/fMnmdzEgJwvCPeFUtfZGb/alBou7RrowhYEbAi4AwGQhGwIuAKM0QArrBksbkBAB/foNB2XgLgWbNm2XvvvefKv/7661vnzp1jowUF1Ryw5oAzRXw6DWmZQpoDDjCPAnCASDG9JBnAP/zwg7377rvuIIbp06fbqaeeag0aNIiNOgKwACwAh3d3AThAKwE4QKSYXpIM4Pnz57uzX3///Xe78sor7YILLrDWrVvHRh0BWAAWgMO7uwAcoJUAHCBSTC9JBjAysFKcKPjll19221LGKQnAArAAHN7jBeAArQTgAJFiekkygBOJhH322Wc2atQoO+6442J1FKHmgFfsBFoFvbwmWoS1oh5ZuQqauTYWuBSk+TZ3ypQpNn78eLcn7yqrrLJcqSdMmGBdu3YN3khCAI4pXQOKnQzgjz/+2O6++2476qijXBujc/EnLkkRsCJgRcDhvb1ORcAsWvn2229thx12yFiC//3vf7bzzjtb48aNU177xhtvuJ/vsssuK/z+mWeesT59+gjAGVXWBZkUWA7AeXk2YuRIe+utt1zk27BhQ+vZs6dbDR2XJAALwAJweG+vNQCPGDHCNt54Y1t77bXtqaeecpDl0PInnnjC1lhjDRs0aJDddNNNBljPOussd4LMfffdZ3/++af7HSfLfP311/bSSy85o/bzzz/bgQceaO+8847NmDHDxo0bZ9tss43179/fvvnmG3vggQestLTUBg8e7NSYOHGiGxbkdJq3337bTjzxRJs0aZJdd911bpXqIYccYptttllK5RQBhzeouF2ZHAEvWrTISkpKXNtjq04gXK9evdjIIgALwAJweHevNQBfccUV7nzU3Xff3Y4++mg755xz3AKVa6+91saMGWPTpk2zbt262ejRo+3cc8+1e++911q0aGHt27e3L7/80jbYYAO75ZZbHJw333xzB9ChQ4faHXfcYV26dHHPfeyxx2yvvfaydddd1/jWDOizZSJDgEB/2LBh7neHHnqo3XnnnXbmmWfa6aefbojw4IMPumcD+uTkADxnns3VRhyLpdEZDEubCAAe3KDAdmzXVhtx6DvgFWyH5oCXl0RzwCvqUStzwCxMef/99x3g5s2b5+bHLrzwQttqq63cN5NExttvv7298sorbvHKJZdcYlOnTrV27dq5P8D7q6++siOPPNLatm3rIluAef/997tImCj62WefdfPCRB1Eyt9995316NHDzQHPmTPHHZLerFkzF+3edddd7lncQ5RNJI4DQB6S0/g/p9k3eYVWwtFy4c5NTl6ZSJRZaUmxNWxQP+38e04WPEWh8EPq5eXZhgvm25ptBWAkUgSsCFgRcLgFrLUImCxdfPHFDsI33HCDi0yHDx/uQFtYWOjmcj/99FMbOXKki0qffPJJW3311V1kyxAew8p81kH03KZNGwdpHykD1NVWW81FvBgAhgEZ4gbAeKB4GEAeUDdt2tQOOuggN7x90kknuQh88uTJ9txzz7nhaxyB5DT289/tvtcm27yFnAIULm6uXZlImNUvNNt7i9Z2eM8u/79GC3KtiJUqD6M3rVq1ir1DIgCv2HwUASsCzuSQ1EoETCaefvppt00fQ8dEsddff72bB27evLn17t3bGbGzzz7brSBl8wIgCZxZSLXWWmu5zzt69erlomg2ODj++OONBVV77723i5JfffVV97vffvvNPvroIwfubbfd1g1lA2VgDuhPOeUUu+aaa+zDDz907+BdROQDBw5MqdVz7060Y68fZ9NnF5nlx5jAqFOasL47r2ZPns1IQcy1WNJaBOBl3UYRsCLgTMDRVpTLFKrVCDhdxfDtpD9blr+zkQGfF9XGubPR96XL34h3J9rAGz4TgJcA+JCdVrPHz9puKYBnzpxp6Ijzkx/DE4EEYAE4ne1QBKwIOJNDUmsRcKXG9+rATQJwpBJKExYFMJ+OMQ/PKEO/fv3cEH/ckgAsAAvAYb1ei7BWdEgE4AxtRwBOD2A+/2KFeadOnaxv376x2vfYqyIAC8ACsAAcpoAAXGGdBOD0AOY3fFfNd9n77LOPWyAXtyQAC8ACcFivVwQsAIe1lMhVAnD5AB47dqz98ssvtu+++wrAFW5duXWDFmEtX5+aA14ROFqEtUyTOrEIq66bIAG4fACz7ScR8AEHHCAA1/XGXMP5E4AF4PKamCJgRcAVNkECcPkAZoMUNk3Zeuut3UYncUsagtYQtIagw3q9ACwAh7UUDUGn1ilpFTQX+f2PWc2nz5Aq3Lxy6gZFwIqAFQGHd2kNQQdo9ey7E23QdeNs+qxF2oijNGEH7rKaPX1OD23EsaTtKAJWBKwIOMCQmrl99zUHrDngsNay5KrXP/vdbn95is1dWBbrjbDYirJegdl+3VrawL3ZslNbUdJEBGABWAAOM6kCsIagw1pK5KppP4+3wsnfWn6iJOZRX8LK8gqtbJW1rVnnja1eQX6FtczFGwRgAVgADuvZArAAHNZSIlcV//C+Fb5xi+UtnGOWF2foJNxRhMVdd7LEnqdZ/QormZs3CMACsAAc1rcFYAE4rKVEAfz9e1b4+k2Wt2B2zAFsZmVlVrzOjpbY70wBWHPAK/QlLcJaXhJ9B7wicDQHrDngCkG4WABeplcSgDmE4Y8//rDS0lJ3fCQnUMUtKQJWBKwIOKzXKwJWBBzWUhQBp9YpCcAcJ3neeee54yI5x5lDGeKWBGABWAAO6/UCsAAc1lIE4CAAE/2yFzSRcM+ePbUTVoVbV27doCFoDUGX16IFYAG4whZPQ9ARyVLMAWsv6GnWqlUrd4Z13JMALAALwOFWQBtxBGglAAvA5TUTDUFrCFpD0AGGVBtxrCCSABzQbgTg8gE8ZswYdxhDr169rG3btgGK5tYlArAALACH9WkNQWsIOqylaA44aA6Yi1iINWvWLFt33XWN/aDjlgRgAVgADuv1ArAAHNZSBOA0AC614rV3sMT+w/Qd8BKFBGABWAAOM6sCsAAc1lIiV5VOeMfyX77a8hbMivlGHAlL5BVY8Ub7Wt5ep1r8vvhN3XQEYAFYAA4zqwKwABzWUiJX/fnrD9asaIYVxnkXyiV6lJYlbEG95tagfWerX1joPj+KcyosLLTp06db69atY3kUY3LdaxX08opoJ6wVgaOdsJZpokVYAfT4+ptv7Y2xb9nCRYssLy8v4I7cvQTglpUUW76VWV6s98VeXMfsALbHHnvYJptsIgCbmQAsAJdn/RQBKwKuMB2/+OILe/zxx23+/PmxB3CFxcvxG/DmDz30UNtuu+0EYAF4hdauCFgRcCaHhIWrVQns8hI5Pg4JgJ966ikBOMdhWpniAeB+/frZtttuKwALwAJwhk6kCFgRcIXtrABcYclic0MygH/66Se76aabrKyszHbaaSc78MADY6MFBdUQtIagM0V8mgPWHHCFjKIAXCG5YnVxMoDZG7tJkyY2b948u/76623o0KGx2pxEABaABeBwE6hFWAFaCcABIsX0knRD0L/88ouLhC+++OJYbU4iAAvAAnC4MRSAA7QSgANEiuklqQA8d+5ce+aZZ9zhDAMGDIiVMgKwACwAh3d5AThAKwE4QKSYXpIM4NmzZ9vTTz/thqBPPvlkNxecnx+fD8gFYAFYAA43hgJwgFYCcIBIMb0kGcCjRo2yhx56yAYPHmwlJSW20UYbWfv27WOjjgAsAAvA4d1dAA7QSgAOECmmlyQD+NNPP7XffvvN+P6zYcOG1r17d1tzzTVjo44ALAALwOHdXQAO0AoAP/roo25YsSofTAe8SpdkmQJFRUV2xBFH6DvgJfUmAAvAAnC4EROAA7Qa/8ME+/L7b624tMTyLN5bUTKnWTx/geUXJSy/ID5zm+maCQutunXrZl27do3VXG86PQRgAVgADoDKkksE4ACtpr7/rc156hOzv4vM4rwXdMIsUZhnhdt1tra9u1s9K4j9YQz169d3ZyHrMIbFHUkAFoAF4ACoCMDhIs0YOc4mDbrPSv+caxbnqI+Tj/LzrPnRPazTHUeb4t/FbUjHES7rSwKwACwAh7NFEXCAVtNHfWaTT3rYSqfNcwCKbSICLi2zZgd1s7UeOM4KYivE8gUXgAXgdF1BhzEsr4z2gl5RDx3GkAEkAvASgQBwWZk169vN1rpvGYDHjh1rLEbaYYcd3MrfuCUBWAAWgMN6vQAsAIe1lMhVAnB6AAPfBx54wH1uw7F8LVu2rLC+2X6DACwAC8BhvVgAFoDDWooAvKJOKSJgVkWPHj3a/vrrL9t///3dYqS4JQFYABaAw3q9ACwAh7UUATgIwFxEFMzhA/vuu6+1adOmwvpm+w0CsAAsAIf1YgFYAA5rKQJwMIDffPNN+/XXXwXgAi1L0yro5buNFmGtCBydB7xME62CDsCx5oCXiJRmEdbbb7/ttl/ca6+9NAQd0J5y+RIBWAAur30rAlYEot3blgAABrNJREFUXGH7JwCXD+DJkycbR/Cx57FWQVe4eeXUDQKwACwAh3dpRcABWs14fpz98e8H9R2w/w744O7W+aHj9R3wkrajOWDNAWsOOMCQmpkiYEXAYS0lctXMV7+2qec+a2Uz5sd+Iw6zhDXpvbl1uLyfALykjcyYMcN9fhWnc3/TdaJFixa57ShbtGhR4X6WizegRWlpqTVu3FgHuZi5U8KYA27evHkuVneFy+RPTavKIT95iQR7FOZuKpoy2xZ+MdESRaUW67MYqOV6+VZ/3VWtYedVYi1FtLWzCUm9evVkYM2Mz9IADnoomdOCxKEdSov1oI2ofSxuDZwZXlhYWKWmkfMArpI6ulkKSAEpIAWkQA0pIADXkLB6rBSQAlJACkiB8hQQgNU+pIAUkAJSQAqsBAVyHsA//vijrbrqqta0adOVIG/deyXzOPzhLNy4pzlz5rhtODt16lTluZxs15KlIKwIZ+FRx44ds7041ZZ/5vlYeMSpN3FOtIvp06e7OeBWrVrJni45P5tdBOkvTZo0qVTzyGkA33zzze7QeTaaOOGEE5yhjXOaPXu2XX/99W5RyTnnnBNnKeybb75x23DiiOCknXfeedagQYNYagJkPvzwQ/vggw+cgWUV9BFHHCEnzcxOP/1022mnnaxXr16xXajHQkX2jH/rrbesc+fO1qNHD9tss81i2Vd8oekrb7zxhts/Yccdd7QOHTpUSo+cBfAPP/xgTz31lDtkAAD/9NNPdtxxx8V6BR/R3i233OJW71188cWVajC5chPRLw4JIyMnnXSSXX311da+fftcKV6FyoGTOmvWLDcyQj8ZM2aMHXTQQda1a9cKPSfXLr7vvvuco7b++uvb0UcfHVsA0zZGjhzp9ooHNqz85dOsOKfTTjvNBg4caF26dHGOamVXQ+csgF966SU3vOg916FDh9pVV10V+6Ektp7Ekx02bFic+8/SsgOfAQMG2G233WbNmjWLrSZssvDqq6+6P1tssYUDTpzTl19+6UZImL5i+PXwww+PNYDvvfde+/zzz2299daz3r172wYbbBDb5vH7778bPFlnnXVs/vz5NnjwYAfiyqScBTBDJsxpAWA2WTjjjDNclBP3uRyGGl955RU7++yzK9Necu6eIUOGWJ8+fWy77baLrYGlUol+p06dahzOMWHCBDcEzXBjHBNDrueff76D7s8//2xTpkxxDkllo5xs1xAnFQeN/7/22mtulOSoo45yc8FxTF999ZUbSTzzzDNd8a+44gr378qknAUwQ9CjRo2yfv36GR4LhuXkk0+O/bwWAH755ZdjPweMMTnrrLNs9913d3N8GNeq7GhTmc5Xl+5BD8qP0/rkk086j37PPfesS1mstbxMmjTJ7rzzTmOagukrdjxi9CzOUZ9vH++99559/PHH1rdvX1tttdVqrU7q0osYkr/00kud/WD4edCgQfbII49UKos5C2DUuPHGG91ZtxMnTrThw4fb2muvXSmRcummTz75xM3xEfnFOeGxjhgxws37Al8ivp133jmWkhDdAN1x48YZ21EC3xNPPDG2o0XAhj+MnDFaxFRW//79Y7td6cyZMx1gGBmhrbCu5oADDohlX/GFvv322238+PFuZfgxxxxju+yyS6X0yGkAowirOrXPb6Xahm6KmQJ+V9o4jwTErMorXFwfCVf4xhy8oTq0yHkA52C9q0hSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KSAAZ1+dKcdSQApIASmQAwoIwDlQiSqCFJACUkAKZJ8CAnD21ZlyLAWkgBSQAjmggACcA5WoIkgBKSAFpED2KfD/ACv5gltg2onZAAAAAElFTkSuQmCC" id="3" name="Shape 3"/>
@@ -2524,8 +2541,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5193600" y="3627600"/>
-          <a:ext cx="304800" cy="304800"/>
+          <a:off x="5184075" y="3618075"/>
+          <a:ext cx="323850" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2548,6 +2565,8 @@
             <a:spcAft>
               <a:spcPts val="0"/>
             </a:spcAft>
+            <a:buSzPts val="1400"/>
+            <a:buFont typeface="Arial"/>
             <a:buNone/>
           </a:pPr>
           <a:r>
@@ -2569,7 +2588,7 @@
     <xdr:ext cx="4200525" cy="2914650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image3.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2625,7 +2644,7 @@
     <xdr:ext cx="3962400" cy="2667000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2910,7 +2929,7 @@
         <v>5</v>
       </c>
       <c r="X13" s="6"/>
-      <c r="Y13" s="7" t="s">
+      <c r="Y13" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2922,10 +2941,10 @@
         <v>1</v>
       </c>
       <c r="M14" s="3"/>
-      <c r="N14" s="12">
+      <c r="N14" s="13">
         <v>12.0</v>
       </c>
-      <c r="O14" s="12" t="s">
+      <c r="O14" s="13" t="s">
         <v>8</v>
       </c>
       <c r="S14" s="9" t="s">
@@ -2935,118 +2954,118 @@
       <c r="U14" s="10">
         <v>13.0</v>
       </c>
-      <c r="W14" s="13" t="s">
+      <c r="W14" s="14" t="s">
         <v>10</v>
       </c>
       <c r="X14" s="6"/>
-      <c r="Y14" s="14">
+      <c r="Y14" s="15">
         <v>3.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="13">
         <v>2.0</v>
       </c>
       <c r="M15" s="3"/>
-      <c r="N15" s="12">
+      <c r="N15" s="13">
         <v>10.0</v>
       </c>
-      <c r="O15" s="12" t="s">
+      <c r="O15" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="W15" s="13" t="s">
+      <c r="W15" s="14" t="s">
         <v>16</v>
       </c>
       <c r="X15" s="6"/>
-      <c r="Y15" s="14">
+      <c r="Y15" s="15">
         <v>25.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="15">
         <v>5.0</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="13">
         <v>2.0</v>
       </c>
       <c r="M16" s="3"/>
-      <c r="N16" s="12">
+      <c r="N16" s="13">
         <v>10.0</v>
       </c>
-      <c r="O16" s="12" t="s">
+      <c r="O16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="W16" s="13" t="s">
+      <c r="W16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="14">
+      <c r="X16" s="18"/>
+      <c r="Y16" s="15">
         <v>2.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="15">
         <v>7.0</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="13">
         <v>4.0</v>
       </c>
       <c r="M17" s="3"/>
-      <c r="N17" s="12">
+      <c r="N17" s="13">
         <v>4.0</v>
       </c>
-      <c r="O17" s="12" t="s">
+      <c r="O17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="16"/>
+      <c r="W17" s="19"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="15">
         <v>5.0</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="13">
         <v>4.0</v>
       </c>
       <c r="M18" s="3"/>
@@ -3054,22 +3073,22 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="2"/>
-      <c r="W18" s="16"/>
+      <c r="W18" s="19"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="15">
         <v>7.0</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="K19" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="13">
         <v>6.0</v>
       </c>
       <c r="M19" s="3"/>
@@ -3077,49 +3096,52 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="2"/>
-      <c r="W19" s="16"/>
+      <c r="W19" s="19"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="15">
         <v>9.0</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
+      <c r="U20" s="20" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="G21" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="14" t="s">
+      <c r="G21" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I21" s="14">
+      <c r="H21" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="15">
         <v>4.0</v>
       </c>
-      <c r="K21" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="L21" s="12" t="s">
+      <c r="K21" s="21" t="s">
         <v>37</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="8" t="s">
+      <c r="T21" s="19"/>
+      <c r="U21" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="V21" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="W21" s="8" t="s">
+      <c r="V21" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="W21" s="23" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3128,14 +3150,14 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="14" t="s">
+      <c r="T22" s="19"/>
+      <c r="U22" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="V22" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="W22" s="18">
+      <c r="V22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="W22" s="25">
         <v>13.0</v>
       </c>
     </row>
@@ -3144,14 +3166,14 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="14" t="s">
+      <c r="T23" s="19"/>
+      <c r="U23" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="V23" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="W23" s="18">
+      <c r="V23" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="W23" s="25">
         <v>4.0</v>
       </c>
     </row>
@@ -3160,14 +3182,14 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="14" t="s">
+      <c r="T24" s="19"/>
+      <c r="U24" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="V24" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="W24" s="18">
+      <c r="V24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="W24" s="25">
         <v>5.0</v>
       </c>
     </row>
@@ -3176,351 +3198,351 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-      <c r="S25" s="16"/>
-      <c r="T25" s="16"/>
-      <c r="U25" s="14" t="s">
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="V25" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="W25" s="18">
+      <c r="V25" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="W25" s="28">
         <v>8.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="F26" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
+      <c r="F26" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="N26" s="3"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
       <c r="W26" s="2"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="F27" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="21" t="s">
+      <c r="F27" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="21" t="s">
+      <c r="G27" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="H27" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="J27" s="21" t="s">
+      <c r="I27" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="16"/>
+      <c r="J27" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
       <c r="W27" s="2"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="F28" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" s="22" t="s">
+      <c r="F28" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="G28" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="I28" s="23">
+      <c r="I28" s="32">
         <v>45933.42638888889</v>
       </c>
-      <c r="J28" s="22"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="16"/>
-      <c r="T28" s="16"/>
-      <c r="U28" s="16"/>
-      <c r="V28" s="16"/>
+      <c r="J28" s="31"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
       <c r="W28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="H29" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="J29" s="33"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="F30" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="32">
+        <v>45933.39097222222</v>
+      </c>
+      <c r="J30" s="31"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="F31" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="34">
+        <v>45872.520833333336</v>
+      </c>
+      <c r="J31" s="33"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="2"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="F32" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="31"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="2"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="F33" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="34">
+        <v>45660.458333333336</v>
+      </c>
+      <c r="J33" s="33"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="2"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="F34" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="32">
+        <v>45933.61111111111</v>
+      </c>
+      <c r="J34" s="31"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="2"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="F35" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="34">
+        <v>45903.368055555555</v>
+      </c>
+      <c r="J35" s="33"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="2"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="F36" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G36" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="32">
+        <v>45932.65625</v>
+      </c>
+      <c r="J36" s="31"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="2"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="2"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="2"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
+      <c r="U39" s="35"/>
+      <c r="V39" s="36"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="2"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="F41" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="2"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="F42" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I42" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="J42" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K42" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
+      <c r="U42" s="19"/>
+      <c r="V42" s="2"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="F43" s="31">
+        <v>10.0</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I43" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="J43" s="31">
+        <v>7.0</v>
+      </c>
+      <c r="K43" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="S43" s="19"/>
+      <c r="T43" s="19"/>
+      <c r="U43" s="19"/>
+      <c r="V43" s="2"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="F44" s="33">
+        <v>23.0</v>
+      </c>
+      <c r="G44" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="H29" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" s="24"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="2"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="F30" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="23">
-        <v>45933.39097222222</v>
-      </c>
-      <c r="J30" s="22"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16"/>
-      <c r="W30" s="2"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="F31" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="G31" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="H31" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="25">
-        <v>45872.520833333336</v>
-      </c>
-      <c r="J31" s="24"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16"/>
-      <c r="U31" s="16"/>
-      <c r="V31" s="16"/>
-      <c r="W31" s="2"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="F32" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="G32" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H32" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="I32" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="J32" s="22"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16"/>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16"/>
-      <c r="W32" s="2"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="F33" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G33" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="I33" s="25">
-        <v>45660.458333333336</v>
-      </c>
-      <c r="J33" s="24"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="16"/>
-      <c r="U33" s="16"/>
-      <c r="V33" s="16"/>
-      <c r="W33" s="2"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="F34" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G34" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="H34" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" s="23">
-        <v>45933.61111111111</v>
-      </c>
-      <c r="J34" s="22"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="16"/>
-      <c r="T34" s="16"/>
-      <c r="U34" s="16"/>
-      <c r="V34" s="2"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="F35" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G35" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="H35" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" s="25">
-        <v>45903.368055555555</v>
-      </c>
-      <c r="J35" s="24"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16"/>
-      <c r="U35" s="16"/>
-      <c r="V35" s="2"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="F36" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G36" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="H36" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" s="23">
-        <v>45932.65625</v>
-      </c>
-      <c r="J36" s="22"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="16"/>
-      <c r="T36" s="16"/>
-      <c r="U36" s="16"/>
-      <c r="V36" s="2"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="R37" s="16"/>
-      <c r="S37" s="16"/>
-      <c r="T37" s="16"/>
-      <c r="U37" s="16"/>
-      <c r="V37" s="2"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="S38" s="16"/>
-      <c r="T38" s="16"/>
-      <c r="U38" s="16"/>
-      <c r="V38" s="2"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="S39" s="16"/>
-      <c r="T39" s="16"/>
-      <c r="U39" s="16"/>
-      <c r="V39" s="2"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="S40" s="16"/>
-      <c r="T40" s="16"/>
-      <c r="U40" s="16"/>
-      <c r="V40" s="2"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="F41" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="6"/>
-      <c r="S41" s="16"/>
-      <c r="T41" s="16"/>
-      <c r="U41" s="16"/>
-      <c r="V41" s="2"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="F42" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H42" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="I42" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="J42" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K42" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="S42" s="16"/>
-      <c r="T42" s="16"/>
-      <c r="U42" s="16"/>
-      <c r="V42" s="2"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="F43" s="22">
-        <v>10.0</v>
-      </c>
-      <c r="G43" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="H43" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="I43" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="J43" s="22">
-        <v>7.0</v>
-      </c>
-      <c r="K43" s="22" t="s">
+      <c r="H44" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="I44" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="J44" s="33">
+        <v>3.0</v>
+      </c>
+      <c r="K44" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="S43" s="16"/>
-      <c r="T43" s="16"/>
-      <c r="U43" s="16"/>
-      <c r="V43" s="2"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="F44" s="24">
-        <v>23.0</v>
-      </c>
-      <c r="G44" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="H44" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="I44" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="J44" s="24">
-        <v>3.0</v>
-      </c>
-      <c r="K44" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="S44" s="16"/>
-      <c r="T44" s="16"/>
-      <c r="U44" s="16"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
+      <c r="U44" s="19"/>
       <c r="V44" s="2"/>
     </row>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -3538,172 +3560,172 @@
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1"/>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="F59" s="27" t="s">
+      <c r="F59" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="F60" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G60" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H60" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I60" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="J60" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K60" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="F61" s="31">
+        <v>23.0</v>
+      </c>
+      <c r="G61" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H61" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-      <c r="K59" s="6"/>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="F60" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G60" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H60" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="I60" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="J60" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K60" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="F61" s="22">
-        <v>23.0</v>
-      </c>
-      <c r="G61" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="H61" s="22" t="s">
+      <c r="I61" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="J61" s="31">
+        <v>3.0</v>
+      </c>
+      <c r="K61" s="31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="F62" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="G62" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="H62" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="I61" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="J61" s="22">
+      <c r="I62" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="J62" s="33">
         <v>3.0</v>
       </c>
-      <c r="K61" s="22" t="s">
+      <c r="K62" s="33" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="F62" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="G62" s="24" t="s">
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="F63" s="31">
+        <v>22.0</v>
+      </c>
+      <c r="G63" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="H63" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I63" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="H62" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="I62" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="J62" s="24">
+      <c r="J63" s="31">
+        <v>7.0</v>
+      </c>
+      <c r="K63" s="31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="F64" s="33">
+        <v>10.0</v>
+      </c>
+      <c r="G64" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H64" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="I64" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="J64" s="33">
+        <v>7.0</v>
+      </c>
+      <c r="K64" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" ht="15.75" customHeight="1">
+      <c r="F65" s="31">
+        <v>6.0</v>
+      </c>
+      <c r="G65" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H65" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I65" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="J65" s="31">
         <v>3.0</v>
       </c>
-      <c r="K62" s="24" t="s">
+      <c r="K65" s="31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="F63" s="22">
-        <v>22.0</v>
-      </c>
-      <c r="G63" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H63" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="I63" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="J63" s="22">
-        <v>7.0</v>
-      </c>
-      <c r="K63" s="22" t="s">
+    <row r="66" ht="15.75" customHeight="1">
+      <c r="F66" s="33">
+        <v>9.0</v>
+      </c>
+      <c r="G66" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="H66" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="I66" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="J66" s="33">
+        <v>5.0</v>
+      </c>
+      <c r="K66" s="33" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="F64" s="24">
-        <v>10.0</v>
-      </c>
-      <c r="G64" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="H64" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="I64" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="J64" s="24">
-        <v>7.0</v>
-      </c>
-      <c r="K64" s="24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="F65" s="22">
-        <v>6.0</v>
-      </c>
-      <c r="G65" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="H65" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="I65" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="J65" s="22">
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="F67" s="31">
+        <v>13.0</v>
+      </c>
+      <c r="G67" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="H67" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="I67" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J67" s="31">
         <v>3.0</v>
       </c>
-      <c r="K65" s="22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="F66" s="24">
-        <v>9.0</v>
-      </c>
-      <c r="G66" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="H66" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="I66" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="J66" s="24">
-        <v>5.0</v>
-      </c>
-      <c r="K66" s="24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" ht="15.75" customHeight="1">
-      <c r="F67" s="22">
-        <v>13.0</v>
-      </c>
-      <c r="G67" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="H67" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="I67" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="J67" s="22">
-        <v>3.0</v>
-      </c>
-      <c r="K67" s="22" t="s">
+      <c r="K67" s="31" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3722,58 +3744,58 @@
     <row r="80" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="H82" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="I82" s="28" t="s">
+      <c r="H82" s="38" t="s">
         <v>70</v>
       </c>
+      <c r="I82" s="38" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="H83" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="I83" s="30">
+      <c r="H83" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="I83" s="40">
         <v>6.0</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="H84" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="I84" s="30">
+      <c r="H84" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="I84" s="40">
         <v>4.0</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="H85" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="I85" s="30">
+      <c r="H85" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="I85" s="40">
         <v>4.0</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="H86" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="I86" s="30">
+      <c r="H86" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="I86" s="40">
         <v>3.0</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="H87" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="I87" s="30">
+      <c r="H87" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I87" s="40">
         <v>1.0</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="H88" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="I88" s="30">
+      <c r="H88" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="I88" s="40">
         <v>1.0</v>
       </c>
     </row>
@@ -3791,170 +3813,170 @@
     <row r="100" ht="15.75" customHeight="1"/>
     <row r="101" ht="15.75" customHeight="1"/>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="H102" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="I102" s="28" t="s">
+      <c r="H102" s="38" t="s">
         <v>78</v>
       </c>
+      <c r="I102" s="38" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="H103" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="I103" s="30">
+      <c r="H103" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="I103" s="40">
         <v>8.0</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="H104" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="I104" s="30">
+      <c r="H104" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="I104" s="40">
         <v>5.0</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="H105" s="29" t="s">
+      <c r="H105" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="I105" s="40">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="106" ht="15.75" customHeight="1">
+      <c r="H106" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="I106" s="40">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="107" ht="15.75" customHeight="1">
+      <c r="H107" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="I107" s="40">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="108" ht="15.75" customHeight="1">
+      <c r="H108" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="I108" s="40">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="109" ht="15.75" customHeight="1">
+      <c r="H109" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I109" s="40">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="110" ht="15.75" customHeight="1">
+      <c r="H110" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="I110" s="40">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="111" ht="15.75" customHeight="1">
+      <c r="H111" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I111" s="40">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="112" ht="15.75" customHeight="1">
+      <c r="H112" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="I112" s="40">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="113" ht="15.75" customHeight="1">
+      <c r="H113" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="I105" s="30">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="106" ht="15.75" customHeight="1">
-      <c r="H106" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="I106" s="30">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="107" ht="15.75" customHeight="1">
-      <c r="H107" s="29" t="s">
+      <c r="I113" s="40">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="114" ht="15.75" customHeight="1">
+      <c r="H114" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="I114" s="40">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="115" ht="15.75" customHeight="1">
+      <c r="H115" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="I115" s="40">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="116" ht="15.75" customHeight="1">
+      <c r="H116" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="I116" s="40">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="117" ht="15.75" customHeight="1">
+      <c r="H117" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="I107" s="30">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="108" ht="15.75" customHeight="1">
-      <c r="H108" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="I108" s="30">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="109" ht="15.75" customHeight="1">
-      <c r="H109" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="I109" s="30">
+      <c r="I117" s="40">
         <v>1.0</v>
       </c>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
-      <c r="H110" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="I110" s="30">
+    <row r="118" ht="15.75" customHeight="1">
+      <c r="H118" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="I118" s="40">
         <v>1.0</v>
       </c>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
-      <c r="H111" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="I111" s="30">
+    <row r="119" ht="15.75" customHeight="1">
+      <c r="H119" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="I119" s="40">
         <v>1.0</v>
       </c>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
-      <c r="H112" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="I112" s="30">
+    <row r="120" ht="15.75" customHeight="1">
+      <c r="H120" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="I120" s="40">
         <v>1.0</v>
       </c>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
-      <c r="H113" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="I113" s="30">
+    <row r="121" ht="15.75" customHeight="1">
+      <c r="H121" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="I121" s="40">
         <v>1.0</v>
       </c>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
-      <c r="H114" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="I114" s="30">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="115" ht="15.75" customHeight="1">
-      <c r="H115" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="I115" s="30">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="116" ht="15.75" customHeight="1">
-      <c r="H116" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="I116" s="30">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="117" ht="15.75" customHeight="1">
-      <c r="H117" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="I117" s="30">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="118" ht="15.75" customHeight="1">
-      <c r="H118" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="I118" s="30">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="119" ht="15.75" customHeight="1">
-      <c r="H119" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="I119" s="30">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="120" ht="15.75" customHeight="1">
-      <c r="H120" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="I120" s="30">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="121" ht="15.75" customHeight="1">
-      <c r="H121" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="I121" s="30">
-        <v>1.0</v>
-      </c>
-    </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="H122" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="I122" s="30">
+      <c r="H122" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="I122" s="40">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>